<commit_message>
Messed around with coefficients updated tolerance in pipe.
</commit_message>
<xml_diff>
--- a/pipe/coefficients-20.xlsx
+++ b/pipe/coefficients-20.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="680" yWindow="680" windowWidth="24320" windowHeight="13880" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1483" uniqueCount="667">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1501" uniqueCount="681">
   <si>
     <t>m^2</t>
   </si>
@@ -2022,15 +2022,59 @@
     <t>m^3/s</t>
   </si>
   <si>
-    <t>&lt;- smallest available restrictor</t>
+    <t>&lt;- 30 gauge syringe</t>
+  </si>
+  <si>
+    <t>sec/vol-change</t>
+  </si>
+  <si>
+    <t>min/vol-change</t>
+  </si>
+  <si>
+    <t>hour/vol-change</t>
+  </si>
+  <si>
+    <t>V_dot_bioreactor</t>
+  </si>
+  <si>
+    <t>Reactor Residence Time [min]</t>
+  </si>
+  <si>
+    <t>Reactor Residence Time [hr]</t>
+  </si>
+  <si>
+    <t>Residence Time In scaffold [min]</t>
+  </si>
+  <si>
+    <t>syringe length</t>
+  </si>
+  <si>
+    <t>Number of Reactors</t>
+  </si>
+  <si>
+    <t>Flow Rate source</t>
+  </si>
+  <si>
+    <t>Source Volume [ml]</t>
+  </si>
+  <si>
+    <t>Change Interval [hr]</t>
+  </si>
+  <si>
+    <t>Flow Rate/reactor [ul/hr]</t>
+  </si>
+  <si>
+    <t>Source vel [m/s]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000000000"/>
+    <numFmt numFmtId="165" formatCode="0.0000000000"/>
+    <numFmt numFmtId="166" formatCode="0.00000"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -2265,7 +2309,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="149">
+  <cellStyleXfs count="161">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2415,8 +2459,20 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2495,8 +2551,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="149">
+  <cellStyles count="161">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2571,6 +2629,12 @@
     <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2645,6 +2709,12 @@
     <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2976,8 +3046,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:DR181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="D68" sqref="D68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2989,9 +3059,14 @@
     <col min="8" max="8" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.1640625" customWidth="1"/>
+    <col min="16" max="16" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="8" customFormat="1">
+    <row r="1" spans="1:17" s="8" customFormat="1">
       <c r="A1" s="43" t="s">
         <v>472</v>
       </c>
@@ -3010,7 +3085,7 @@
       <c r="M1" s="42"/>
       <c r="N1" s="42"/>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:17">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -3029,7 +3104,7 @@
       </c>
       <c r="J2" s="17"/>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:17">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -3048,7 +3123,7 @@
       </c>
       <c r="J3" s="17"/>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:17">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -3066,8 +3141,14 @@
         <v>500</v>
       </c>
       <c r="J4" s="17"/>
-    </row>
-    <row r="5" spans="1:14">
+      <c r="M4" t="s">
+        <v>3</v>
+      </c>
+      <c r="N4" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
       <c r="A5" s="1" t="s">
         <v>473</v>
       </c>
@@ -3095,8 +3176,15 @@
         <v>483.21136368279321</v>
       </c>
       <c r="J5" s="17"/>
-    </row>
-    <row r="6" spans="1:14">
+      <c r="M5">
+        <v>104015.61374</v>
+      </c>
+      <c r="N5">
+        <f>(M5-B7)*0.000145037738</f>
+        <v>0.95638083719051936</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
       <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
@@ -3124,7 +3212,7 @@
       </c>
       <c r="J6" s="17"/>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:17">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -3142,8 +3230,14 @@
         <v>0</v>
       </c>
       <c r="J7" s="17"/>
-    </row>
-    <row r="8" spans="1:14">
+      <c r="P7" t="s">
+        <v>675</v>
+      </c>
+      <c r="Q7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17">
       <c r="H8" s="31" t="s">
         <v>501</v>
       </c>
@@ -3152,8 +3246,14 @@
         <v>500</v>
       </c>
       <c r="J8" s="17"/>
-    </row>
-    <row r="9" spans="1:14">
+      <c r="P8" t="s">
+        <v>679</v>
+      </c>
+      <c r="Q8">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -3169,8 +3269,18 @@
         <v>9810</v>
       </c>
       <c r="J9" s="17"/>
-    </row>
-    <row r="10" spans="1:14">
+      <c r="N9" t="s">
+        <v>674</v>
+      </c>
+      <c r="P9" t="s">
+        <v>676</v>
+      </c>
+      <c r="Q9">
+        <f>Q7*Q8</f>
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -3180,8 +3290,17 @@
       <c r="H10" s="31"/>
       <c r="I10" s="7"/>
       <c r="J10" s="17"/>
-    </row>
-    <row r="11" spans="1:14">
+      <c r="N10">
+        <v>0.107</v>
+      </c>
+      <c r="P10" t="s">
+        <v>677</v>
+      </c>
+      <c r="Q10">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -3197,8 +3316,15 @@
         <v>-22.304131365184734</v>
       </c>
       <c r="J11" s="17"/>
-    </row>
-    <row r="12" spans="1:14">
+      <c r="P11" t="s">
+        <v>678</v>
+      </c>
+      <c r="Q11">
+        <f>Q10/(Q9/1000)</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17">
       <c r="A12" t="s">
         <v>474</v>
       </c>
@@ -3216,8 +3342,21 @@
         <v>-8090.9649947299904</v>
       </c>
       <c r="J12" s="17"/>
-    </row>
-    <row r="13" spans="1:14">
+      <c r="N12" t="s">
+        <v>670</v>
+      </c>
+      <c r="O12" t="s">
+        <v>519</v>
+      </c>
+      <c r="P12" t="s">
+        <v>680</v>
+      </c>
+      <c r="Q12" s="3">
+        <f>Q9/10^9/60^2/(PI()*(B24/2)^2)</f>
+        <v>1.2402953166523691E-6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -3229,11 +3368,26 @@
       </c>
       <c r="I13" s="7">
         <f>-I2*B19/(B27)^2</f>
-        <v>-1105.2631578947367</v>
+        <v>-12668.249999999996</v>
       </c>
       <c r="J13" s="17"/>
-    </row>
-    <row r="14" spans="1:14">
+      <c r="N13">
+        <f>20*(B29/2)^2*PI()</f>
+        <v>2.3379732528015242E-3</v>
+      </c>
+      <c r="O13" s="50">
+        <f>B32*N13/N14</f>
+        <v>1.2402953166523689E-6</v>
+      </c>
+      <c r="P13" t="s">
+        <v>678</v>
+      </c>
+      <c r="Q13" s="51">
+        <f>N10/Q12/60^2</f>
+        <v>23.963826858948615</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17">
       <c r="A14" t="s">
         <v>390</v>
       </c>
@@ -3248,8 +3402,12 @@
         <v>-72818.684952569907</v>
       </c>
       <c r="J14" s="17"/>
-    </row>
-    <row r="15" spans="1:14">
+      <c r="N14">
+        <f>(B24/2)^2*PI()</f>
+        <v>5.5990249670440702E-4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17">
       <c r="A15" s="36"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -3269,8 +3427,12 @@
         <v>-12.009674818597151</v>
       </c>
       <c r="J15" s="17"/>
-    </row>
-    <row r="16" spans="1:14">
+      <c r="O15">
+        <f>O13*N14*60^2*100^3</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17">
       <c r="A16" s="31" t="s">
         <v>475</v>
       </c>
@@ -3300,7 +3462,7 @@
       <c r="J16" s="17"/>
       <c r="M16" s="3"/>
     </row>
-    <row r="17" spans="1:13">
+    <row r="17" spans="1:15">
       <c r="A17" s="31" t="s">
         <v>476</v>
       </c>
@@ -3321,11 +3483,15 @@
       </c>
       <c r="I17" s="34">
         <f>-I2*B16/(B24^2)</f>
-        <v>-3.4635416666666674</v>
+        <v>-1.7910196524007909</v>
       </c>
       <c r="J17" s="35"/>
-    </row>
-    <row r="18" spans="1:13">
+      <c r="O17">
+        <f>N10/O13/60^2</f>
+        <v>23.963826858948622</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15">
       <c r="A18" s="31" t="s">
         <v>477</v>
       </c>
@@ -3345,12 +3511,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:13">
+    <row r="19" spans="1:15">
       <c r="A19" s="31" t="s">
         <v>478</v>
       </c>
       <c r="B19" s="38">
-        <v>1E-3</v>
+        <f>F19*E19</f>
+        <v>1.2699999999999999E-2</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>13</v>
@@ -3358,13 +3525,17 @@
       <c r="D19" s="7" t="s">
         <v>492</v>
       </c>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
+      <c r="E19" s="7">
+        <v>1</v>
+      </c>
+      <c r="F19" s="7">
+        <v>1.2699999999999999E-2</v>
+      </c>
       <c r="G19" s="17">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:13">
+    <row r="20" spans="1:15">
       <c r="A20" s="31" t="s">
         <v>479</v>
       </c>
@@ -3387,10 +3558,14 @@
         <v>659</v>
       </c>
       <c r="L20">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13">
+        <v>125</v>
+      </c>
+      <c r="N20">
+        <f>1/100^3</f>
+        <v>9.9999999999999995E-7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15">
       <c r="A21" s="31" t="s">
         <v>480</v>
       </c>
@@ -3410,12 +3585,16 @@
         <v>665</v>
       </c>
       <c r="L21">
-        <f>L20/60^2/100^3</f>
-        <v>1.3888888888888889E-8</v>
+        <f>L20/60^2/10^9</f>
+        <v>3.4722222222222221E-11</v>
       </c>
       <c r="M21" s="3"/>
-    </row>
-    <row r="22" spans="1:13">
+      <c r="N21">
+        <f>1/10^9</f>
+        <v>1.0000000000000001E-9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15">
       <c r="A22" s="39" t="s">
         <v>481</v>
       </c>
@@ -3434,7 +3613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:13">
+    <row r="23" spans="1:15">
       <c r="A23" s="36"/>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
@@ -3452,13 +3631,16 @@
       <c r="L23">
         <v>6.0000000000000001E-3</v>
       </c>
-    </row>
-    <row r="24" spans="1:13">
+      <c r="M23" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15">
       <c r="A24" s="31" t="s">
         <v>482</v>
       </c>
       <c r="B24" s="41">
-        <v>1.9199999999999998E-2</v>
+        <v>2.6700000000000002E-2</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>13</v>
@@ -3477,8 +3659,16 @@
       <c r="L24">
         <v>1.2E-2</v>
       </c>
-    </row>
-    <row r="25" spans="1:13">
+      <c r="M24">
+        <f>L24/B32/60</f>
+        <v>673.33629680683907</v>
+      </c>
+      <c r="N24">
+        <f>M24/60</f>
+        <v>11.222271613447317</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15">
       <c r="A25" s="31" t="s">
         <v>483</v>
       </c>
@@ -3501,8 +3691,17 @@
         <f>PI()*(L23/2)^2*L24</f>
         <v>3.3929200658769765E-7</v>
       </c>
-    </row>
-    <row r="26" spans="1:13">
+      <c r="M25" t="s">
+        <v>667</v>
+      </c>
+      <c r="N25" t="s">
+        <v>668</v>
+      </c>
+      <c r="O25" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15">
       <c r="A26" s="31" t="s">
         <v>484</v>
       </c>
@@ -3518,13 +3717,25 @@
       <c r="G26" s="17">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:13">
+      <c r="M26">
+        <f>L25/L21</f>
+        <v>9771.6097897256932</v>
+      </c>
+      <c r="N26">
+        <f>M26/60</f>
+        <v>162.86016316209489</v>
+      </c>
+      <c r="O26">
+        <f>N26/60</f>
+        <v>2.7143360527015816</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15">
       <c r="A27" s="31" t="s">
         <v>485</v>
       </c>
       <c r="B27" s="7">
-        <v>1.5200000000000001E-4</v>
+        <v>1.6000000000000001E-4</v>
       </c>
       <c r="C27" s="7" t="s">
         <v>13</v>
@@ -3548,7 +3759,7 @@
         <v>1.4027839516809146E-6</v>
       </c>
     </row>
-    <row r="28" spans="1:13">
+    <row r="28" spans="1:15">
       <c r="A28" s="31" t="s">
         <v>486</v>
       </c>
@@ -3572,7 +3783,7 @@
         <v>24.187046492878256</v>
       </c>
     </row>
-    <row r="29" spans="1:13">
+    <row r="29" spans="1:15">
       <c r="A29" s="31" t="s">
         <v>487</v>
       </c>
@@ -3589,7 +3800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:13">
+    <row r="30" spans="1:15">
       <c r="A30" s="39" t="s">
         <v>488</v>
       </c>
@@ -3605,21 +3816,37 @@
       <c r="G30" s="35">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:13">
+      <c r="M30" t="s">
+        <v>671</v>
+      </c>
+      <c r="N30" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15">
+      <c r="M31">
+        <f>B21/B32/60</f>
+        <v>3927.7950647065613</v>
+      </c>
+      <c r="N31">
+        <f>M31/60</f>
+        <v>65.463251078442696</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15">
       <c r="A32" t="s">
         <v>470</v>
       </c>
       <c r="B32" s="30">
         <f>D32*E32</f>
-        <v>4.9121896016017085E-4</v>
+        <v>2.9702839568943406E-7</v>
       </c>
       <c r="C32" t="s">
         <v>16</v>
       </c>
       <c r="D32">
-        <f>L21/(PI()*(L23/2)^2)</f>
-        <v>4.9121896016017085E-4</v>
+        <f>L21/(PI()*(B29/2)^2)</f>
+        <v>2.9702839568943406E-7</v>
       </c>
       <c r="E32">
         <v>1</v>
@@ -3643,7 +3870,7 @@
       </c>
       <c r="I34">
         <f ca="1">1+RAND()*F16*IF(RAND()&gt;0.5,1,-1)</f>
-        <v>0.99525488945765583</v>
+        <v>0.96167861021466028</v>
       </c>
     </row>
     <row r="35" spans="1:10">
@@ -3658,7 +3885,7 @@
       </c>
       <c r="I35">
         <f ca="1">ROUND(RAND(),0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:10">
@@ -4172,11 +4399,11 @@
       </c>
       <c r="B50" s="7">
         <f ca="1">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$24+($G$24=0))*($B$24*(B54=0)+B55*B54)</f>
-        <v>1.9199999999999998E-2</v>
+        <v>2.6700000000000002E-2</v>
       </c>
       <c r="C50" s="7">
         <f ca="1">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$25+($G$25=0))*($B$25*(C54=0)+C55*C54)</f>
-        <v>1.0936528803737525E-3</v>
+        <v>1.1457342506153738E-3</v>
       </c>
       <c r="D50" s="7">
         <f ca="1">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$26+($G$26=0))*($B$26*(D54=0)+D55*D54)</f>
@@ -4184,7 +4411,7 @@
       </c>
       <c r="E50" s="7">
         <f ca="1">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$27+($G$27=0))*($B$27*(E54=0)+E55*E54)</f>
-        <v>1.5200000000000001E-4</v>
+        <v>1.6000000000000001E-4</v>
       </c>
       <c r="F50" s="7">
         <f ca="1">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$28+($G$28=0))*($B$28*(F54=0)+F55*F54)</f>
@@ -4200,7 +4427,7 @@
       </c>
       <c r="I50" s="7">
         <f t="shared" ref="I50" ca="1" si="1">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$25+($G$25=0))*($B$25*(I54=0)+I55*I54)</f>
-        <v>1.0809803407347642E-3</v>
+        <v>1.1018734474090481E-3</v>
       </c>
       <c r="J50" s="7">
         <f t="shared" ref="J50" ca="1" si="2">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$26+($G$26=0))*($B$26*(J54=0)+J55*J54)</f>
@@ -4208,7 +4435,7 @@
       </c>
       <c r="K50" s="7">
         <f t="shared" ref="K50" ca="1" si="3">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$27+($G$27=0))*($B$27*(K54=0)+K55*K54)</f>
-        <v>1.5200000000000001E-4</v>
+        <v>1.6000000000000001E-4</v>
       </c>
       <c r="L50" s="7">
         <f t="shared" ref="L50" ca="1" si="4">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$28+($G$28=0))*($B$28*(L54=0)+L55*L54)</f>
@@ -4224,7 +4451,7 @@
       </c>
       <c r="O50" s="7">
         <f t="shared" ref="O50" ca="1" si="7">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$25+($G$25=0))*($B$25*(O54=0)+O55*O54)</f>
-        <v>9.7644276405843718E-4</v>
+        <v>9.7807852162779788E-4</v>
       </c>
       <c r="P50" s="7">
         <f t="shared" ref="P50" ca="1" si="8">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$26+($G$26=0))*($B$26*(P54=0)+P55*P54)</f>
@@ -4232,7 +4459,7 @@
       </c>
       <c r="Q50" s="7">
         <f t="shared" ref="Q50" ca="1" si="9">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$27+($G$27=0))*($B$27*(Q54=0)+Q55*Q54)</f>
-        <v>1.5200000000000001E-4</v>
+        <v>1.6000000000000001E-4</v>
       </c>
       <c r="R50" s="7">
         <f t="shared" ref="R50" ca="1" si="10">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$28+($G$28=0))*($B$28*(R54=0)+R55*R54)</f>
@@ -4248,7 +4475,7 @@
       </c>
       <c r="U50" s="7">
         <f t="shared" ref="U50" ca="1" si="13">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$25+($G$25=0))*($B$25*(U54=0)+U55*U54)</f>
-        <v>1.0072184448302259E-3</v>
+        <v>1.0700924767829633E-3</v>
       </c>
       <c r="V50" s="7">
         <f t="shared" ref="V50" ca="1" si="14">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$26+($G$26=0))*($B$26*(V54=0)+V55*V54)</f>
@@ -4256,7 +4483,7 @@
       </c>
       <c r="W50" s="7">
         <f t="shared" ref="W50" ca="1" si="15">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$27+($G$27=0))*($B$27*(W54=0)+W55*W54)</f>
-        <v>1.5200000000000001E-4</v>
+        <v>1.6000000000000001E-4</v>
       </c>
       <c r="X50" s="7">
         <f t="shared" ref="X50" ca="1" si="16">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$28+($G$28=0))*($B$28*(X54=0)+X55*X54)</f>
@@ -4272,7 +4499,7 @@
       </c>
       <c r="AA50" s="7">
         <f t="shared" ref="AA50" ca="1" si="19">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$25+($G$25=0))*($B$25*(AA54=0)+AA55*AA54)</f>
-        <v>9.94300177038572E-4</v>
+        <v>1.0250094228422811E-3</v>
       </c>
       <c r="AB50" s="7">
         <f t="shared" ref="AB50" ca="1" si="20">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$26+($G$26=0))*($B$26*(AB54=0)+AB55*AB54)</f>
@@ -4280,7 +4507,7 @@
       </c>
       <c r="AC50" s="7">
         <f t="shared" ref="AC50" ca="1" si="21">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$27+($G$27=0))*($B$27*(AC54=0)+AC55*AC54)</f>
-        <v>1.5200000000000001E-4</v>
+        <v>1.6000000000000001E-4</v>
       </c>
       <c r="AD50" s="7">
         <f t="shared" ref="AD50" ca="1" si="22">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$28+($G$28=0))*($B$28*(AD54=0)+AD55*AD54)</f>
@@ -4296,7 +4523,7 @@
       </c>
       <c r="AG50" s="7">
         <f t="shared" ref="AG50" ca="1" si="25">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$25+($G$25=0))*($B$25*(AG54=0)+AG55*AG54)</f>
-        <v>9.9876921849646034E-4</v>
+        <v>1.1005068126898789E-3</v>
       </c>
       <c r="AH50" s="7">
         <f t="shared" ref="AH50" ca="1" si="26">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$26+($G$26=0))*($B$26*(AH54=0)+AH55*AH54)</f>
@@ -4304,7 +4531,7 @@
       </c>
       <c r="AI50" s="7">
         <f t="shared" ref="AI50" ca="1" si="27">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$27+($G$27=0))*($B$27*(AI54=0)+AI55*AI54)</f>
-        <v>1.5200000000000001E-4</v>
+        <v>1.6000000000000001E-4</v>
       </c>
       <c r="AJ50" s="7">
         <f t="shared" ref="AJ50" ca="1" si="28">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$28+($G$28=0))*($B$28*(AJ54=0)+AJ55*AJ54)</f>
@@ -4320,7 +4547,7 @@
       </c>
       <c r="AM50" s="7">
         <f t="shared" ref="AM50" ca="1" si="31">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$25+($G$25=0))*($B$25*(AM54=0)+AM55*AM54)</f>
-        <v>1.1240622513536255E-3</v>
+        <v>1.1738023629627504E-3</v>
       </c>
       <c r="AN50" s="7">
         <f t="shared" ref="AN50" ca="1" si="32">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$26+($G$26=0))*($B$26*(AN54=0)+AN55*AN54)</f>
@@ -4328,7 +4555,7 @@
       </c>
       <c r="AO50" s="7">
         <f t="shared" ref="AO50" ca="1" si="33">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$27+($G$27=0))*($B$27*(AO54=0)+AO55*AO54)</f>
-        <v>1.5200000000000001E-4</v>
+        <v>1.6000000000000001E-4</v>
       </c>
       <c r="AP50" s="7">
         <f t="shared" ref="AP50" ca="1" si="34">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$28+($G$28=0))*($B$28*(AP54=0)+AP55*AP54)</f>
@@ -4344,7 +4571,7 @@
       </c>
       <c r="AS50" s="7">
         <f t="shared" ref="AS50" ca="1" si="37">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$25+($G$25=0))*($B$25*(AS54=0)+AS55*AS54)</f>
-        <v>1.1317969705969863E-3</v>
+        <v>9.7704108891370767E-4</v>
       </c>
       <c r="AT50" s="7">
         <f t="shared" ref="AT50" ca="1" si="38">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$26+($G$26=0))*($B$26*(AT54=0)+AT55*AT54)</f>
@@ -4352,7 +4579,7 @@
       </c>
       <c r="AU50" s="7">
         <f t="shared" ref="AU50" ca="1" si="39">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$27+($G$27=0))*($B$27*(AU54=0)+AU55*AU54)</f>
-        <v>1.5200000000000001E-4</v>
+        <v>1.6000000000000001E-4</v>
       </c>
       <c r="AV50" s="7">
         <f t="shared" ref="AV50" ca="1" si="40">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$28+($G$28=0))*($B$28*(AV54=0)+AV55*AV54)</f>
@@ -4368,7 +4595,7 @@
       </c>
       <c r="AY50" s="7">
         <f t="shared" ref="AY50" ca="1" si="43">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$25+($G$25=0))*($B$25*(AY54=0)+AY55*AY54)</f>
-        <v>1.0512392299987128E-3</v>
+        <v>1.1180826844703247E-3</v>
       </c>
       <c r="AZ50" s="7">
         <f t="shared" ref="AZ50" ca="1" si="44">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$26+($G$26=0))*($B$26*(AZ54=0)+AZ55*AZ54)</f>
@@ -4376,7 +4603,7 @@
       </c>
       <c r="BA50" s="7">
         <f t="shared" ref="BA50" ca="1" si="45">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$27+($G$27=0))*($B$27*(BA54=0)+BA55*BA54)</f>
-        <v>1.5200000000000001E-4</v>
+        <v>1.6000000000000001E-4</v>
       </c>
       <c r="BB50" s="7">
         <f t="shared" ref="BB50" ca="1" si="46">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$28+($G$28=0))*($B$28*(BB54=0)+BB55*BB54)</f>
@@ -4392,7 +4619,7 @@
       </c>
       <c r="BE50" s="7">
         <f t="shared" ref="BE50" ca="1" si="49">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$25+($G$25=0))*($B$25*(BE54=0)+BE55*BE54)</f>
-        <v>1.1631241559320667E-3</v>
+        <v>1.0316969530925408E-3</v>
       </c>
       <c r="BF50" s="7">
         <f t="shared" ref="BF50" ca="1" si="50">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$26+($G$26=0))*($B$26*(BF54=0)+BF55*BF54)</f>
@@ -4400,7 +4627,7 @@
       </c>
       <c r="BG50" s="7">
         <f t="shared" ref="BG50" ca="1" si="51">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$27+($G$27=0))*($B$27*(BG54=0)+BG55*BG54)</f>
-        <v>1.5200000000000001E-4</v>
+        <v>1.6000000000000001E-4</v>
       </c>
       <c r="BH50" s="7">
         <f t="shared" ref="BH50" ca="1" si="52">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$28+($G$28=0))*($B$28*(BH54=0)+BH55*BH54)</f>
@@ -4416,7 +4643,7 @@
       </c>
       <c r="BK50" s="7">
         <f t="shared" ref="BK50" ca="1" si="55">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$25+($G$25=0))*($B$25*(BK54=0)+BK55*BK54)</f>
-        <v>1.0803430463264569E-3</v>
+        <v>1.1380097522071466E-3</v>
       </c>
       <c r="BL50" s="7">
         <f t="shared" ref="BL50" ca="1" si="56">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$26+($G$26=0))*($B$26*(BL54=0)+BL55*BL54)</f>
@@ -4424,7 +4651,7 @@
       </c>
       <c r="BM50" s="7">
         <f t="shared" ref="BM50" ca="1" si="57">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$27+($G$27=0))*($B$27*(BM54=0)+BM55*BM54)</f>
-        <v>1.5200000000000001E-4</v>
+        <v>1.6000000000000001E-4</v>
       </c>
       <c r="BN50" s="7">
         <f t="shared" ref="BN50" ca="1" si="58">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$28+($G$28=0))*($B$28*(BN54=0)+BN55*BN54)</f>
@@ -4440,7 +4667,7 @@
       </c>
       <c r="BQ50" s="7">
         <f t="shared" ref="BQ50" ca="1" si="61">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$25+($G$25=0))*($B$25*(BQ54=0)+BQ55*BQ54)</f>
-        <v>9.8432757558565391E-4</v>
+        <v>9.8744414424573718E-4</v>
       </c>
       <c r="BR50" s="7">
         <f t="shared" ref="BR50" ca="1" si="62">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$26+($G$26=0))*($B$26*(BR54=0)+BR55*BR54)</f>
@@ -4448,7 +4675,7 @@
       </c>
       <c r="BS50" s="7">
         <f t="shared" ref="BS50" ca="1" si="63">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$27+($G$27=0))*($B$27*(BS54=0)+BS55*BS54)</f>
-        <v>1.5200000000000001E-4</v>
+        <v>1.6000000000000001E-4</v>
       </c>
       <c r="BT50" s="7">
         <f t="shared" ref="BT50" ca="1" si="64">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$28+($G$28=0))*($B$28*(BT54=0)+BT55*BT54)</f>
@@ -4464,7 +4691,7 @@
       </c>
       <c r="BW50" s="7">
         <f t="shared" ref="BW50" ca="1" si="67">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$25+($G$25=0))*($B$25*(BW54=0)+BW55*BW54)</f>
-        <v>1.03282138438224E-3</v>
+        <v>1.0886570699087327E-3</v>
       </c>
       <c r="BX50" s="7">
         <f t="shared" ref="BX50" ca="1" si="68">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$26+($G$26=0))*($B$26*(BX54=0)+BX55*BX54)</f>
@@ -4472,7 +4699,7 @@
       </c>
       <c r="BY50" s="7">
         <f t="shared" ref="BY50" ca="1" si="69">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$27+($G$27=0))*($B$27*(BY54=0)+BY55*BY54)</f>
-        <v>1.5200000000000001E-4</v>
+        <v>1.6000000000000001E-4</v>
       </c>
       <c r="BZ50" s="7">
         <f t="shared" ref="BZ50" ca="1" si="70">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$28+($G$28=0))*($B$28*(BZ54=0)+BZ55*BZ54)</f>
@@ -4488,7 +4715,7 @@
       </c>
       <c r="CC50" s="7">
         <f t="shared" ref="CC50" ca="1" si="73">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$25+($G$25=0))*($B$25*(CC54=0)+CC55*CC54)</f>
-        <v>1.1248441206555984E-3</v>
+        <v>1.026795304041261E-3</v>
       </c>
       <c r="CD50" s="7">
         <f t="shared" ref="CD50" ca="1" si="74">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$26+($G$26=0))*($B$26*(CD54=0)+CD55*CD54)</f>
@@ -4496,7 +4723,7 @@
       </c>
       <c r="CE50" s="7">
         <f t="shared" ref="CE50" ca="1" si="75">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$27+($G$27=0))*($B$27*(CE54=0)+CE55*CE54)</f>
-        <v>1.5200000000000001E-4</v>
+        <v>1.6000000000000001E-4</v>
       </c>
       <c r="CF50" s="7">
         <f t="shared" ref="CF50" ca="1" si="76">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$28+($G$28=0))*($B$28*(CF54=0)+CF55*CF54)</f>
@@ -4512,7 +4739,7 @@
       </c>
       <c r="CI50" s="7">
         <f t="shared" ref="CI50" ca="1" si="79">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$25+($G$25=0))*($B$25*(CI54=0)+CI55*CI54)</f>
-        <v>1.1620797443383068E-3</v>
+        <v>1.098805578734709E-3</v>
       </c>
       <c r="CJ50" s="7">
         <f t="shared" ref="CJ50" ca="1" si="80">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$26+($G$26=0))*($B$26*(CJ54=0)+CJ55*CJ54)</f>
@@ -4520,7 +4747,7 @@
       </c>
       <c r="CK50" s="7">
         <f t="shared" ref="CK50" ca="1" si="81">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$27+($G$27=0))*($B$27*(CK54=0)+CK55*CK54)</f>
-        <v>1.5200000000000001E-4</v>
+        <v>1.6000000000000001E-4</v>
       </c>
       <c r="CL50" s="7">
         <f t="shared" ref="CL50" ca="1" si="82">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$28+($G$28=0))*($B$28*(CL54=0)+CL55*CL54)</f>
@@ -4536,7 +4763,7 @@
       </c>
       <c r="CO50" s="7">
         <f t="shared" ref="CO50" ca="1" si="85">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$25+($G$25=0))*($B$25*(CO54=0)+CO55*CO54)</f>
-        <v>9.6417493981809091E-4</v>
+        <v>1.0077457000628326E-3</v>
       </c>
       <c r="CP50" s="7">
         <f t="shared" ref="CP50" ca="1" si="86">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$26+($G$26=0))*($B$26*(CP54=0)+CP55*CP54)</f>
@@ -4544,7 +4771,7 @@
       </c>
       <c r="CQ50" s="7">
         <f t="shared" ref="CQ50" ca="1" si="87">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$27+($G$27=0))*($B$27*(CQ54=0)+CQ55*CQ54)</f>
-        <v>1.5200000000000001E-4</v>
+        <v>1.6000000000000001E-4</v>
       </c>
       <c r="CR50" s="7">
         <f t="shared" ref="CR50" ca="1" si="88">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$28+($G$28=0))*($B$28*(CR54=0)+CR55*CR54)</f>
@@ -4560,7 +4787,7 @@
       </c>
       <c r="CU50" s="7">
         <f t="shared" ref="CU50" ca="1" si="91">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$25+($G$25=0))*($B$25*(CU54=0)+CU55*CU54)</f>
-        <v>1.0055583863316407E-3</v>
+        <v>1.0726524354769803E-3</v>
       </c>
       <c r="CV50" s="7">
         <f t="shared" ref="CV50" ca="1" si="92">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$26+($G$26=0))*($B$26*(CV54=0)+CV55*CV54)</f>
@@ -4568,7 +4795,7 @@
       </c>
       <c r="CW50" s="7">
         <f t="shared" ref="CW50" ca="1" si="93">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$27+($G$27=0))*($B$27*(CW54=0)+CW55*CW54)</f>
-        <v>1.5200000000000001E-4</v>
+        <v>1.6000000000000001E-4</v>
       </c>
       <c r="CX50" s="7">
         <f t="shared" ref="CX50" ca="1" si="94">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$28+($G$28=0))*($B$28*(CX54=0)+CX55*CX54)</f>
@@ -4584,7 +4811,7 @@
       </c>
       <c r="DA50" s="7">
         <f t="shared" ref="DA50" ca="1" si="97">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$25+($G$25=0))*($B$25*(DA54=0)+DA55*DA54)</f>
-        <v>1.0623482574907063E-3</v>
+        <v>1.1756581567291741E-3</v>
       </c>
       <c r="DB50" s="7">
         <f t="shared" ref="DB50" ca="1" si="98">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$26+($G$26=0))*($B$26*(DB54=0)+DB55*DB54)</f>
@@ -4592,7 +4819,7 @@
       </c>
       <c r="DC50" s="7">
         <f t="shared" ref="DC50" ca="1" si="99">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$27+($G$27=0))*($B$27*(DC54=0)+DC55*DC54)</f>
-        <v>1.5200000000000001E-4</v>
+        <v>1.6000000000000001E-4</v>
       </c>
       <c r="DD50" s="7">
         <f t="shared" ref="DD50" ca="1" si="100">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$28+($G$28=0))*($B$28*(DD54=0)+DD55*DD54)</f>
@@ -4608,7 +4835,7 @@
       </c>
       <c r="DG50" s="7">
         <f t="shared" ref="DG50" ca="1" si="103">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$25+($G$25=0))*($B$25*(DG54=0)+DG55*DG54)</f>
-        <v>1.1190825281185341E-3</v>
+        <v>9.9143158431283496E-4</v>
       </c>
       <c r="DH50" s="7">
         <f t="shared" ref="DH50" ca="1" si="104">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$26+($G$26=0))*($B$26*(DH54=0)+DH55*DH54)</f>
@@ -4616,7 +4843,7 @@
       </c>
       <c r="DI50" s="7">
         <f t="shared" ref="DI50" ca="1" si="105">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$27+($G$27=0))*($B$27*(DI54=0)+DI55*DI54)</f>
-        <v>1.5200000000000001E-4</v>
+        <v>1.6000000000000001E-4</v>
       </c>
       <c r="DJ50" s="7">
         <f t="shared" ref="DJ50" ca="1" si="106">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$28+($G$28=0))*($B$28*(DJ54=0)+DJ55*DJ54)</f>
@@ -4632,7 +4859,7 @@
       </c>
       <c r="DM50" s="7">
         <f t="shared" ref="DM50" ca="1" si="109">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$25+($G$25=0))*($B$25*(DM54=0)+DM55*DM54)</f>
-        <v>1.1043018498480012E-3</v>
+        <v>9.9715770363938009E-4</v>
       </c>
       <c r="DN50" s="7">
         <f t="shared" ref="DN50" ca="1" si="110">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$26+($G$26=0))*($B$26*(DN54=0)+DN55*DN54)</f>
@@ -4640,7 +4867,7 @@
       </c>
       <c r="DO50" s="7">
         <f t="shared" ref="DO50" ca="1" si="111">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$27+($G$27=0))*($B$27*(DO54=0)+DO55*DO54)</f>
-        <v>1.5200000000000001E-4</v>
+        <v>1.6000000000000001E-4</v>
       </c>
       <c r="DP50" s="7">
         <f t="shared" ref="DP50" ca="1" si="112">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$28+($G$28=0))*($B$28*(DP54=0)+DP55*DP54)</f>
@@ -4673,7 +4900,7 @@
       </c>
       <c r="E51" s="7">
         <f ca="1">(RAND()*$G$19+($G$19=0))*($B$19*(E57=0)+E58*E57)</f>
-        <v>1E-3</v>
+        <v>1.2699999999999999E-2</v>
       </c>
       <c r="F51" s="7">
         <f ca="1">(RAND()*$G$20+($G$20=0))*($B$20*(F57=0)+F58*F57)</f>
@@ -4697,7 +4924,7 @@
       </c>
       <c r="K51" s="7">
         <f ca="1">(RAND()*$G$19+($G$19=0))*($B$19*(K57=0)+K58*K57)</f>
-        <v>1E-3</v>
+        <v>1.2699999999999999E-2</v>
       </c>
       <c r="L51" s="7">
         <f ca="1">(RAND()*$G$20+($G$20=0))*($B$20*(L57=0)+L58*L57)</f>
@@ -4721,7 +4948,7 @@
       </c>
       <c r="Q51" s="7">
         <f ca="1">(RAND()*$G$19+($G$19=0))*($B$19*(Q57=0)+Q58*Q57)</f>
-        <v>1E-3</v>
+        <v>1.2699999999999999E-2</v>
       </c>
       <c r="R51" s="7">
         <f ca="1">(RAND()*$G$20+($G$20=0))*($B$20*(R57=0)+R58*R57)</f>
@@ -4745,7 +4972,7 @@
       </c>
       <c r="W51" s="7">
         <f ca="1">(RAND()*$G$19+($G$19=0))*($B$19*(W57=0)+W58*W57)</f>
-        <v>1E-3</v>
+        <v>1.2699999999999999E-2</v>
       </c>
       <c r="X51" s="7">
         <f ca="1">(RAND()*$G$20+($G$20=0))*($B$20*(X57=0)+X58*X57)</f>
@@ -4769,7 +4996,7 @@
       </c>
       <c r="AC51" s="7">
         <f ca="1">(RAND()*$G$19+($G$19=0))*($B$19*(AC57=0)+AC58*AC57)</f>
-        <v>1E-3</v>
+        <v>1.2699999999999999E-2</v>
       </c>
       <c r="AD51" s="7">
         <f ca="1">(RAND()*$G$20+($G$20=0))*($B$20*(AD57=0)+AD58*AD57)</f>
@@ -4793,7 +5020,7 @@
       </c>
       <c r="AI51" s="7">
         <f ca="1">(RAND()*$G$19+($G$19=0))*($B$19*(AI57=0)+AI58*AI57)</f>
-        <v>1E-3</v>
+        <v>1.2699999999999999E-2</v>
       </c>
       <c r="AJ51" s="7">
         <f ca="1">(RAND()*$G$20+($G$20=0))*($B$20*(AJ57=0)+AJ58*AJ57)</f>
@@ -4817,7 +5044,7 @@
       </c>
       <c r="AO51" s="7">
         <f ca="1">(RAND()*$G$19+($G$19=0))*($B$19*(AO57=0)+AO58*AO57)</f>
-        <v>1E-3</v>
+        <v>1.2699999999999999E-2</v>
       </c>
       <c r="AP51" s="7">
         <f ca="1">(RAND()*$G$20+($G$20=0))*($B$20*(AP57=0)+AP58*AP57)</f>
@@ -4841,7 +5068,7 @@
       </c>
       <c r="AU51" s="7">
         <f ca="1">(RAND()*$G$19+($G$19=0))*($B$19*(AU57=0)+AU58*AU57)</f>
-        <v>1E-3</v>
+        <v>1.2699999999999999E-2</v>
       </c>
       <c r="AV51" s="7">
         <f ca="1">(RAND()*$G$20+($G$20=0))*($B$20*(AV57=0)+AV58*AV57)</f>
@@ -4865,7 +5092,7 @@
       </c>
       <c r="BA51" s="7">
         <f ca="1">(RAND()*$G$19+($G$19=0))*($B$19*(BA57=0)+BA58*BA57)</f>
-        <v>1E-3</v>
+        <v>1.2699999999999999E-2</v>
       </c>
       <c r="BB51" s="7">
         <f ca="1">(RAND()*$G$20+($G$20=0))*($B$20*(BB57=0)+BB58*BB57)</f>
@@ -4889,7 +5116,7 @@
       </c>
       <c r="BG51" s="7">
         <f ca="1">(RAND()*$G$19+($G$19=0))*($B$19*(BG57=0)+BG58*BG57)</f>
-        <v>1E-3</v>
+        <v>1.2699999999999999E-2</v>
       </c>
       <c r="BH51" s="7">
         <f ca="1">(RAND()*$G$20+($G$20=0))*($B$20*(BH57=0)+BH58*BH57)</f>
@@ -4913,7 +5140,7 @@
       </c>
       <c r="BM51" s="7">
         <f ca="1">(RAND()*$G$19+($G$19=0))*($B$19*(BM57=0)+BM58*BM57)</f>
-        <v>1E-3</v>
+        <v>1.2699999999999999E-2</v>
       </c>
       <c r="BN51" s="7">
         <f ca="1">(RAND()*$G$20+($G$20=0))*($B$20*(BN57=0)+BN58*BN57)</f>
@@ -4937,7 +5164,7 @@
       </c>
       <c r="BS51" s="7">
         <f ca="1">(RAND()*$G$19+($G$19=0))*($B$19*(BS57=0)+BS58*BS57)</f>
-        <v>1E-3</v>
+        <v>1.2699999999999999E-2</v>
       </c>
       <c r="BT51" s="7">
         <f ca="1">(RAND()*$G$20+($G$20=0))*($B$20*(BT57=0)+BT58*BT57)</f>
@@ -4961,7 +5188,7 @@
       </c>
       <c r="BY51" s="7">
         <f ca="1">(RAND()*$G$19+($G$19=0))*($B$19*(BY57=0)+BY58*BY57)</f>
-        <v>1E-3</v>
+        <v>1.2699999999999999E-2</v>
       </c>
       <c r="BZ51" s="7">
         <f ca="1">(RAND()*$G$20+($G$20=0))*($B$20*(BZ57=0)+BZ58*BZ57)</f>
@@ -4985,7 +5212,7 @@
       </c>
       <c r="CE51" s="7">
         <f ca="1">(RAND()*$G$19+($G$19=0))*($B$19*(CE57=0)+CE58*CE57)</f>
-        <v>1E-3</v>
+        <v>1.2699999999999999E-2</v>
       </c>
       <c r="CF51" s="7">
         <f ca="1">(RAND()*$G$20+($G$20=0))*($B$20*(CF57=0)+CF58*CF57)</f>
@@ -5009,7 +5236,7 @@
       </c>
       <c r="CK51" s="7">
         <f ca="1">(RAND()*$G$19+($G$19=0))*($B$19*(CK57=0)+CK58*CK57)</f>
-        <v>1E-3</v>
+        <v>1.2699999999999999E-2</v>
       </c>
       <c r="CL51" s="7">
         <f ca="1">(RAND()*$G$20+($G$20=0))*($B$20*(CL57=0)+CL58*CL57)</f>
@@ -5033,7 +5260,7 @@
       </c>
       <c r="CQ51" s="7">
         <f ca="1">(RAND()*$G$19+($G$19=0))*($B$19*(CQ57=0)+CQ58*CQ57)</f>
-        <v>1E-3</v>
+        <v>1.2699999999999999E-2</v>
       </c>
       <c r="CR51" s="7">
         <f ca="1">(RAND()*$G$20+($G$20=0))*($B$20*(CR57=0)+CR58*CR57)</f>
@@ -5057,7 +5284,7 @@
       </c>
       <c r="CW51" s="7">
         <f ca="1">(RAND()*$G$19+($G$19=0))*($B$19*(CW57=0)+CW58*CW57)</f>
-        <v>1E-3</v>
+        <v>1.2699999999999999E-2</v>
       </c>
       <c r="CX51" s="7">
         <f ca="1">(RAND()*$G$20+($G$20=0))*($B$20*(CX57=0)+CX58*CX57)</f>
@@ -5081,7 +5308,7 @@
       </c>
       <c r="DC51" s="7">
         <f ca="1">(RAND()*$G$19+($G$19=0))*($B$19*(DC57=0)+DC58*DC57)</f>
-        <v>1E-3</v>
+        <v>1.2699999999999999E-2</v>
       </c>
       <c r="DD51" s="7">
         <f ca="1">(RAND()*$G$20+($G$20=0))*($B$20*(DD57=0)+DD58*DD57)</f>
@@ -5105,7 +5332,7 @@
       </c>
       <c r="DI51" s="7">
         <f ca="1">(RAND()*$G$19+($G$19=0))*($B$19*(DI57=0)+DI58*DI57)</f>
-        <v>1E-3</v>
+        <v>1.2699999999999999E-2</v>
       </c>
       <c r="DJ51" s="7">
         <f ca="1">(RAND()*$G$20+($G$20=0))*($B$20*(DJ57=0)+DJ58*DJ57)</f>
@@ -5129,7 +5356,7 @@
       </c>
       <c r="DO51" s="7">
         <f ca="1">(RAND()*$G$19+($G$19=0))*($B$19*(DO57=0)+DO58*DO57)</f>
-        <v>1E-3</v>
+        <v>1.2699999999999999E-2</v>
       </c>
       <c r="DP51" s="7">
         <f ca="1">(RAND()*$G$20+($G$20=0))*($B$20*(DP57=0)+DP58*DP57)</f>
@@ -5150,11 +5377,11 @@
       </c>
       <c r="B52" s="7">
         <f ca="1">-$I$2*B51/(B50^2)</f>
-        <v>-3.4635416666666674</v>
+        <v>-1.7910196524007909</v>
       </c>
       <c r="C52" s="7">
         <f t="shared" ref="C52:H52" ca="1" si="115">-$I$2*C51/(C50^2)</f>
-        <v>-21.349802775421026</v>
+        <v>-19.452932394345336</v>
       </c>
       <c r="D52" s="7">
         <f t="shared" ca="1" si="115"/>
@@ -5162,7 +5389,7 @@
       </c>
       <c r="E52" s="7">
         <f t="shared" ca="1" si="115"/>
-        <v>-1105.2631578947367</v>
+        <v>-12668.249999999996</v>
       </c>
       <c r="F52" s="7">
         <f t="shared" ca="1" si="115"/>
@@ -5178,7 +5405,7 @@
       </c>
       <c r="I52" s="7">
         <f t="shared" ref="I52" ca="1" si="116">-$I$2*I51/(I50^2)</f>
-        <v>-21.853312604256569</v>
+        <v>-21.032429132701449</v>
       </c>
       <c r="J52" s="7">
         <f t="shared" ref="J52" ca="1" si="117">-$I$2*J51/(J50^2)</f>
@@ -5186,7 +5413,7 @@
       </c>
       <c r="K52" s="7">
         <f t="shared" ref="K52" ca="1" si="118">-$I$2*K51/(K50^2)</f>
-        <v>-1105.2631578947367</v>
+        <v>-12668.249999999996</v>
       </c>
       <c r="L52" s="7">
         <f t="shared" ref="L52" ca="1" si="119">-$I$2*L51/(L50^2)</f>
@@ -5202,7 +5429,7 @@
       </c>
       <c r="O52" s="7">
         <f t="shared" ref="O52" ca="1" si="122">-$I$2*O51/(O50^2)</f>
-        <v>-26.783004040415257</v>
+        <v>-26.693494116920768</v>
       </c>
       <c r="P52" s="7">
         <f t="shared" ref="P52" ca="1" si="123">-$I$2*P51/(P50^2)</f>
@@ -5210,7 +5437,7 @@
       </c>
       <c r="Q52" s="7">
         <f t="shared" ref="Q52" ca="1" si="124">-$I$2*Q51/(Q50^2)</f>
-        <v>-1105.2631578947367</v>
+        <v>-12668.249999999996</v>
       </c>
       <c r="R52" s="7">
         <f t="shared" ref="R52" ca="1" si="125">-$I$2*R51/(R50^2)</f>
@@ -5226,7 +5453,7 @@
       </c>
       <c r="U52" s="7">
         <f t="shared" ref="U52" ca="1" si="128">-$I$2*U51/(U50^2)</f>
-        <v>-25.171293242802196</v>
+        <v>-22.300276511075925</v>
       </c>
       <c r="V52" s="7">
         <f t="shared" ref="V52" ca="1" si="129">-$I$2*V51/(V50^2)</f>
@@ -5234,7 +5461,7 @@
       </c>
       <c r="W52" s="7">
         <f t="shared" ref="W52" ca="1" si="130">-$I$2*W51/(W50^2)</f>
-        <v>-1105.2631578947367</v>
+        <v>-12668.249999999996</v>
       </c>
       <c r="X52" s="7">
         <f t="shared" ref="X52" ca="1" si="131">-$I$2*X51/(X50^2)</f>
@@ -5250,7 +5477,7 @@
       </c>
       <c r="AA52" s="7">
         <f t="shared" ref="AA52" ca="1" si="134">-$I$2*AA51/(AA50^2)</f>
-        <v>-25.829609247876594</v>
+        <v>-24.305085545001432</v>
       </c>
       <c r="AB52" s="7">
         <f t="shared" ref="AB52" ca="1" si="135">-$I$2*AB51/(AB50^2)</f>
@@ -5258,7 +5485,7 @@
       </c>
       <c r="AC52" s="7">
         <f t="shared" ref="AC52" ca="1" si="136">-$I$2*AC51/(AC50^2)</f>
-        <v>-1105.2631578947367</v>
+        <v>-12668.249999999996</v>
       </c>
       <c r="AD52" s="7">
         <f t="shared" ref="AD52" ca="1" si="137">-$I$2*AD51/(AD50^2)</f>
@@ -5274,7 +5501,7 @@
       </c>
       <c r="AG52" s="7">
         <f t="shared" ref="AG52" ca="1" si="140">-$I$2*AG51/(AG50^2)</f>
-        <v>-25.598974711249898</v>
+        <v>-21.08469867762695</v>
       </c>
       <c r="AH52" s="7">
         <f t="shared" ref="AH52" ca="1" si="141">-$I$2*AH51/(AH50^2)</f>
@@ -5282,7 +5509,7 @@
       </c>
       <c r="AI52" s="7">
         <f t="shared" ref="AI52" ca="1" si="142">-$I$2*AI51/(AI50^2)</f>
-        <v>-1105.2631578947367</v>
+        <v>-12668.249999999996</v>
       </c>
       <c r="AJ52" s="7">
         <f t="shared" ref="AJ52" ca="1" si="143">-$I$2*AJ51/(AJ50^2)</f>
@@ -5298,7 +5525,7 @@
       </c>
       <c r="AM52" s="7">
         <f t="shared" ref="AM52" ca="1" si="146">-$I$2*AM51/(AM50^2)</f>
-        <v>-20.210271269393107</v>
+        <v>-18.53373336524518</v>
       </c>
       <c r="AN52" s="7">
         <f t="shared" ref="AN52" ca="1" si="147">-$I$2*AN51/(AN50^2)</f>
@@ -5306,7 +5533,7 @@
       </c>
       <c r="AO52" s="7">
         <f t="shared" ref="AO52" ca="1" si="148">-$I$2*AO51/(AO50^2)</f>
-        <v>-1105.2631578947367</v>
+        <v>-12668.249999999996</v>
       </c>
       <c r="AP52" s="7">
         <f t="shared" ref="AP52" ca="1" si="149">-$I$2*AP51/(AP50^2)</f>
@@ -5322,7 +5549,7 @@
       </c>
       <c r="AS52" s="7">
         <f t="shared" ref="AS52" ca="1" si="152">-$I$2*AS51/(AS50^2)</f>
-        <v>-19.934980508296537</v>
+        <v>-26.75021108935896</v>
       </c>
       <c r="AT52" s="7">
         <f t="shared" ref="AT52" ca="1" si="153">-$I$2*AT51/(AT50^2)</f>
@@ -5330,7 +5557,7 @@
       </c>
       <c r="AU52" s="7">
         <f t="shared" ref="AU52" ca="1" si="154">-$I$2*AU51/(AU50^2)</f>
-        <v>-1105.2631578947367</v>
+        <v>-12668.249999999996</v>
       </c>
       <c r="AV52" s="7">
         <f t="shared" ref="AV52" ca="1" si="155">-$I$2*AV51/(AV50^2)</f>
@@ -5346,7 +5573,7 @@
       </c>
       <c r="AY52" s="7">
         <f t="shared" ref="AY52" ca="1" si="158">-$I$2*AY51/(AY50^2)</f>
-        <v>-23.107329155352367</v>
+        <v>-20.427020572620904</v>
       </c>
       <c r="AZ52" s="7">
         <f t="shared" ref="AZ52" ca="1" si="159">-$I$2*AZ51/(AZ50^2)</f>
@@ -5354,7 +5581,7 @@
       </c>
       <c r="BA52" s="7">
         <f t="shared" ref="BA52" ca="1" si="160">-$I$2*BA51/(BA50^2)</f>
-        <v>-1105.2631578947367</v>
+        <v>-12668.249999999996</v>
       </c>
       <c r="BB52" s="7">
         <f t="shared" ref="BB52" ca="1" si="161">-$I$2*BB51/(BB50^2)</f>
@@ -5370,7 +5597,7 @@
       </c>
       <c r="BE52" s="7">
         <f t="shared" ref="BE52" ca="1" si="164">-$I$2*BE51/(BE50^2)</f>
-        <v>-18.87559798237616</v>
+        <v>-23.99101232145248</v>
       </c>
       <c r="BF52" s="7">
         <f t="shared" ref="BF52" ca="1" si="165">-$I$2*BF51/(BF50^2)</f>
@@ -5378,7 +5605,7 @@
       </c>
       <c r="BG52" s="7">
         <f t="shared" ref="BG52" ca="1" si="166">-$I$2*BG51/(BG50^2)</f>
-        <v>-1105.2631578947367</v>
+        <v>-12668.249999999996</v>
       </c>
       <c r="BH52" s="7">
         <f t="shared" ref="BH52" ca="1" si="167">-$I$2*BH51/(BH50^2)</f>
@@ -5394,7 +5621,7 @@
       </c>
       <c r="BK52" s="7">
         <f t="shared" ref="BK52" ca="1" si="170">-$I$2*BK51/(BK50^2)</f>
-        <v>-21.879102748859633</v>
+        <v>-19.717911004498202</v>
       </c>
       <c r="BL52" s="7">
         <f t="shared" ref="BL52" ca="1" si="171">-$I$2*BL51/(BL50^2)</f>
@@ -5402,7 +5629,7 @@
       </c>
       <c r="BM52" s="7">
         <f t="shared" ref="BM52" ca="1" si="172">-$I$2*BM51/(BM50^2)</f>
-        <v>-1105.2631578947367</v>
+        <v>-12668.249999999996</v>
       </c>
       <c r="BN52" s="7">
         <f t="shared" ref="BN52" ca="1" si="173">-$I$2*BN51/(BN50^2)</f>
@@ -5418,7 +5645,7 @@
       </c>
       <c r="BQ52" s="7">
         <f t="shared" ref="BQ52" ca="1" si="176">-$I$2*BQ51/(BQ50^2)</f>
-        <v>-26.355639948896734</v>
+        <v>-26.189535287171168</v>
       </c>
       <c r="BR52" s="7">
         <f t="shared" ref="BR52" ca="1" si="177">-$I$2*BR51/(BR50^2)</f>
@@ -5426,7 +5653,7 @@
       </c>
       <c r="BS52" s="7">
         <f t="shared" ref="BS52" ca="1" si="178">-$I$2*BS51/(BS50^2)</f>
-        <v>-1105.2631578947367</v>
+        <v>-12668.249999999996</v>
       </c>
       <c r="BT52" s="7">
         <f t="shared" ref="BT52" ca="1" si="179">-$I$2*BT51/(BT50^2)</f>
@@ -5442,7 +5669,7 @@
       </c>
       <c r="BW52" s="7">
         <f t="shared" ref="BW52" ca="1" si="182">-$I$2*BW51/(BW50^2)</f>
-        <v>-23.938802789713073</v>
+        <v>-21.54619941796609</v>
       </c>
       <c r="BX52" s="7">
         <f t="shared" ref="BX52" ca="1" si="183">-$I$2*BX51/(BX50^2)</f>
@@ -5450,7 +5677,7 @@
       </c>
       <c r="BY52" s="7">
         <f t="shared" ref="BY52" ca="1" si="184">-$I$2*BY51/(BY50^2)</f>
-        <v>-1105.2631578947367</v>
+        <v>-12668.249999999996</v>
       </c>
       <c r="BZ52" s="7">
         <f t="shared" ref="BZ52" ca="1" si="185">-$I$2*BZ51/(BZ50^2)</f>
@@ -5466,7 +5693,7 @@
       </c>
       <c r="CC52" s="7">
         <f t="shared" ref="CC52" ca="1" si="188">-$I$2*CC51/(CC50^2)</f>
-        <v>-20.182185068724372</v>
+        <v>-24.220612529543523</v>
       </c>
       <c r="CD52" s="7">
         <f t="shared" ref="CD52" ca="1" si="189">-$I$2*CD51/(CD50^2)</f>
@@ -5474,7 +5701,7 @@
       </c>
       <c r="CE52" s="7">
         <f t="shared" ref="CE52" ca="1" si="190">-$I$2*CE51/(CE50^2)</f>
-        <v>-1105.2631578947367</v>
+        <v>-12668.249999999996</v>
       </c>
       <c r="CF52" s="7">
         <f t="shared" ref="CF52" ca="1" si="191">-$I$2*CF51/(CF50^2)</f>
@@ -5490,7 +5717,7 @@
       </c>
       <c r="CI52" s="7">
         <f t="shared" ref="CI52" ca="1" si="194">-$I$2*CI51/(CI50^2)</f>
-        <v>-18.909541870193848</v>
+        <v>-21.15003830462129</v>
       </c>
       <c r="CJ52" s="7">
         <f t="shared" ref="CJ52" ca="1" si="195">-$I$2*CJ51/(CJ50^2)</f>
@@ -5498,7 +5725,7 @@
       </c>
       <c r="CK52" s="7">
         <f t="shared" ref="CK52" ca="1" si="196">-$I$2*CK51/(CK50^2)</f>
-        <v>-1105.2631578947367</v>
+        <v>-12668.249999999996</v>
       </c>
       <c r="CL52" s="7">
         <f t="shared" ref="CL52" ca="1" si="197">-$I$2*CL51/(CL50^2)</f>
@@ -5514,7 +5741,7 @@
       </c>
       <c r="CO52" s="7">
         <f t="shared" ref="CO52" ca="1" si="200">-$I$2*CO51/(CO50^2)</f>
-        <v>-27.468895100562523</v>
+        <v>-25.144960757970832</v>
       </c>
       <c r="CP52" s="7">
         <f t="shared" ref="CP52" ca="1" si="201">-$I$2*CP51/(CP50^2)</f>
@@ -5522,7 +5749,7 @@
       </c>
       <c r="CQ52" s="7">
         <f t="shared" ref="CQ52" ca="1" si="202">-$I$2*CQ51/(CQ50^2)</f>
-        <v>-1105.2631578947367</v>
+        <v>-12668.249999999996</v>
       </c>
       <c r="CR52" s="7">
         <f t="shared" ref="CR52" ca="1" si="203">-$I$2*CR51/(CR50^2)</f>
@@ -5538,7 +5765,7 @@
       </c>
       <c r="CU52" s="7">
         <f t="shared" ref="CU52" ca="1" si="206">-$I$2*CU51/(CU50^2)</f>
-        <v>-25.254471527763798</v>
+        <v>-22.193961244571938</v>
       </c>
       <c r="CV52" s="7">
         <f t="shared" ref="CV52" ca="1" si="207">-$I$2*CV51/(CV50^2)</f>
@@ -5546,7 +5773,7 @@
       </c>
       <c r="CW52" s="7">
         <f t="shared" ref="CW52" ca="1" si="208">-$I$2*CW51/(CW50^2)</f>
-        <v>-1105.2631578947367</v>
+        <v>-12668.249999999996</v>
       </c>
       <c r="CX52" s="7">
         <f t="shared" ref="CX52" ca="1" si="209">-$I$2*CX51/(CX50^2)</f>
@@ -5562,7 +5789,7 @@
       </c>
       <c r="DA52" s="7">
         <f t="shared" ref="DA52" ca="1" si="212">-$I$2*DA51/(DA50^2)</f>
-        <v>-22.626587004960651</v>
+        <v>-18.475268002143633</v>
       </c>
       <c r="DB52" s="7">
         <f t="shared" ref="DB52" ca="1" si="213">-$I$2*DB51/(DB50^2)</f>
@@ -5570,7 +5797,7 @@
       </c>
       <c r="DC52" s="7">
         <f t="shared" ref="DC52" ca="1" si="214">-$I$2*DC51/(DC50^2)</f>
-        <v>-1105.2631578947367</v>
+        <v>-12668.249999999996</v>
       </c>
       <c r="DD52" s="7">
         <f t="shared" ref="DD52" ca="1" si="215">-$I$2*DD51/(DD50^2)</f>
@@ -5586,7 +5813,7 @@
       </c>
       <c r="DG52" s="7">
         <f t="shared" ref="DG52" ca="1" si="218">-$I$2*DG51/(DG50^2)</f>
-        <v>-20.390535858705309</v>
+        <v>-25.979295464242917</v>
       </c>
       <c r="DH52" s="7">
         <f t="shared" ref="DH52" ca="1" si="219">-$I$2*DH51/(DH50^2)</f>
@@ -5594,7 +5821,7 @@
       </c>
       <c r="DI52" s="7">
         <f t="shared" ref="DI52" ca="1" si="220">-$I$2*DI51/(DI50^2)</f>
-        <v>-1105.2631578947367</v>
+        <v>-12668.249999999996</v>
       </c>
       <c r="DJ52" s="7">
         <f t="shared" ref="DJ52" ca="1" si="221">-$I$2*DJ51/(DJ50^2)</f>
@@ -5610,7 +5837,7 @@
       </c>
       <c r="DM52" s="7">
         <f t="shared" ref="DM52" ca="1" si="224">-$I$2*DM51/(DM50^2)</f>
-        <v>-20.940028591964573</v>
+        <v>-25.68178300262484</v>
       </c>
       <c r="DN52" s="7">
         <f t="shared" ref="DN52" ca="1" si="225">-$I$2*DN51/(DN50^2)</f>
@@ -5618,7 +5845,7 @@
       </c>
       <c r="DO52" s="7">
         <f t="shared" ref="DO52" ca="1" si="226">-$I$2*DO51/(DO50^2)</f>
-        <v>-1105.2631578947367</v>
+        <v>-12668.249999999996</v>
       </c>
       <c r="DP52" s="7">
         <f t="shared" ref="DP52" ca="1" si="227">-$I$2*DP51/(DP50^2)</f>
@@ -7362,7 +7589,7 @@
     </row>
     <row r="61" spans="1:122">
       <c r="B61" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A61)-ROW($A$61)+1)</f>
+        <f t="shared" ref="B61:B92" si="230">INDEX($B$49:$DR$49,1,ROW(A61)-ROW($A$61)+1)</f>
         <v>V_SA</v>
       </c>
       <c r="C61" t="s">
@@ -7374,7 +7601,7 @@
     </row>
     <row r="62" spans="1:122">
       <c r="B62" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A62)-ROW($A$61)+1)</f>
+        <f t="shared" si="230"/>
         <v>V_AB1</v>
       </c>
       <c r="C62" t="s">
@@ -7386,7 +7613,7 @@
     </row>
     <row r="63" spans="1:122">
       <c r="B63" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A63)-ROW($A$61)+1)</f>
+        <f t="shared" si="230"/>
         <v>V_BC1</v>
       </c>
       <c r="C63" t="s">
@@ -7398,7 +7625,7 @@
     </row>
     <row r="64" spans="1:122">
       <c r="B64" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A64)-ROW($A$61)+1)</f>
+        <f t="shared" si="230"/>
         <v>V_CD1</v>
       </c>
       <c r="C64" t="s">
@@ -7420,7 +7647,7 @@
     </row>
     <row r="65" spans="2:8">
       <c r="B65" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A65)-ROW($A$61)+1)</f>
+        <f t="shared" si="230"/>
         <v>V_DE1</v>
       </c>
       <c r="C65" t="s">
@@ -7432,7 +7659,7 @@
     </row>
     <row r="66" spans="2:8">
       <c r="B66" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A66)-ROW($A$61)+1)</f>
+        <f t="shared" si="230"/>
         <v>V_EF1</v>
       </c>
       <c r="C66" t="s">
@@ -7444,19 +7671,19 @@
     </row>
     <row r="67" spans="2:8">
       <c r="B67" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A67)-ROW($A$61)+1)</f>
+        <f t="shared" si="230"/>
         <v>V_FG1</v>
       </c>
       <c r="C67" t="s">
         <v>620</v>
       </c>
       <c r="D67">
-        <v>-0.1</v>
+        <v>-0.62</v>
       </c>
     </row>
     <row r="68" spans="2:8">
       <c r="B68" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A68)-ROW($A$61)+1)</f>
+        <f t="shared" si="230"/>
         <v>V_AB2</v>
       </c>
       <c r="C68" t="s">
@@ -7468,7 +7695,7 @@
     </row>
     <row r="69" spans="2:8">
       <c r="B69" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A69)-ROW($A$61)+1)</f>
+        <f t="shared" si="230"/>
         <v>V_BC2</v>
       </c>
       <c r="C69" t="s">
@@ -7480,7 +7707,7 @@
     </row>
     <row r="70" spans="2:8">
       <c r="B70" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A70)-ROW($A$61)+1)</f>
+        <f t="shared" si="230"/>
         <v>V_CD2</v>
       </c>
       <c r="C70" t="s">
@@ -7490,7 +7717,7 @@
         <v>0</v>
       </c>
       <c r="F70">
-        <f t="shared" ref="F70" ca="1" si="230">((1+RAND()*$I$43*(RANDBETWEEN(0,1)*2-1))*$J$43+($J$43=0))*($I$41*(H70=0)+G70*H70)</f>
+        <f t="shared" ref="F70" ca="1" si="231">((1+RAND()*$I$43*(RANDBETWEEN(0,1)*2-1))*$J$43+($J$43=0))*($I$41*(H70=0)+G70*H70)</f>
         <v>0</v>
       </c>
       <c r="G70" s="7">
@@ -7502,7 +7729,7 @@
     </row>
     <row r="71" spans="2:8">
       <c r="B71" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A71)-ROW($A$61)+1)</f>
+        <f t="shared" si="230"/>
         <v>V_DE2</v>
       </c>
       <c r="C71" t="s">
@@ -7514,7 +7741,7 @@
     </row>
     <row r="72" spans="2:8">
       <c r="B72" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A72)-ROW($A$61)+1)</f>
+        <f t="shared" si="230"/>
         <v>V_EF2</v>
       </c>
       <c r="C72" t="s">
@@ -7526,19 +7753,19 @@
     </row>
     <row r="73" spans="2:8">
       <c r="B73" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A73)-ROW($A$61)+1)</f>
+        <f t="shared" si="230"/>
         <v>V_FG2</v>
       </c>
       <c r="C73" t="s">
         <v>621</v>
       </c>
       <c r="D73">
-        <v>0</v>
+        <v>-0.7</v>
       </c>
     </row>
     <row r="74" spans="2:8">
       <c r="B74" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A74)-ROW($A$61)+1)</f>
+        <f t="shared" si="230"/>
         <v>V_AB3</v>
       </c>
       <c r="C74" t="s">
@@ -7550,7 +7777,7 @@
     </row>
     <row r="75" spans="2:8">
       <c r="B75" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A75)-ROW($A$61)+1)</f>
+        <f t="shared" si="230"/>
         <v>V_BC3</v>
       </c>
       <c r="C75" t="s">
@@ -7562,7 +7789,7 @@
     </row>
     <row r="76" spans="2:8">
       <c r="B76" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A76)-ROW($A$61)+1)</f>
+        <f t="shared" si="230"/>
         <v>V_CD3</v>
       </c>
       <c r="C76" t="s">
@@ -7572,7 +7799,7 @@
         <v>0</v>
       </c>
       <c r="F76">
-        <f t="shared" ref="F76" ca="1" si="231">((1+RAND()*$I$43*(RANDBETWEEN(0,1)*2-1))*$J$43+($J$43=0))*($I$41*(H76=0)+G76*H76)</f>
+        <f t="shared" ref="F76" ca="1" si="232">((1+RAND()*$I$43*(RANDBETWEEN(0,1)*2-1))*$J$43+($J$43=0))*($I$41*(H76=0)+G76*H76)</f>
         <v>0</v>
       </c>
       <c r="G76" s="7">
@@ -7584,7 +7811,7 @@
     </row>
     <row r="77" spans="2:8">
       <c r="B77" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A77)-ROW($A$61)+1)</f>
+        <f t="shared" si="230"/>
         <v>V_DE3</v>
       </c>
       <c r="C77" t="s">
@@ -7596,7 +7823,7 @@
     </row>
     <row r="78" spans="2:8">
       <c r="B78" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A78)-ROW($A$61)+1)</f>
+        <f t="shared" si="230"/>
         <v>V_EF3</v>
       </c>
       <c r="C78" t="s">
@@ -7608,19 +7835,19 @@
     </row>
     <row r="79" spans="2:8">
       <c r="B79" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A79)-ROW($A$61)+1)</f>
+        <f t="shared" si="230"/>
         <v>V_FG3</v>
       </c>
       <c r="C79" t="s">
         <v>622</v>
       </c>
       <c r="D79">
-        <v>0</v>
+        <v>-0.7</v>
       </c>
     </row>
     <row r="80" spans="2:8">
       <c r="B80" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A80)-ROW($A$61)+1)</f>
+        <f t="shared" si="230"/>
         <v>V_AB4</v>
       </c>
       <c r="C80" t="s">
@@ -7632,7 +7859,7 @@
     </row>
     <row r="81" spans="2:8">
       <c r="B81" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A81)-ROW($A$61)+1)</f>
+        <f t="shared" si="230"/>
         <v>V_BC4</v>
       </c>
       <c r="C81" t="s">
@@ -7644,7 +7871,7 @@
     </row>
     <row r="82" spans="2:8">
       <c r="B82" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A82)-ROW($A$61)+1)</f>
+        <f t="shared" si="230"/>
         <v>V_CD4</v>
       </c>
       <c r="C82" t="s">
@@ -7654,7 +7881,7 @@
         <v>0</v>
       </c>
       <c r="F82">
-        <f t="shared" ref="F82" ca="1" si="232">((1+RAND()*$I$43*(RANDBETWEEN(0,1)*2-1))*$J$43+($J$43=0))*($I$41*(H82=0)+G82*H82)</f>
+        <f t="shared" ref="F82" ca="1" si="233">((1+RAND()*$I$43*(RANDBETWEEN(0,1)*2-1))*$J$43+($J$43=0))*($I$41*(H82=0)+G82*H82)</f>
         <v>0</v>
       </c>
       <c r="G82" s="7">
@@ -7666,7 +7893,7 @@
     </row>
     <row r="83" spans="2:8">
       <c r="B83" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A83)-ROW($A$61)+1)</f>
+        <f t="shared" si="230"/>
         <v>V_DE4</v>
       </c>
       <c r="C83" t="s">
@@ -7678,7 +7905,7 @@
     </row>
     <row r="84" spans="2:8">
       <c r="B84" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A84)-ROW($A$61)+1)</f>
+        <f t="shared" si="230"/>
         <v>V_EF4</v>
       </c>
       <c r="C84" t="s">
@@ -7690,19 +7917,19 @@
     </row>
     <row r="85" spans="2:8">
       <c r="B85" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A85)-ROW($A$61)+1)</f>
+        <f t="shared" si="230"/>
         <v>V_FG4</v>
       </c>
       <c r="C85" t="s">
         <v>623</v>
       </c>
       <c r="D85">
-        <v>0</v>
+        <v>-0.7</v>
       </c>
     </row>
     <row r="86" spans="2:8">
       <c r="B86" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A86)-ROW($A$61)+1)</f>
+        <f t="shared" si="230"/>
         <v>V_AB5</v>
       </c>
       <c r="C86" t="s">
@@ -7714,7 +7941,7 @@
     </row>
     <row r="87" spans="2:8">
       <c r="B87" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A87)-ROW($A$61)+1)</f>
+        <f t="shared" si="230"/>
         <v>V_BC5</v>
       </c>
       <c r="C87" t="s">
@@ -7726,7 +7953,7 @@
     </row>
     <row r="88" spans="2:8">
       <c r="B88" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A88)-ROW($A$61)+1)</f>
+        <f t="shared" si="230"/>
         <v>V_CD5</v>
       </c>
       <c r="C88" t="s">
@@ -7736,7 +7963,7 @@
         <v>0</v>
       </c>
       <c r="F88">
-        <f t="shared" ref="F88" ca="1" si="233">((1+RAND()*$I$43*(RANDBETWEEN(0,1)*2-1))*$J$43+($J$43=0))*($I$41*(H88=0)+G88*H88)</f>
+        <f t="shared" ref="F88" ca="1" si="234">((1+RAND()*$I$43*(RANDBETWEEN(0,1)*2-1))*$J$43+($J$43=0))*($I$41*(H88=0)+G88*H88)</f>
         <v>0</v>
       </c>
       <c r="G88" s="7">
@@ -7748,7 +7975,7 @@
     </row>
     <row r="89" spans="2:8">
       <c r="B89" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A89)-ROW($A$61)+1)</f>
+        <f t="shared" si="230"/>
         <v>V_DE5</v>
       </c>
       <c r="C89" t="s">
@@ -7760,7 +7987,7 @@
     </row>
     <row r="90" spans="2:8">
       <c r="B90" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A90)-ROW($A$61)+1)</f>
+        <f t="shared" si="230"/>
         <v>V_EF5</v>
       </c>
       <c r="C90" t="s">
@@ -7772,19 +7999,19 @@
     </row>
     <row r="91" spans="2:8">
       <c r="B91" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A91)-ROW($A$61)+1)</f>
+        <f t="shared" si="230"/>
         <v>V_FG5</v>
       </c>
       <c r="C91" t="s">
         <v>624</v>
       </c>
       <c r="D91">
-        <v>0</v>
+        <v>-0.7</v>
       </c>
     </row>
     <row r="92" spans="2:8">
       <c r="B92" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A92)-ROW($A$61)+1)</f>
+        <f t="shared" si="230"/>
         <v>V_AB6</v>
       </c>
       <c r="C92" t="s">
@@ -7796,7 +8023,7 @@
     </row>
     <row r="93" spans="2:8">
       <c r="B93" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A93)-ROW($A$61)+1)</f>
+        <f t="shared" ref="B93:B124" si="235">INDEX($B$49:$DR$49,1,ROW(A93)-ROW($A$61)+1)</f>
         <v>V_BC6</v>
       </c>
       <c r="C93" t="s">
@@ -7808,7 +8035,7 @@
     </row>
     <row r="94" spans="2:8">
       <c r="B94" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A94)-ROW($A$61)+1)</f>
+        <f t="shared" si="235"/>
         <v>V_CD6</v>
       </c>
       <c r="C94" t="s">
@@ -7818,7 +8045,7 @@
         <v>0</v>
       </c>
       <c r="F94">
-        <f t="shared" ref="F94" ca="1" si="234">((1+RAND()*$I$43*(RANDBETWEEN(0,1)*2-1))*$J$43+($J$43=0))*($I$41*(H94=0)+G94*H94)</f>
+        <f t="shared" ref="F94" ca="1" si="236">((1+RAND()*$I$43*(RANDBETWEEN(0,1)*2-1))*$J$43+($J$43=0))*($I$41*(H94=0)+G94*H94)</f>
         <v>0</v>
       </c>
       <c r="G94" s="7">
@@ -7830,7 +8057,7 @@
     </row>
     <row r="95" spans="2:8">
       <c r="B95" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A95)-ROW($A$61)+1)</f>
+        <f t="shared" si="235"/>
         <v>V_DE6</v>
       </c>
       <c r="C95" t="s">
@@ -7842,7 +8069,7 @@
     </row>
     <row r="96" spans="2:8">
       <c r="B96" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A96)-ROW($A$61)+1)</f>
+        <f t="shared" si="235"/>
         <v>V_EF6</v>
       </c>
       <c r="C96" t="s">
@@ -7854,19 +8081,19 @@
     </row>
     <row r="97" spans="2:8">
       <c r="B97" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A97)-ROW($A$61)+1)</f>
+        <f t="shared" si="235"/>
         <v>V_FG6</v>
       </c>
       <c r="C97" t="s">
         <v>625</v>
       </c>
       <c r="D97">
-        <v>0</v>
+        <v>-0.7</v>
       </c>
     </row>
     <row r="98" spans="2:8">
       <c r="B98" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A98)-ROW($A$61)+1)</f>
+        <f t="shared" si="235"/>
         <v>V_AB7</v>
       </c>
       <c r="C98" t="s">
@@ -7878,7 +8105,7 @@
     </row>
     <row r="99" spans="2:8">
       <c r="B99" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A99)-ROW($A$61)+1)</f>
+        <f t="shared" si="235"/>
         <v>V_BC7</v>
       </c>
       <c r="C99" t="s">
@@ -7890,7 +8117,7 @@
     </row>
     <row r="100" spans="2:8">
       <c r="B100" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A100)-ROW($A$61)+1)</f>
+        <f t="shared" si="235"/>
         <v>V_CD7</v>
       </c>
       <c r="C100" t="s">
@@ -7900,7 +8127,7 @@
         <v>0</v>
       </c>
       <c r="F100">
-        <f t="shared" ref="F100" ca="1" si="235">((1+RAND()*$I$43*(RANDBETWEEN(0,1)*2-1))*$J$43+($J$43=0))*($I$41*(H100=0)+G100*H100)</f>
+        <f t="shared" ref="F100" ca="1" si="237">((1+RAND()*$I$43*(RANDBETWEEN(0,1)*2-1))*$J$43+($J$43=0))*($I$41*(H100=0)+G100*H100)</f>
         <v>0</v>
       </c>
       <c r="G100" s="7">
@@ -7912,7 +8139,7 @@
     </row>
     <row r="101" spans="2:8">
       <c r="B101" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A101)-ROW($A$61)+1)</f>
+        <f t="shared" si="235"/>
         <v>V_DE7</v>
       </c>
       <c r="C101" t="s">
@@ -7924,7 +8151,7 @@
     </row>
     <row r="102" spans="2:8">
       <c r="B102" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A102)-ROW($A$61)+1)</f>
+        <f t="shared" si="235"/>
         <v>V_EF7</v>
       </c>
       <c r="C102" t="s">
@@ -7936,19 +8163,19 @@
     </row>
     <row r="103" spans="2:8">
       <c r="B103" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A103)-ROW($A$61)+1)</f>
+        <f t="shared" si="235"/>
         <v>V_FG7</v>
       </c>
       <c r="C103" t="s">
         <v>626</v>
       </c>
       <c r="D103">
-        <v>0</v>
+        <v>-0.7</v>
       </c>
     </row>
     <row r="104" spans="2:8">
       <c r="B104" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A104)-ROW($A$61)+1)</f>
+        <f t="shared" si="235"/>
         <v>V_AB8</v>
       </c>
       <c r="C104" t="s">
@@ -7960,7 +8187,7 @@
     </row>
     <row r="105" spans="2:8">
       <c r="B105" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A105)-ROW($A$61)+1)</f>
+        <f t="shared" si="235"/>
         <v>V_BC8</v>
       </c>
       <c r="C105" t="s">
@@ -7972,7 +8199,7 @@
     </row>
     <row r="106" spans="2:8">
       <c r="B106" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A106)-ROW($A$61)+1)</f>
+        <f t="shared" si="235"/>
         <v>V_CD8</v>
       </c>
       <c r="C106" t="s">
@@ -7982,7 +8209,7 @@
         <v>0</v>
       </c>
       <c r="F106">
-        <f t="shared" ref="F106" ca="1" si="236">((1+RAND()*$I$43*(RANDBETWEEN(0,1)*2-1))*$J$43+($J$43=0))*($I$41*(H106=0)+G106*H106)</f>
+        <f t="shared" ref="F106" ca="1" si="238">((1+RAND()*$I$43*(RANDBETWEEN(0,1)*2-1))*$J$43+($J$43=0))*($I$41*(H106=0)+G106*H106)</f>
         <v>0</v>
       </c>
       <c r="G106" s="7">
@@ -7994,7 +8221,7 @@
     </row>
     <row r="107" spans="2:8">
       <c r="B107" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A107)-ROW($A$61)+1)</f>
+        <f t="shared" si="235"/>
         <v>V_DE8</v>
       </c>
       <c r="C107" t="s">
@@ -8006,7 +8233,7 @@
     </row>
     <row r="108" spans="2:8">
       <c r="B108" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A108)-ROW($A$61)+1)</f>
+        <f t="shared" si="235"/>
         <v>V_EF8</v>
       </c>
       <c r="C108" t="s">
@@ -8018,19 +8245,19 @@
     </row>
     <row r="109" spans="2:8">
       <c r="B109" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A109)-ROW($A$61)+1)</f>
+        <f t="shared" si="235"/>
         <v>V_FG8</v>
       </c>
       <c r="C109" t="s">
         <v>627</v>
       </c>
       <c r="D109">
-        <v>0</v>
+        <v>-0.7</v>
       </c>
     </row>
     <row r="110" spans="2:8">
       <c r="B110" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A110)-ROW($A$61)+1)</f>
+        <f t="shared" si="235"/>
         <v>V_AB9</v>
       </c>
       <c r="C110" t="s">
@@ -8042,7 +8269,7 @@
     </row>
     <row r="111" spans="2:8">
       <c r="B111" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A111)-ROW($A$61)+1)</f>
+        <f t="shared" si="235"/>
         <v>V_BC9</v>
       </c>
       <c r="C111" t="s">
@@ -8054,7 +8281,7 @@
     </row>
     <row r="112" spans="2:8">
       <c r="B112" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A112)-ROW($A$61)+1)</f>
+        <f t="shared" si="235"/>
         <v>V_CD9</v>
       </c>
       <c r="C112" t="s">
@@ -8064,7 +8291,7 @@
         <v>0</v>
       </c>
       <c r="F112">
-        <f t="shared" ref="F112" ca="1" si="237">((1+RAND()*$I$43*(RANDBETWEEN(0,1)*2-1))*$J$43+($J$43=0))*($I$41*(H112=0)+G112*H112)</f>
+        <f t="shared" ref="F112" ca="1" si="239">((1+RAND()*$I$43*(RANDBETWEEN(0,1)*2-1))*$J$43+($J$43=0))*($I$41*(H112=0)+G112*H112)</f>
         <v>0</v>
       </c>
       <c r="G112" s="7">
@@ -8076,7 +8303,7 @@
     </row>
     <row r="113" spans="2:8">
       <c r="B113" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A113)-ROW($A$61)+1)</f>
+        <f t="shared" si="235"/>
         <v>V_DE9</v>
       </c>
       <c r="C113" t="s">
@@ -8088,7 +8315,7 @@
     </row>
     <row r="114" spans="2:8">
       <c r="B114" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A114)-ROW($A$61)+1)</f>
+        <f t="shared" si="235"/>
         <v>V_EF9</v>
       </c>
       <c r="C114" t="s">
@@ -8100,19 +8327,19 @@
     </row>
     <row r="115" spans="2:8">
       <c r="B115" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A115)-ROW($A$61)+1)</f>
+        <f t="shared" si="235"/>
         <v>V_FG9</v>
       </c>
       <c r="C115" t="s">
         <v>628</v>
       </c>
       <c r="D115">
-        <v>0</v>
+        <v>-0.7</v>
       </c>
     </row>
     <row r="116" spans="2:8">
       <c r="B116" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A116)-ROW($A$61)+1)</f>
+        <f t="shared" si="235"/>
         <v>V_AB10</v>
       </c>
       <c r="C116" t="s">
@@ -8124,7 +8351,7 @@
     </row>
     <row r="117" spans="2:8">
       <c r="B117" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A117)-ROW($A$61)+1)</f>
+        <f t="shared" si="235"/>
         <v>V_BC10</v>
       </c>
       <c r="C117" t="s">
@@ -8136,7 +8363,7 @@
     </row>
     <row r="118" spans="2:8">
       <c r="B118" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A118)-ROW($A$61)+1)</f>
+        <f t="shared" si="235"/>
         <v>V_CD10</v>
       </c>
       <c r="C118" t="s">
@@ -8146,7 +8373,7 @@
         <v>0</v>
       </c>
       <c r="F118">
-        <f t="shared" ref="F118" ca="1" si="238">((1+RAND()*$I$43*(RANDBETWEEN(0,1)*2-1))*$J$43+($J$43=0))*($I$41*(H118=0)+G118*H118)</f>
+        <f t="shared" ref="F118" ca="1" si="240">((1+RAND()*$I$43*(RANDBETWEEN(0,1)*2-1))*$J$43+($J$43=0))*($I$41*(H118=0)+G118*H118)</f>
         <v>0</v>
       </c>
       <c r="G118" s="7">
@@ -8158,7 +8385,7 @@
     </row>
     <row r="119" spans="2:8">
       <c r="B119" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A119)-ROW($A$61)+1)</f>
+        <f t="shared" si="235"/>
         <v>V_DE10</v>
       </c>
       <c r="C119" t="s">
@@ -8170,7 +8397,7 @@
     </row>
     <row r="120" spans="2:8">
       <c r="B120" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A120)-ROW($A$61)+1)</f>
+        <f t="shared" si="235"/>
         <v>V_EF10</v>
       </c>
       <c r="C120" t="s">
@@ -8182,19 +8409,19 @@
     </row>
     <row r="121" spans="2:8">
       <c r="B121" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A121)-ROW($A$61)+1)</f>
+        <f t="shared" si="235"/>
         <v>V_FG10</v>
       </c>
       <c r="C121" t="s">
         <v>629</v>
       </c>
       <c r="D121">
-        <v>0</v>
+        <v>-0.7</v>
       </c>
     </row>
     <row r="122" spans="2:8">
       <c r="B122" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A122)-ROW($A$61)+1)</f>
+        <f t="shared" si="235"/>
         <v>V_AB11</v>
       </c>
       <c r="C122" t="s">
@@ -8206,7 +8433,7 @@
     </row>
     <row r="123" spans="2:8">
       <c r="B123" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A123)-ROW($A$61)+1)</f>
+        <f t="shared" si="235"/>
         <v>V_BC11</v>
       </c>
       <c r="C123" t="s">
@@ -8218,7 +8445,7 @@
     </row>
     <row r="124" spans="2:8">
       <c r="B124" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A124)-ROW($A$61)+1)</f>
+        <f t="shared" si="235"/>
         <v>V_CD11</v>
       </c>
       <c r="C124" t="s">
@@ -8228,7 +8455,7 @@
         <v>0</v>
       </c>
       <c r="F124">
-        <f t="shared" ref="F124" ca="1" si="239">((1+RAND()*$I$43*(RANDBETWEEN(0,1)*2-1))*$J$43+($J$43=0))*($I$41*(H124=0)+G124*H124)</f>
+        <f t="shared" ref="F124" ca="1" si="241">((1+RAND()*$I$43*(RANDBETWEEN(0,1)*2-1))*$J$43+($J$43=0))*($I$41*(H124=0)+G124*H124)</f>
         <v>0</v>
       </c>
       <c r="G124" s="7">
@@ -8240,7 +8467,7 @@
     </row>
     <row r="125" spans="2:8">
       <c r="B125" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A125)-ROW($A$61)+1)</f>
+        <f t="shared" ref="B125:B156" si="242">INDEX($B$49:$DR$49,1,ROW(A125)-ROW($A$61)+1)</f>
         <v>V_DE11</v>
       </c>
       <c r="C125" t="s">
@@ -8252,7 +8479,7 @@
     </row>
     <row r="126" spans="2:8">
       <c r="B126" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A126)-ROW($A$61)+1)</f>
+        <f t="shared" si="242"/>
         <v>V_EF11</v>
       </c>
       <c r="C126" t="s">
@@ -8264,19 +8491,19 @@
     </row>
     <row r="127" spans="2:8">
       <c r="B127" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A127)-ROW($A$61)+1)</f>
+        <f t="shared" si="242"/>
         <v>V_FG11</v>
       </c>
       <c r="C127" t="s">
         <v>630</v>
       </c>
       <c r="D127">
-        <v>0</v>
+        <v>-0.7</v>
       </c>
     </row>
     <row r="128" spans="2:8">
       <c r="B128" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A128)-ROW($A$61)+1)</f>
+        <f t="shared" si="242"/>
         <v>V_AB12</v>
       </c>
       <c r="C128" t="s">
@@ -8288,7 +8515,7 @@
     </row>
     <row r="129" spans="2:8">
       <c r="B129" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A129)-ROW($A$61)+1)</f>
+        <f t="shared" si="242"/>
         <v>V_BC12</v>
       </c>
       <c r="C129" t="s">
@@ -8300,7 +8527,7 @@
     </row>
     <row r="130" spans="2:8">
       <c r="B130" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A130)-ROW($A$61)+1)</f>
+        <f t="shared" si="242"/>
         <v>V_CD12</v>
       </c>
       <c r="C130" t="s">
@@ -8310,7 +8537,7 @@
         <v>0</v>
       </c>
       <c r="F130">
-        <f t="shared" ref="F130" ca="1" si="240">((1+RAND()*$I$43*(RANDBETWEEN(0,1)*2-1))*$J$43+($J$43=0))*($I$41*(H130=0)+G130*H130)</f>
+        <f t="shared" ref="F130" ca="1" si="243">((1+RAND()*$I$43*(RANDBETWEEN(0,1)*2-1))*$J$43+($J$43=0))*($I$41*(H130=0)+G130*H130)</f>
         <v>0</v>
       </c>
       <c r="G130" s="7">
@@ -8322,7 +8549,7 @@
     </row>
     <row r="131" spans="2:8">
       <c r="B131" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A131)-ROW($A$61)+1)</f>
+        <f t="shared" si="242"/>
         <v>V_DE12</v>
       </c>
       <c r="C131" t="s">
@@ -8334,7 +8561,7 @@
     </row>
     <row r="132" spans="2:8">
       <c r="B132" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A132)-ROW($A$61)+1)</f>
+        <f t="shared" si="242"/>
         <v>V_EF12</v>
       </c>
       <c r="C132" t="s">
@@ -8346,19 +8573,19 @@
     </row>
     <row r="133" spans="2:8">
       <c r="B133" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A133)-ROW($A$61)+1)</f>
+        <f t="shared" si="242"/>
         <v>V_FG12</v>
       </c>
       <c r="C133" t="s">
         <v>631</v>
       </c>
       <c r="D133">
-        <v>0</v>
+        <v>-0.7</v>
       </c>
     </row>
     <row r="134" spans="2:8">
       <c r="B134" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A134)-ROW($A$61)+1)</f>
+        <f t="shared" si="242"/>
         <v>V_AB13</v>
       </c>
       <c r="C134" t="s">
@@ -8370,7 +8597,7 @@
     </row>
     <row r="135" spans="2:8">
       <c r="B135" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A135)-ROW($A$61)+1)</f>
+        <f t="shared" si="242"/>
         <v>V_BC13</v>
       </c>
       <c r="C135" t="s">
@@ -8382,7 +8609,7 @@
     </row>
     <row r="136" spans="2:8">
       <c r="B136" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A136)-ROW($A$61)+1)</f>
+        <f t="shared" si="242"/>
         <v>V_CD13</v>
       </c>
       <c r="C136" t="s">
@@ -8392,7 +8619,7 @@
         <v>0</v>
       </c>
       <c r="F136">
-        <f t="shared" ref="F136" ca="1" si="241">((1+RAND()*$I$43*(RANDBETWEEN(0,1)*2-1))*$J$43+($J$43=0))*($I$41*(H136=0)+G136*H136)</f>
+        <f t="shared" ref="F136" ca="1" si="244">((1+RAND()*$I$43*(RANDBETWEEN(0,1)*2-1))*$J$43+($J$43=0))*($I$41*(H136=0)+G136*H136)</f>
         <v>0</v>
       </c>
       <c r="G136" s="7">
@@ -8404,7 +8631,7 @@
     </row>
     <row r="137" spans="2:8">
       <c r="B137" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A137)-ROW($A$61)+1)</f>
+        <f t="shared" si="242"/>
         <v>V_DE13</v>
       </c>
       <c r="C137" t="s">
@@ -8416,7 +8643,7 @@
     </row>
     <row r="138" spans="2:8">
       <c r="B138" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A138)-ROW($A$61)+1)</f>
+        <f t="shared" si="242"/>
         <v>V_EF13</v>
       </c>
       <c r="C138" t="s">
@@ -8428,19 +8655,19 @@
     </row>
     <row r="139" spans="2:8">
       <c r="B139" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A139)-ROW($A$61)+1)</f>
+        <f t="shared" si="242"/>
         <v>V_FG13</v>
       </c>
       <c r="C139" t="s">
         <v>632</v>
       </c>
       <c r="D139">
-        <v>0</v>
+        <v>-0.7</v>
       </c>
     </row>
     <row r="140" spans="2:8">
       <c r="B140" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A140)-ROW($A$61)+1)</f>
+        <f t="shared" si="242"/>
         <v>V_AB14</v>
       </c>
       <c r="C140" t="s">
@@ -8452,7 +8679,7 @@
     </row>
     <row r="141" spans="2:8">
       <c r="B141" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A141)-ROW($A$61)+1)</f>
+        <f t="shared" si="242"/>
         <v>V_BC14</v>
       </c>
       <c r="C141" t="s">
@@ -8464,7 +8691,7 @@
     </row>
     <row r="142" spans="2:8">
       <c r="B142" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A142)-ROW($A$61)+1)</f>
+        <f t="shared" si="242"/>
         <v>V_CD14</v>
       </c>
       <c r="C142" t="s">
@@ -8474,7 +8701,7 @@
         <v>0</v>
       </c>
       <c r="F142">
-        <f t="shared" ref="F142" ca="1" si="242">((1+RAND()*$I$43*(RANDBETWEEN(0,1)*2-1))*$J$43+($J$43=0))*($I$41*(H142=0)+G142*H142)</f>
+        <f t="shared" ref="F142" ca="1" si="245">((1+RAND()*$I$43*(RANDBETWEEN(0,1)*2-1))*$J$43+($J$43=0))*($I$41*(H142=0)+G142*H142)</f>
         <v>0</v>
       </c>
       <c r="G142" s="7">
@@ -8486,7 +8713,7 @@
     </row>
     <row r="143" spans="2:8">
       <c r="B143" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A143)-ROW($A$61)+1)</f>
+        <f t="shared" si="242"/>
         <v>V_DE14</v>
       </c>
       <c r="C143" t="s">
@@ -8498,7 +8725,7 @@
     </row>
     <row r="144" spans="2:8">
       <c r="B144" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A144)-ROW($A$61)+1)</f>
+        <f t="shared" si="242"/>
         <v>V_EF14</v>
       </c>
       <c r="C144" t="s">
@@ -8510,19 +8737,19 @@
     </row>
     <row r="145" spans="2:8">
       <c r="B145" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A145)-ROW($A$61)+1)</f>
+        <f t="shared" si="242"/>
         <v>V_FG14</v>
       </c>
       <c r="C145" t="s">
         <v>633</v>
       </c>
       <c r="D145">
-        <v>0</v>
+        <v>-0.7</v>
       </c>
     </row>
     <row r="146" spans="2:8">
       <c r="B146" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A146)-ROW($A$61)+1)</f>
+        <f t="shared" si="242"/>
         <v>V_AB15</v>
       </c>
       <c r="C146" t="s">
@@ -8534,7 +8761,7 @@
     </row>
     <row r="147" spans="2:8">
       <c r="B147" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A147)-ROW($A$61)+1)</f>
+        <f t="shared" si="242"/>
         <v>V_BC15</v>
       </c>
       <c r="C147" t="s">
@@ -8546,7 +8773,7 @@
     </row>
     <row r="148" spans="2:8">
       <c r="B148" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A148)-ROW($A$61)+1)</f>
+        <f t="shared" si="242"/>
         <v>V_CD15</v>
       </c>
       <c r="C148" t="s">
@@ -8556,7 +8783,7 @@
         <v>0</v>
       </c>
       <c r="F148">
-        <f t="shared" ref="F148" ca="1" si="243">((1+RAND()*$I$43*(RANDBETWEEN(0,1)*2-1))*$J$43+($J$43=0))*($I$41*(H148=0)+G148*H148)</f>
+        <f t="shared" ref="F148" ca="1" si="246">((1+RAND()*$I$43*(RANDBETWEEN(0,1)*2-1))*$J$43+($J$43=0))*($I$41*(H148=0)+G148*H148)</f>
         <v>0</v>
       </c>
       <c r="G148" s="7">
@@ -8568,7 +8795,7 @@
     </row>
     <row r="149" spans="2:8">
       <c r="B149" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A149)-ROW($A$61)+1)</f>
+        <f t="shared" si="242"/>
         <v>V_DE15</v>
       </c>
       <c r="C149" t="s">
@@ -8580,7 +8807,7 @@
     </row>
     <row r="150" spans="2:8">
       <c r="B150" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A150)-ROW($A$61)+1)</f>
+        <f t="shared" si="242"/>
         <v>V_EF15</v>
       </c>
       <c r="C150" t="s">
@@ -8592,19 +8819,19 @@
     </row>
     <row r="151" spans="2:8">
       <c r="B151" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A151)-ROW($A$61)+1)</f>
+        <f t="shared" si="242"/>
         <v>V_FG15</v>
       </c>
       <c r="C151" t="s">
         <v>634</v>
       </c>
       <c r="D151">
-        <v>0</v>
+        <v>-0.7</v>
       </c>
     </row>
     <row r="152" spans="2:8">
       <c r="B152" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A152)-ROW($A$61)+1)</f>
+        <f t="shared" si="242"/>
         <v>V_AB16</v>
       </c>
       <c r="C152" t="s">
@@ -8616,7 +8843,7 @@
     </row>
     <row r="153" spans="2:8">
       <c r="B153" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A153)-ROW($A$61)+1)</f>
+        <f t="shared" si="242"/>
         <v>V_BC16</v>
       </c>
       <c r="C153" t="s">
@@ -8628,7 +8855,7 @@
     </row>
     <row r="154" spans="2:8">
       <c r="B154" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A154)-ROW($A$61)+1)</f>
+        <f t="shared" si="242"/>
         <v>V_CD16</v>
       </c>
       <c r="C154" t="s">
@@ -8638,7 +8865,7 @@
         <v>0</v>
       </c>
       <c r="F154">
-        <f t="shared" ref="F154" ca="1" si="244">((1+RAND()*$I$43*(RANDBETWEEN(0,1)*2-1))*$J$43+($J$43=0))*($I$41*(H154=0)+G154*H154)</f>
+        <f t="shared" ref="F154" ca="1" si="247">((1+RAND()*$I$43*(RANDBETWEEN(0,1)*2-1))*$J$43+($J$43=0))*($I$41*(H154=0)+G154*H154)</f>
         <v>0</v>
       </c>
       <c r="G154" s="7">
@@ -8650,7 +8877,7 @@
     </row>
     <row r="155" spans="2:8">
       <c r="B155" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A155)-ROW($A$61)+1)</f>
+        <f t="shared" si="242"/>
         <v>V_DE16</v>
       </c>
       <c r="C155" t="s">
@@ -8662,7 +8889,7 @@
     </row>
     <row r="156" spans="2:8">
       <c r="B156" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A156)-ROW($A$61)+1)</f>
+        <f t="shared" si="242"/>
         <v>V_EF16</v>
       </c>
       <c r="C156" t="s">
@@ -8674,19 +8901,19 @@
     </row>
     <row r="157" spans="2:8">
       <c r="B157" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A157)-ROW($A$61)+1)</f>
+        <f t="shared" ref="B157:B181" si="248">INDEX($B$49:$DR$49,1,ROW(A157)-ROW($A$61)+1)</f>
         <v>V_FG16</v>
       </c>
       <c r="C157" t="s">
         <v>635</v>
       </c>
       <c r="D157">
-        <v>0</v>
+        <v>-0.7</v>
       </c>
     </row>
     <row r="158" spans="2:8">
       <c r="B158" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A158)-ROW($A$61)+1)</f>
+        <f t="shared" si="248"/>
         <v>V_AB17</v>
       </c>
       <c r="C158" t="s">
@@ -8698,7 +8925,7 @@
     </row>
     <row r="159" spans="2:8">
       <c r="B159" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A159)-ROW($A$61)+1)</f>
+        <f t="shared" si="248"/>
         <v>V_BC17</v>
       </c>
       <c r="C159" t="s">
@@ -8710,7 +8937,7 @@
     </row>
     <row r="160" spans="2:8">
       <c r="B160" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A160)-ROW($A$61)+1)</f>
+        <f t="shared" si="248"/>
         <v>V_CD17</v>
       </c>
       <c r="C160" t="s">
@@ -8720,7 +8947,7 @@
         <v>0</v>
       </c>
       <c r="F160">
-        <f t="shared" ref="F160" ca="1" si="245">((1+RAND()*$I$43*(RANDBETWEEN(0,1)*2-1))*$J$43+($J$43=0))*($I$41*(H160=0)+G160*H160)</f>
+        <f t="shared" ref="F160" ca="1" si="249">((1+RAND()*$I$43*(RANDBETWEEN(0,1)*2-1))*$J$43+($J$43=0))*($I$41*(H160=0)+G160*H160)</f>
         <v>0</v>
       </c>
       <c r="G160" s="7">
@@ -8732,7 +8959,7 @@
     </row>
     <row r="161" spans="2:8">
       <c r="B161" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A161)-ROW($A$61)+1)</f>
+        <f t="shared" si="248"/>
         <v>V_DE17</v>
       </c>
       <c r="C161" t="s">
@@ -8744,7 +8971,7 @@
     </row>
     <row r="162" spans="2:8">
       <c r="B162" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A162)-ROW($A$61)+1)</f>
+        <f t="shared" si="248"/>
         <v>V_EF17</v>
       </c>
       <c r="C162" t="s">
@@ -8756,19 +8983,19 @@
     </row>
     <row r="163" spans="2:8">
       <c r="B163" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A163)-ROW($A$61)+1)</f>
+        <f t="shared" si="248"/>
         <v>V_FG17</v>
       </c>
       <c r="C163" t="s">
         <v>636</v>
       </c>
       <c r="D163">
-        <v>0</v>
+        <v>-0.7</v>
       </c>
     </row>
     <row r="164" spans="2:8">
       <c r="B164" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A164)-ROW($A$61)+1)</f>
+        <f t="shared" si="248"/>
         <v>V_AB18</v>
       </c>
       <c r="C164" t="s">
@@ -8780,7 +9007,7 @@
     </row>
     <row r="165" spans="2:8">
       <c r="B165" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A165)-ROW($A$61)+1)</f>
+        <f t="shared" si="248"/>
         <v>V_BC18</v>
       </c>
       <c r="C165" t="s">
@@ -8792,7 +9019,7 @@
     </row>
     <row r="166" spans="2:8">
       <c r="B166" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A166)-ROW($A$61)+1)</f>
+        <f t="shared" si="248"/>
         <v>V_CD18</v>
       </c>
       <c r="C166" t="s">
@@ -8802,7 +9029,7 @@
         <v>0</v>
       </c>
       <c r="F166">
-        <f t="shared" ref="F166" ca="1" si="246">((1+RAND()*$I$43*(RANDBETWEEN(0,1)*2-1))*$J$43+($J$43=0))*($I$41*(H166=0)+G166*H166)</f>
+        <f t="shared" ref="F166" ca="1" si="250">((1+RAND()*$I$43*(RANDBETWEEN(0,1)*2-1))*$J$43+($J$43=0))*($I$41*(H166=0)+G166*H166)</f>
         <v>0</v>
       </c>
       <c r="G166" s="7">
@@ -8814,7 +9041,7 @@
     </row>
     <row r="167" spans="2:8">
       <c r="B167" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A167)-ROW($A$61)+1)</f>
+        <f t="shared" si="248"/>
         <v>V_DE18</v>
       </c>
       <c r="C167" t="s">
@@ -8826,7 +9053,7 @@
     </row>
     <row r="168" spans="2:8">
       <c r="B168" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A168)-ROW($A$61)+1)</f>
+        <f t="shared" si="248"/>
         <v>V_EF18</v>
       </c>
       <c r="C168" t="s">
@@ -8838,19 +9065,19 @@
     </row>
     <row r="169" spans="2:8">
       <c r="B169" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A169)-ROW($A$61)+1)</f>
+        <f t="shared" si="248"/>
         <v>V_FG18</v>
       </c>
       <c r="C169" t="s">
         <v>637</v>
       </c>
       <c r="D169">
-        <v>0</v>
+        <v>-0.7</v>
       </c>
     </row>
     <row r="170" spans="2:8">
       <c r="B170" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A170)-ROW($A$61)+1)</f>
+        <f t="shared" si="248"/>
         <v>V_AB19</v>
       </c>
       <c r="C170" t="s">
@@ -8862,7 +9089,7 @@
     </row>
     <row r="171" spans="2:8">
       <c r="B171" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A171)-ROW($A$61)+1)</f>
+        <f t="shared" si="248"/>
         <v>V_BC19</v>
       </c>
       <c r="C171" t="s">
@@ -8874,7 +9101,7 @@
     </row>
     <row r="172" spans="2:8">
       <c r="B172" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A172)-ROW($A$61)+1)</f>
+        <f t="shared" si="248"/>
         <v>V_CD19</v>
       </c>
       <c r="C172" t="s">
@@ -8884,7 +9111,7 @@
         <v>0</v>
       </c>
       <c r="F172">
-        <f t="shared" ref="F172" ca="1" si="247">((1+RAND()*$I$43*(RANDBETWEEN(0,1)*2-1))*$J$43+($J$43=0))*($I$41*(H172=0)+G172*H172)</f>
+        <f t="shared" ref="F172" ca="1" si="251">((1+RAND()*$I$43*(RANDBETWEEN(0,1)*2-1))*$J$43+($J$43=0))*($I$41*(H172=0)+G172*H172)</f>
         <v>0</v>
       </c>
       <c r="G172" s="7">
@@ -8896,7 +9123,7 @@
     </row>
     <row r="173" spans="2:8">
       <c r="B173" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A173)-ROW($A$61)+1)</f>
+        <f t="shared" si="248"/>
         <v>V_DE19</v>
       </c>
       <c r="C173" t="s">
@@ -8908,7 +9135,7 @@
     </row>
     <row r="174" spans="2:8">
       <c r="B174" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A174)-ROW($A$61)+1)</f>
+        <f t="shared" si="248"/>
         <v>V_EF19</v>
       </c>
       <c r="C174" t="s">
@@ -8920,19 +9147,19 @@
     </row>
     <row r="175" spans="2:8">
       <c r="B175" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A175)-ROW($A$61)+1)</f>
+        <f t="shared" si="248"/>
         <v>V_FG19</v>
       </c>
       <c r="C175" t="s">
         <v>638</v>
       </c>
       <c r="D175">
-        <v>0</v>
+        <v>-0.7</v>
       </c>
     </row>
     <row r="176" spans="2:8">
       <c r="B176" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A176)-ROW($A$61)+1)</f>
+        <f t="shared" si="248"/>
         <v>V_AB20</v>
       </c>
       <c r="C176" t="s">
@@ -8944,7 +9171,7 @@
     </row>
     <row r="177" spans="2:8">
       <c r="B177" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A177)-ROW($A$61)+1)</f>
+        <f t="shared" si="248"/>
         <v>V_BC20</v>
       </c>
       <c r="C177" t="s">
@@ -8956,7 +9183,7 @@
     </row>
     <row r="178" spans="2:8">
       <c r="B178" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A178)-ROW($A$61)+1)</f>
+        <f t="shared" si="248"/>
         <v>V_CD20</v>
       </c>
       <c r="C178" t="s">
@@ -8966,7 +9193,7 @@
         <v>0</v>
       </c>
       <c r="F178">
-        <f t="shared" ref="F178" ca="1" si="248">((1+RAND()*$I$43*(RANDBETWEEN(0,1)*2-1))*$J$43+($J$43=0))*($I$41*(H178=0)+G178*H178)</f>
+        <f t="shared" ref="F178" ca="1" si="252">((1+RAND()*$I$43*(RANDBETWEEN(0,1)*2-1))*$J$43+($J$43=0))*($I$41*(H178=0)+G178*H178)</f>
         <v>0</v>
       </c>
       <c r="G178" s="7">
@@ -8978,7 +9205,7 @@
     </row>
     <row r="179" spans="2:8">
       <c r="B179" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A179)-ROW($A$61)+1)</f>
+        <f t="shared" si="248"/>
         <v>V_DE20</v>
       </c>
       <c r="C179" t="s">
@@ -8990,7 +9217,7 @@
     </row>
     <row r="180" spans="2:8">
       <c r="B180" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A180)-ROW($A$61)+1)</f>
+        <f t="shared" si="248"/>
         <v>V_FG20</v>
       </c>
       <c r="C180" t="s">
@@ -9002,14 +9229,14 @@
     </row>
     <row r="181" spans="2:8">
       <c r="B181" t="str">
-        <f>INDEX($B$49:$DR$49,1,ROW(A181)-ROW($A$61)+1)</f>
+        <f t="shared" si="248"/>
         <v>V_EF20</v>
       </c>
       <c r="C181" t="s">
         <v>639</v>
       </c>
       <c r="D181">
-        <v>0</v>
+        <v>-0.7</v>
       </c>
     </row>
   </sheetData>
@@ -9749,7 +9976,7 @@
       </c>
       <c r="CZ3" s="6">
         <f ca="1">Sheet1!B52</f>
-        <v>-3.4635416666666674</v>
+        <v>-1.7910196524007909</v>
       </c>
     </row>
     <row r="4" spans="1:225">
@@ -9758,87 +9985,87 @@
       </c>
       <c r="CZ4" s="3">
         <f ca="1">Sheet1!B50^2</f>
-        <v>3.6863999999999994E-4</v>
+        <v>7.1289000000000009E-4</v>
       </c>
       <c r="DA4">
         <f ca="1">-(Sheet1!C50^2)</f>
-        <v>-1.1960766227498054E-6</v>
+        <v>-1.3127069730331721E-6</v>
       </c>
       <c r="DG4">
         <f ca="1">-(Sheet1!I50^2)</f>
-        <v>-1.168518497055047E-6</v>
+        <v>-1.2141250941051004E-6</v>
       </c>
       <c r="DM4">
         <f ca="1">-(Sheet1!O50^2)</f>
-        <v>-9.5344047148208087E-7</v>
+        <v>-9.5663759446961865E-7</v>
       </c>
       <c r="DS4">
         <f ca="1">-(Sheet1!U50^2)</f>
-        <v>-1.0144889956062187E-6</v>
+        <v>-1.1450979088674969E-6</v>
       </c>
       <c r="DY4">
         <f ca="1">-(Sheet1!AA50^2)</f>
-        <v>-9.8863284205893557E-7</v>
+        <v>-1.0506443169154662E-6</v>
       </c>
       <c r="EE4">
         <f ca="1">-(Sheet1!AG50^2)</f>
-        <v>-9.9753995181603022E-7</v>
+        <v>-1.2111152447768363E-6</v>
       </c>
       <c r="EK4">
         <f ca="1">-(Sheet1!AM50^2)</f>
-        <v>-1.2635159449181813E-6</v>
+        <v>-1.3778119872969364E-6</v>
       </c>
       <c r="EQ4">
         <f ca="1">-(Sheet1!AS50^2)</f>
-        <v>-1.2809643826525153E-6</v>
+        <v>-9.5460928942568367E-7</v>
       </c>
       <c r="EW4">
         <f ca="1">-(Sheet1!AY50^2)</f>
-        <v>-1.1051039186882867E-6</v>
+        <v>-1.2501088893123676E-6</v>
       </c>
       <c r="FC4">
         <f ca="1">-(Sheet1!BE50^2)</f>
-        <v>-1.3528578021126827E-6</v>
+        <v>-1.0643986030204324E-6</v>
       </c>
       <c r="FI4">
         <f ca="1">-(Sheet1!BK50^2)</f>
-        <v>-1.1671410977459289E-6</v>
+        <v>-1.2950661961185711E-6</v>
       </c>
       <c r="FO4">
         <f ca="1">-(Sheet1!BQ50^2)</f>
-        <v>-9.6890077605833115E-7</v>
+        <v>-9.750459380051963E-7</v>
       </c>
       <c r="FU4">
         <f ca="1">-(Sheet1!BW50^2)</f>
-        <v>-1.0667200120372466E-6</v>
+        <v>-1.1851742158622673E-6</v>
       </c>
       <c r="GA4">
         <f ca="1">-(Sheet1!CC50^2)</f>
-        <v>-1.2652742957734665E-6</v>
+        <v>-1.0543085964011856E-6</v>
       </c>
       <c r="GG4">
         <f ca="1">-(Sheet1!CI50^2)</f>
-        <v>-1.3504293322013845E-6</v>
+        <v>-1.2073736998585188E-6</v>
       </c>
       <c r="GM4">
         <f ca="1">-(Sheet1!CO50^2)</f>
-        <v>-9.2963331457321917E-7</v>
+        <v>-1.0155513959951284E-6</v>
       </c>
       <c r="GS4">
         <f ca="1">-(Sheet1!CU50^2)</f>
-        <v>-1.0111476683218931E-6</v>
+        <v>-1.1505832473346974E-6</v>
       </c>
       <c r="GY4">
         <f ca="1">-(Sheet1!DA50^2)</f>
-        <v>-1.1285838201935401E-6</v>
+        <v>-1.3821721014838394E-6</v>
       </c>
       <c r="HE4">
         <f ca="1">-(Sheet1!DG50^2)</f>
-        <v>-1.2523457047401696E-6</v>
+        <v>-9.8293658637305797E-7</v>
       </c>
       <c r="HK4">
         <f ca="1">-(Sheet1!DM50^2)</f>
-        <v>-1.2194825755777175E-6</v>
+        <v>-9.9432348592736186E-7</v>
       </c>
     </row>
     <row r="5" spans="1:225" s="6" customFormat="1">
@@ -9853,7 +10080,7 @@
       </c>
       <c r="DA5" s="6">
         <f ca="1">Sheet1!C$52</f>
-        <v>-21.349802775421026</v>
+        <v>-19.452932394345336</v>
       </c>
     </row>
     <row r="6" spans="1:225">
@@ -9883,7 +10110,7 @@
       </c>
       <c r="DC7">
         <f ca="1">Sheet1!E$52</f>
-        <v>-1105.2631578947367</v>
+        <v>-12668.249999999996</v>
       </c>
     </row>
     <row r="8" spans="1:225">
@@ -9934,7 +10161,7 @@
       </c>
       <c r="DA11">
         <f ca="1">(Sheet1!C$50^2)</f>
-        <v>1.1960766227498054E-6</v>
+        <v>1.3127069730331721E-6</v>
       </c>
       <c r="DB11">
         <f ca="1">-(Sheet1!D$50^2)</f>
@@ -9951,7 +10178,7 @@
       </c>
       <c r="DC12">
         <f ca="1">-(Sheet1!E$50^2)</f>
-        <v>-2.3104000000000003E-8</v>
+        <v>-2.5600000000000004E-8</v>
       </c>
     </row>
     <row r="13" spans="1:225">
@@ -9960,7 +10187,7 @@
       </c>
       <c r="DC13">
         <f ca="1">-DC12</f>
-        <v>2.3104000000000003E-8</v>
+        <v>2.5600000000000004E-8</v>
       </c>
       <c r="DD13">
         <f ca="1">-(Sheet1!F$50^2)</f>
@@ -10005,7 +10232,7 @@
       </c>
       <c r="DG16" s="6">
         <f ca="1">Sheet1!I$52</f>
-        <v>-21.853312604256569</v>
+        <v>-21.032429132701449</v>
       </c>
     </row>
     <row r="17" spans="1:122">
@@ -10035,7 +10262,7 @@
       </c>
       <c r="DI18">
         <f ca="1">Sheet1!K$52</f>
-        <v>-1105.2631578947367</v>
+        <v>-12668.249999999996</v>
       </c>
     </row>
     <row r="19" spans="1:122">
@@ -10086,7 +10313,7 @@
       </c>
       <c r="DG22">
         <f ca="1">(Sheet1!I$50^2)</f>
-        <v>1.168518497055047E-6</v>
+        <v>1.2141250941051004E-6</v>
       </c>
       <c r="DH22">
         <f ca="1">-(Sheet1!J$50^2)</f>
@@ -10103,7 +10330,7 @@
       </c>
       <c r="DI23">
         <f ca="1">-(Sheet1!K$50^2)</f>
-        <v>-2.3104000000000003E-8</v>
+        <v>-2.5600000000000004E-8</v>
       </c>
     </row>
     <row r="24" spans="1:122">
@@ -10112,7 +10339,7 @@
       </c>
       <c r="DI24">
         <f ca="1">-DI23</f>
-        <v>2.3104000000000003E-8</v>
+        <v>2.5600000000000004E-8</v>
       </c>
       <c r="DJ24">
         <f ca="1">-(Sheet1!L$50^2)</f>
@@ -10157,7 +10384,7 @@
       </c>
       <c r="DM27" s="6">
         <f ca="1">Sheet1!O$52</f>
-        <v>-26.783004040415257</v>
+        <v>-26.693494116920768</v>
       </c>
     </row>
     <row r="28" spans="1:122">
@@ -10187,7 +10414,7 @@
       </c>
       <c r="DO29">
         <f ca="1">Sheet1!Q$52</f>
-        <v>-1105.2631578947367</v>
+        <v>-12668.249999999996</v>
       </c>
     </row>
     <row r="30" spans="1:122">
@@ -10243,7 +10470,7 @@
       <c r="L33" s="4"/>
       <c r="DM33">
         <f ca="1">(Sheet1!O$50^2)</f>
-        <v>9.5344047148208087E-7</v>
+        <v>9.5663759446961865E-7</v>
       </c>
       <c r="DN33">
         <f ca="1">-(Sheet1!P$50^2)</f>
@@ -10265,7 +10492,7 @@
       </c>
       <c r="DO34">
         <f ca="1">-(Sheet1!Q$50^2)</f>
-        <v>-2.3104000000000003E-8</v>
+        <v>-2.5600000000000004E-8</v>
       </c>
     </row>
     <row r="35" spans="1:128">
@@ -10279,7 +10506,7 @@
       <c r="L35" s="4"/>
       <c r="DO35">
         <f ca="1">-DO34</f>
-        <v>2.3104000000000003E-8</v>
+        <v>2.5600000000000004E-8</v>
       </c>
       <c r="DP35">
         <f ca="1">-(Sheet1!R$50^2)</f>
@@ -10334,7 +10561,7 @@
       </c>
       <c r="DS38" s="6">
         <f ca="1">Sheet1!U$52</f>
-        <v>-25.171293242802196</v>
+        <v>-22.300276511075925</v>
       </c>
     </row>
     <row r="39" spans="1:128">
@@ -10364,7 +10591,7 @@
       </c>
       <c r="DU40">
         <f ca="1">Sheet1!W$52</f>
-        <v>-1105.2631578947367</v>
+        <v>-12668.249999999996</v>
       </c>
     </row>
     <row r="41" spans="1:128">
@@ -10430,7 +10657,7 @@
       <c r="Q44" s="4"/>
       <c r="DS44">
         <f ca="1">(Sheet1!U$50^2)</f>
-        <v>1.0144889956062187E-6</v>
+        <v>1.1450979088674969E-6</v>
       </c>
       <c r="DT44">
         <f ca="1">-(Sheet1!V$50^2)</f>
@@ -10452,7 +10679,7 @@
       </c>
       <c r="DU45">
         <f ca="1">-(Sheet1!W$50^2)</f>
-        <v>-2.3104000000000003E-8</v>
+        <v>-2.5600000000000004E-8</v>
       </c>
     </row>
     <row r="46" spans="1:128">
@@ -10466,7 +10693,7 @@
       <c r="Q46" s="4"/>
       <c r="DU46">
         <f ca="1">-DU45</f>
-        <v>2.3104000000000003E-8</v>
+        <v>2.5600000000000004E-8</v>
       </c>
       <c r="DV46">
         <f ca="1">-(Sheet1!X$50^2)</f>
@@ -10511,7 +10738,7 @@
       </c>
       <c r="DY49" s="6">
         <f ca="1">Sheet1!AA$52</f>
-        <v>-25.829609247876594</v>
+        <v>-24.305085545001432</v>
       </c>
     </row>
     <row r="50" spans="1:139">
@@ -10546,7 +10773,7 @@
       </c>
       <c r="EA51">
         <f ca="1">Sheet1!AC$52</f>
-        <v>-1105.2631578947367</v>
+        <v>-12668.249999999996</v>
       </c>
     </row>
     <row r="52" spans="1:139">
@@ -10617,7 +10844,7 @@
       <c r="V55" s="4"/>
       <c r="DY55">
         <f ca="1">(Sheet1!AA$50^2)</f>
-        <v>9.8863284205893557E-7</v>
+        <v>1.0506443169154662E-6</v>
       </c>
       <c r="DZ55">
         <f ca="1">-(Sheet1!AB$50^2)</f>
@@ -10634,7 +10861,7 @@
       </c>
       <c r="EA56">
         <f ca="1">-(Sheet1!AC$50^2)</f>
-        <v>-2.3104000000000003E-8</v>
+        <v>-2.5600000000000004E-8</v>
       </c>
     </row>
     <row r="57" spans="1:139">
@@ -10643,7 +10870,7 @@
       </c>
       <c r="EA57">
         <f ca="1">-EA56</f>
-        <v>2.3104000000000003E-8</v>
+        <v>2.5600000000000004E-8</v>
       </c>
       <c r="EB57">
         <f ca="1">-(Sheet1!AD$50^2)</f>
@@ -10693,7 +10920,7 @@
       </c>
       <c r="EE60" s="6">
         <f ca="1">Sheet1!AG$52</f>
-        <v>-25.598974711249898</v>
+        <v>-21.08469867762695</v>
       </c>
     </row>
     <row r="61" spans="1:139">
@@ -10733,7 +10960,7 @@
       </c>
       <c r="EG62">
         <f ca="1">Sheet1!AI$52</f>
-        <v>-1105.2631578947367</v>
+        <v>-12668.249999999996</v>
       </c>
     </row>
     <row r="63" spans="1:139">
@@ -10794,7 +11021,7 @@
       </c>
       <c r="EE66">
         <f ca="1">(Sheet1!AG$50^2)</f>
-        <v>9.9753995181603022E-7</v>
+        <v>1.2111152447768363E-6</v>
       </c>
       <c r="EF66">
         <f ca="1">-(Sheet1!AH$50^2)</f>
@@ -10811,7 +11038,7 @@
       </c>
       <c r="EG67">
         <f ca="1">-(Sheet1!AI$50^2)</f>
-        <v>-2.3104000000000003E-8</v>
+        <v>-2.5600000000000004E-8</v>
       </c>
     </row>
     <row r="68" spans="1:146">
@@ -10820,7 +11047,7 @@
       </c>
       <c r="EG68">
         <f ca="1">-EG67</f>
-        <v>2.3104000000000003E-8</v>
+        <v>2.5600000000000004E-8</v>
       </c>
       <c r="EH68">
         <f ca="1">-(Sheet1!AJ$50^2)</f>
@@ -10883,7 +11110,7 @@
       </c>
       <c r="EK71" s="6">
         <f ca="1">Sheet1!AM$52</f>
-        <v>-20.210271269393107</v>
+        <v>-18.53373336524518</v>
       </c>
     </row>
     <row r="72" spans="1:146">
@@ -10925,7 +11152,7 @@
       </c>
       <c r="EM73">
         <f ca="1">Sheet1!AO$52</f>
-        <v>-1105.2631578947367</v>
+        <v>-12668.249999999996</v>
       </c>
     </row>
     <row r="74" spans="1:146">
@@ -10976,7 +11203,7 @@
       </c>
       <c r="EK77">
         <f ca="1">(Sheet1!AM$50^2)</f>
-        <v>1.2635159449181813E-6</v>
+        <v>1.3778119872969364E-6</v>
       </c>
       <c r="EL77">
         <f ca="1">-(Sheet1!AN$50^2)</f>
@@ -10998,7 +11225,7 @@
       </c>
       <c r="EM78">
         <f ca="1">-(Sheet1!AO$50^2)</f>
-        <v>-2.3104000000000003E-8</v>
+        <v>-2.5600000000000004E-8</v>
       </c>
     </row>
     <row r="79" spans="1:146">
@@ -11012,7 +11239,7 @@
       <c r="AK79" s="4"/>
       <c r="EM79">
         <f ca="1">-EM78</f>
-        <v>2.3104000000000003E-8</v>
+        <v>2.5600000000000004E-8</v>
       </c>
       <c r="EN79">
         <f ca="1">-(Sheet1!AP$50^2)</f>
@@ -11072,7 +11299,7 @@
       </c>
       <c r="EQ82" s="6">
         <f ca="1">Sheet1!AS$52</f>
-        <v>-19.934980508296537</v>
+        <v>-26.75021108935896</v>
       </c>
     </row>
     <row r="83" spans="1:156">
@@ -11102,7 +11329,7 @@
       </c>
       <c r="ES84">
         <f ca="1">Sheet1!AU$52</f>
-        <v>-1105.2631578947367</v>
+        <v>-12668.249999999996</v>
       </c>
     </row>
     <row r="85" spans="1:156">
@@ -11159,7 +11386,7 @@
       <c r="AP88" s="4"/>
       <c r="EQ88">
         <f ca="1">(Sheet1!AS$50^2)</f>
-        <v>1.2809643826525153E-6</v>
+        <v>9.5460928942568367E-7</v>
       </c>
       <c r="ER88">
         <f ca="1">-(Sheet1!AT$50^2)</f>
@@ -11181,7 +11408,7 @@
       </c>
       <c r="ES89">
         <f ca="1">-(Sheet1!AU$50^2)</f>
-        <v>-2.3104000000000003E-8</v>
+        <v>-2.5600000000000004E-8</v>
       </c>
     </row>
     <row r="90" spans="1:156">
@@ -11195,7 +11422,7 @@
       <c r="AP90" s="4"/>
       <c r="ES90">
         <f ca="1">-ES89</f>
-        <v>2.3104000000000003E-8</v>
+        <v>2.5600000000000004E-8</v>
       </c>
       <c r="ET90">
         <f ca="1">-(Sheet1!AV$50^2)</f>
@@ -11245,7 +11472,7 @@
       </c>
       <c r="EW93" s="6">
         <f ca="1">Sheet1!AY$52</f>
-        <v>-23.107329155352367</v>
+        <v>-20.427020572620904</v>
       </c>
     </row>
     <row r="94" spans="1:156">
@@ -11275,7 +11502,7 @@
       </c>
       <c r="EY95">
         <f ca="1">Sheet1!BA$52</f>
-        <v>-1105.2631578947367</v>
+        <v>-12668.249999999996</v>
       </c>
     </row>
     <row r="96" spans="1:156">
@@ -11334,7 +11561,7 @@
       <c r="AU99" s="4"/>
       <c r="EW99">
         <f ca="1">(Sheet1!AY$50^2)</f>
-        <v>1.1051039186882867E-6</v>
+        <v>1.2501088893123676E-6</v>
       </c>
       <c r="EX99">
         <f ca="1">-(Sheet1!AZ$50^2)</f>
@@ -11356,7 +11583,7 @@
       </c>
       <c r="EY100">
         <f ca="1">-(Sheet1!BA$50^2)</f>
-        <v>-2.3104000000000003E-8</v>
+        <v>-2.5600000000000004E-8</v>
       </c>
     </row>
     <row r="101" spans="1:164">
@@ -11365,7 +11592,7 @@
       </c>
       <c r="EY101">
         <f ca="1">-EY100</f>
-        <v>2.3104000000000003E-8</v>
+        <v>2.5600000000000004E-8</v>
       </c>
       <c r="EZ101">
         <f ca="1">-(Sheet1!BB$50^2)</f>
@@ -11410,7 +11637,7 @@
       </c>
       <c r="FC104" s="6">
         <f ca="1">Sheet1!BE$52</f>
-        <v>-18.87559798237616</v>
+        <v>-23.99101232145248</v>
       </c>
     </row>
     <row r="105" spans="1:164">
@@ -11442,7 +11669,7 @@
       </c>
       <c r="FE106">
         <f ca="1">Sheet1!BG$52</f>
-        <v>-1105.2631578947367</v>
+        <v>-12668.249999999996</v>
       </c>
     </row>
     <row r="107" spans="1:164">
@@ -11496,7 +11723,7 @@
       </c>
       <c r="FC110">
         <f ca="1">(Sheet1!BE$50^2)</f>
-        <v>1.3528578021126827E-6</v>
+        <v>1.0643986030204324E-6</v>
       </c>
       <c r="FD110">
         <f ca="1">-(Sheet1!BF$50^2)</f>
@@ -11513,7 +11740,7 @@
       </c>
       <c r="FE111">
         <f ca="1">-(Sheet1!BG$50^2)</f>
-        <v>-2.3104000000000003E-8</v>
+        <v>-2.5600000000000004E-8</v>
       </c>
     </row>
     <row r="112" spans="1:164">
@@ -11522,7 +11749,7 @@
       </c>
       <c r="FE112">
         <f ca="1">-FE111</f>
-        <v>2.3104000000000003E-8</v>
+        <v>2.5600000000000004E-8</v>
       </c>
       <c r="FF112">
         <f ca="1">-(Sheet1!BH$50^2)</f>
@@ -11573,7 +11800,7 @@
       </c>
       <c r="FI115" s="6">
         <f ca="1">Sheet1!BK$52</f>
-        <v>-21.879102748859633</v>
+        <v>-19.717911004498202</v>
       </c>
     </row>
     <row r="116" spans="1:173">
@@ -11605,7 +11832,7 @@
       </c>
       <c r="FK117">
         <f ca="1">Sheet1!BM$52</f>
-        <v>-1105.2631578947367</v>
+        <v>-12668.249999999996</v>
       </c>
     </row>
     <row r="118" spans="1:173">
@@ -11657,7 +11884,7 @@
       </c>
       <c r="FI121">
         <f ca="1">(Sheet1!BK$50^2)</f>
-        <v>1.1671410977459289E-6</v>
+        <v>1.2950661961185711E-6</v>
       </c>
       <c r="FJ121">
         <f ca="1">-(Sheet1!BL$50^2)</f>
@@ -11674,7 +11901,7 @@
       </c>
       <c r="FK122">
         <f ca="1">-(Sheet1!BM$50^2)</f>
-        <v>-2.3104000000000003E-8</v>
+        <v>-2.5600000000000004E-8</v>
       </c>
     </row>
     <row r="123" spans="1:173">
@@ -11689,7 +11916,7 @@
       <c r="BJ123" s="4"/>
       <c r="FK123">
         <f ca="1">-FK122</f>
-        <v>2.3104000000000003E-8</v>
+        <v>2.5600000000000004E-8</v>
       </c>
       <c r="FL123">
         <f ca="1">-(Sheet1!BN$50^2)</f>
@@ -11748,7 +11975,7 @@
       </c>
       <c r="FO126" s="6">
         <f ca="1">Sheet1!BQ$52</f>
-        <v>-26.355639948896734</v>
+        <v>-26.189535287171168</v>
       </c>
     </row>
     <row r="127" spans="1:173">
@@ -11780,7 +12007,7 @@
       </c>
       <c r="FQ128">
         <f ca="1">Sheet1!BS$52</f>
-        <v>-1105.2631578947367</v>
+        <v>-12668.249999999996</v>
       </c>
     </row>
     <row r="129" spans="1:182">
@@ -11836,7 +12063,7 @@
       <c r="BO132" s="4"/>
       <c r="FO132">
         <f ca="1">(Sheet1!BQ$50^2)</f>
-        <v>9.6890077605833115E-7</v>
+        <v>9.750459380051963E-7</v>
       </c>
       <c r="FP132">
         <f ca="1">-(Sheet1!BR$50^2)</f>
@@ -11858,7 +12085,7 @@
       </c>
       <c r="FQ133">
         <f ca="1">-(Sheet1!BS$50^2)</f>
-        <v>-2.3104000000000003E-8</v>
+        <v>-2.5600000000000004E-8</v>
       </c>
     </row>
     <row r="134" spans="1:182">
@@ -11872,7 +12099,7 @@
       <c r="BO134" s="4"/>
       <c r="FQ134">
         <f ca="1">-FQ133</f>
-        <v>2.3104000000000003E-8</v>
+        <v>2.5600000000000004E-8</v>
       </c>
       <c r="FR134">
         <f ca="1">-(Sheet1!BT$50^2)</f>
@@ -11927,7 +12154,7 @@
       </c>
       <c r="FU137" s="6">
         <f ca="1">Sheet1!BW$52</f>
-        <v>-23.938802789713073</v>
+        <v>-21.54619941796609</v>
       </c>
     </row>
     <row r="138" spans="1:182">
@@ -11957,7 +12184,7 @@
       </c>
       <c r="FW139">
         <f ca="1">Sheet1!BY$52</f>
-        <v>-1105.2631578947367</v>
+        <v>-12668.249999999996</v>
       </c>
     </row>
     <row r="140" spans="1:182">
@@ -12021,7 +12248,7 @@
       <c r="BT143" s="4"/>
       <c r="FU143">
         <f ca="1">(Sheet1!BW$50^2)</f>
-        <v>1.0667200120372466E-6</v>
+        <v>1.1851742158622673E-6</v>
       </c>
       <c r="FV143">
         <f ca="1">-(Sheet1!BX$50^2)</f>
@@ -12043,7 +12270,7 @@
       </c>
       <c r="FW144">
         <f ca="1">-(Sheet1!BY$50^2)</f>
-        <v>-2.3104000000000003E-8</v>
+        <v>-2.5600000000000004E-8</v>
       </c>
     </row>
     <row r="145" spans="1:190">
@@ -12057,7 +12284,7 @@
       <c r="BT145" s="4"/>
       <c r="FW145">
         <f ca="1">-FW144</f>
-        <v>2.3104000000000003E-8</v>
+        <v>2.5600000000000004E-8</v>
       </c>
       <c r="FX145">
         <f ca="1">-(Sheet1!BZ$50^2)</f>
@@ -12102,7 +12329,7 @@
       </c>
       <c r="GA148" s="6">
         <f ca="1">Sheet1!CC$52</f>
-        <v>-20.182185068724372</v>
+        <v>-24.220612529543523</v>
       </c>
     </row>
     <row r="149" spans="1:190">
@@ -12136,7 +12363,7 @@
       <c r="BY150" s="4"/>
       <c r="GC150">
         <f ca="1">Sheet1!CE$52</f>
-        <v>-1105.2631578947367</v>
+        <v>-12668.249999999996</v>
       </c>
     </row>
     <row r="151" spans="1:190">
@@ -12204,7 +12431,7 @@
       <c r="BY154" s="4"/>
       <c r="GA154">
         <f ca="1">(Sheet1!CC$50^2)</f>
-        <v>1.2652742957734665E-6</v>
+        <v>1.0543085964011856E-6</v>
       </c>
       <c r="GB154">
         <f ca="1">-(Sheet1!CD$50^2)</f>
@@ -12221,7 +12448,7 @@
       </c>
       <c r="GC155">
         <f ca="1">-(Sheet1!CE$50^2)</f>
-        <v>-2.3104000000000003E-8</v>
+        <v>-2.5600000000000004E-8</v>
       </c>
     </row>
     <row r="156" spans="1:190">
@@ -12230,7 +12457,7 @@
       </c>
       <c r="GC156">
         <f ca="1">-GC155</f>
-        <v>2.3104000000000003E-8</v>
+        <v>2.5600000000000004E-8</v>
       </c>
       <c r="GD156">
         <f ca="1">-(Sheet1!CF$50^2)</f>
@@ -12279,7 +12506,7 @@
       <c r="CD159" s="22"/>
       <c r="GG159" s="6">
         <f ca="1">Sheet1!CI$52</f>
-        <v>-18.909541870193848</v>
+        <v>-21.15003830462129</v>
       </c>
     </row>
     <row r="160" spans="1:190">
@@ -12317,7 +12544,7 @@
       <c r="CD161" s="4"/>
       <c r="GI161">
         <f ca="1">Sheet1!CK$52</f>
-        <v>-1105.2631578947367</v>
+        <v>-12668.249999999996</v>
       </c>
     </row>
     <row r="162" spans="1:200">
@@ -12376,7 +12603,7 @@
       </c>
       <c r="GG165">
         <f ca="1">(Sheet1!CI$50^2)</f>
-        <v>1.3504293322013845E-6</v>
+        <v>1.2073736998585188E-6</v>
       </c>
       <c r="GH165">
         <f ca="1">-(Sheet1!CJ$50^2)</f>
@@ -12393,7 +12620,7 @@
       </c>
       <c r="GI166">
         <f ca="1">-(Sheet1!CK$50^2)</f>
-        <v>-2.3104000000000003E-8</v>
+        <v>-2.5600000000000004E-8</v>
       </c>
     </row>
     <row r="167" spans="1:200">
@@ -12402,7 +12629,7 @@
       </c>
       <c r="GI167">
         <f ca="1">-GI166</f>
-        <v>2.3104000000000003E-8</v>
+        <v>2.5600000000000004E-8</v>
       </c>
       <c r="GJ167">
         <f ca="1">-(Sheet1!CL$50^2)</f>
@@ -12461,7 +12688,7 @@
       <c r="CI170" s="22"/>
       <c r="GM170" s="6">
         <f ca="1">Sheet1!CO$52</f>
-        <v>-27.468895100562523</v>
+        <v>-25.144960757970832</v>
       </c>
     </row>
     <row r="171" spans="1:200">
@@ -12499,7 +12726,7 @@
       <c r="CI172" s="4"/>
       <c r="GO172">
         <f ca="1">Sheet1!CQ$52</f>
-        <v>-1105.2631578947367</v>
+        <v>-12668.249999999996</v>
       </c>
     </row>
     <row r="173" spans="1:200">
@@ -12550,7 +12777,7 @@
       </c>
       <c r="GM176">
         <f ca="1">(Sheet1!CO$50^2)</f>
-        <v>9.2963331457321917E-7</v>
+        <v>1.0155513959951284E-6</v>
       </c>
       <c r="GN176">
         <f ca="1">-(Sheet1!CP$50^2)</f>
@@ -12572,7 +12799,7 @@
       </c>
       <c r="GO177">
         <f ca="1">-(Sheet1!CQ$50^2)</f>
-        <v>-2.3104000000000003E-8</v>
+        <v>-2.5600000000000004E-8</v>
       </c>
     </row>
     <row r="178" spans="1:207">
@@ -12586,7 +12813,7 @@
       <c r="CN178" s="4"/>
       <c r="GO178">
         <f ca="1">-GO177</f>
-        <v>2.3104000000000003E-8</v>
+        <v>2.5600000000000004E-8</v>
       </c>
       <c r="GP178">
         <f ca="1">-(Sheet1!CR$50^2)</f>
@@ -12645,7 +12872,7 @@
       <c r="CN181" s="22"/>
       <c r="GS181" s="6">
         <f ca="1">Sheet1!CU$52</f>
-        <v>-25.254471527763798</v>
+        <v>-22.193961244571938</v>
       </c>
     </row>
     <row r="182" spans="1:207">
@@ -12675,7 +12902,7 @@
       </c>
       <c r="GU183">
         <f ca="1">Sheet1!CW$52</f>
-        <v>-1105.2631578947367</v>
+        <v>-12668.249999999996</v>
       </c>
     </row>
     <row r="184" spans="1:207">
@@ -12736,7 +12963,7 @@
       <c r="CS187" s="4"/>
       <c r="GS187">
         <f ca="1">(Sheet1!CU$50^2)</f>
-        <v>1.0111476683218931E-6</v>
+        <v>1.1505832473346974E-6</v>
       </c>
       <c r="GT187">
         <f ca="1">-(Sheet1!CV$50^2)</f>
@@ -12758,7 +12985,7 @@
       </c>
       <c r="GU188">
         <f ca="1">-(Sheet1!CW$50^2)</f>
-        <v>-2.3104000000000003E-8</v>
+        <v>-2.5600000000000004E-8</v>
       </c>
     </row>
     <row r="189" spans="1:207">
@@ -12772,7 +12999,7 @@
       <c r="CS189" s="4"/>
       <c r="GU189">
         <f ca="1">-GU188</f>
-        <v>2.3104000000000003E-8</v>
+        <v>2.5600000000000004E-8</v>
       </c>
       <c r="GV189">
         <f ca="1">-(Sheet1!CX$50^2)</f>
@@ -12822,7 +13049,7 @@
       </c>
       <c r="GY192" s="6">
         <f ca="1">Sheet1!DA$52</f>
-        <v>-22.626587004960651</v>
+        <v>-18.475268002143633</v>
       </c>
     </row>
     <row r="193" spans="1:218">
@@ -12852,7 +13079,7 @@
       </c>
       <c r="HA194">
         <f ca="1">Sheet1!DC$52</f>
-        <v>-1105.2631578947367</v>
+        <v>-12668.249999999996</v>
       </c>
     </row>
     <row r="195" spans="1:218">
@@ -12923,7 +13150,7 @@
       <c r="CX198" s="4"/>
       <c r="GY198">
         <f ca="1">(Sheet1!DA$50^2)</f>
-        <v>1.1285838201935401E-6</v>
+        <v>1.3821721014838394E-6</v>
       </c>
       <c r="GZ198">
         <f ca="1">-(Sheet1!DB$50^2)</f>
@@ -12945,7 +13172,7 @@
       </c>
       <c r="HA199">
         <f ca="1">-(Sheet1!DC$50^2)</f>
-        <v>-2.3104000000000003E-8</v>
+        <v>-2.5600000000000004E-8</v>
       </c>
     </row>
     <row r="200" spans="1:218">
@@ -12954,7 +13181,7 @@
       </c>
       <c r="HA200">
         <f ca="1">-HA199</f>
-        <v>2.3104000000000003E-8</v>
+        <v>2.5600000000000004E-8</v>
       </c>
       <c r="HB200">
         <f ca="1">-(Sheet1!DD$50^2)</f>
@@ -12999,7 +13226,7 @@
       </c>
       <c r="HE203" s="6">
         <f ca="1">Sheet1!DG$52</f>
-        <v>-20.390535858705309</v>
+        <v>-25.979295464242917</v>
       </c>
     </row>
     <row r="204" spans="1:218">
@@ -13029,7 +13256,7 @@
       </c>
       <c r="HG205">
         <f ca="1">Sheet1!DI$52</f>
-        <v>-1105.2631578947367</v>
+        <v>-12668.249999999996</v>
       </c>
     </row>
     <row r="206" spans="1:218">
@@ -13080,7 +13307,7 @@
       </c>
       <c r="HE209">
         <f ca="1">(Sheet1!DG$50^2)</f>
-        <v>1.2523457047401696E-6</v>
+        <v>9.8293658637305797E-7</v>
       </c>
       <c r="HF209">
         <f ca="1">-(Sheet1!DH$50^2)</f>
@@ -13097,7 +13324,7 @@
       </c>
       <c r="HG210">
         <f ca="1">-(Sheet1!DI$50^2)</f>
-        <v>-2.3104000000000003E-8</v>
+        <v>-2.5600000000000004E-8</v>
       </c>
     </row>
     <row r="211" spans="1:223">
@@ -13106,7 +13333,7 @@
       </c>
       <c r="HG211">
         <f ca="1">-HG210</f>
-        <v>2.3104000000000003E-8</v>
+        <v>2.5600000000000004E-8</v>
       </c>
       <c r="HH211">
         <f ca="1">-(Sheet1!DJ$50^2)</f>
@@ -13151,7 +13378,7 @@
       </c>
       <c r="HK214" s="6">
         <f ca="1">Sheet1!DM$52</f>
-        <v>-20.940028591964573</v>
+        <v>-25.68178300262484</v>
       </c>
       <c r="HO214" s="22"/>
     </row>
@@ -13188,7 +13415,7 @@
       <c r="HL216" s="7"/>
       <c r="HM216" s="7">
         <f ca="1">Sheet1!DO$52</f>
-        <v>-1105.2631578947367</v>
+        <v>-12668.249999999996</v>
       </c>
       <c r="HN216" s="7"/>
       <c r="HO216" s="4"/>
@@ -13250,7 +13477,7 @@
       </c>
       <c r="HK220" s="7">
         <f ca="1">(Sheet1!DM$50^2)</f>
-        <v>1.2194825755777175E-6</v>
+        <v>9.9432348592736186E-7</v>
       </c>
       <c r="HL220" s="7">
         <f ca="1">-(Sheet1!DN$50^2)</f>
@@ -13270,7 +13497,7 @@
       </c>
       <c r="HM221" s="7">
         <f ca="1">-(Sheet1!DO$50^2)</f>
-        <v>-2.3104000000000003E-8</v>
+        <v>-2.5600000000000004E-8</v>
       </c>
       <c r="HN221" s="7"/>
     </row>
@@ -13282,7 +13509,7 @@
       <c r="HL222" s="7"/>
       <c r="HM222" s="7">
         <f ca="1">-HM221</f>
-        <v>2.3104000000000003E-8</v>
+        <v>2.5600000000000004E-8</v>
       </c>
       <c r="HN222" s="7">
         <f ca="1">-(Sheet1!DP$50^2)</f>
@@ -16230,7 +16457,7 @@
       </c>
       <c r="B10" s="7">
         <f>Sheet1!$D$67*Sheet1!$I$9-Sheet1!$B$7</f>
-        <v>-98402.6</v>
+        <v>-103503.8</v>
       </c>
     </row>
     <row r="11" spans="1:2" s="7" customFormat="1">
@@ -16324,7 +16551,7 @@
       </c>
       <c r="B21" s="7">
         <f>Sheet1!$D$73*Sheet1!$I$9-Sheet1!$B$7</f>
-        <v>-97421.6</v>
+        <v>-104288.6</v>
       </c>
     </row>
     <row r="22" spans="1:2" s="7" customFormat="1">
@@ -16418,7 +16645,7 @@
       </c>
       <c r="B32" s="7">
         <f>Sheet1!$D$79*Sheet1!$I$9-Sheet1!$B$7</f>
-        <v>-97421.6</v>
+        <v>-104288.6</v>
       </c>
     </row>
     <row r="33" spans="1:2" s="7" customFormat="1">
@@ -16512,7 +16739,7 @@
       </c>
       <c r="B43" s="7">
         <f>Sheet1!$D$85*Sheet1!$I$9-Sheet1!$B$7</f>
-        <v>-97421.6</v>
+        <v>-104288.6</v>
       </c>
     </row>
     <row r="44" spans="1:2" s="7" customFormat="1">
@@ -16606,7 +16833,7 @@
       </c>
       <c r="B54" s="7">
         <f>Sheet1!$D$91*Sheet1!$I$9-Sheet1!$B$7</f>
-        <v>-97421.6</v>
+        <v>-104288.6</v>
       </c>
     </row>
     <row r="55" spans="1:2" s="7" customFormat="1">
@@ -16700,7 +16927,7 @@
       </c>
       <c r="B65" s="7">
         <f>Sheet1!$D$97*Sheet1!$I$9-Sheet1!$B$7</f>
-        <v>-97421.6</v>
+        <v>-104288.6</v>
       </c>
     </row>
     <row r="66" spans="1:2" s="7" customFormat="1">
@@ -16794,7 +17021,7 @@
       </c>
       <c r="B76" s="7">
         <f>Sheet1!$D$103*Sheet1!$I$9-Sheet1!$B$7</f>
-        <v>-97421.6</v>
+        <v>-104288.6</v>
       </c>
     </row>
     <row r="77" spans="1:2" s="7" customFormat="1">
@@ -16888,7 +17115,7 @@
       </c>
       <c r="B87" s="7">
         <f>Sheet1!$D$109*Sheet1!$I$9-Sheet1!$B$7</f>
-        <v>-97421.6</v>
+        <v>-104288.6</v>
       </c>
     </row>
     <row r="88" spans="1:2" s="7" customFormat="1">
@@ -16982,7 +17209,7 @@
       </c>
       <c r="B98" s="7">
         <f>Sheet1!$D$115*Sheet1!$I$9-Sheet1!$B$7</f>
-        <v>-97421.6</v>
+        <v>-104288.6</v>
       </c>
     </row>
     <row r="99" spans="1:2" s="7" customFormat="1">
@@ -17076,7 +17303,7 @@
       </c>
       <c r="B109" s="7">
         <f>Sheet1!$D$121*Sheet1!$I$9-Sheet1!$B$7</f>
-        <v>-97421.6</v>
+        <v>-104288.6</v>
       </c>
     </row>
     <row r="110" spans="1:2" s="7" customFormat="1">
@@ -17170,7 +17397,7 @@
       </c>
       <c r="B120" s="7">
         <f>Sheet1!$D$127*Sheet1!$I$9-Sheet1!$B$7</f>
-        <v>-97421.6</v>
+        <v>-104288.6</v>
       </c>
     </row>
     <row r="121" spans="1:2" s="7" customFormat="1">
@@ -17264,7 +17491,7 @@
       </c>
       <c r="B131" s="7">
         <f>Sheet1!$D$133*Sheet1!$I$9-Sheet1!$B$7</f>
-        <v>-97421.6</v>
+        <v>-104288.6</v>
       </c>
     </row>
     <row r="132" spans="1:2" s="7" customFormat="1">
@@ -17358,7 +17585,7 @@
       </c>
       <c r="B142" s="7">
         <f>Sheet1!$D$139*Sheet1!$I$9-Sheet1!$B$7</f>
-        <v>-97421.6</v>
+        <v>-104288.6</v>
       </c>
     </row>
     <row r="143" spans="1:2" s="7" customFormat="1">
@@ -17452,7 +17679,7 @@
       </c>
       <c r="B153" s="7">
         <f>Sheet1!$D$145*Sheet1!$I$9-Sheet1!$B$7</f>
-        <v>-97421.6</v>
+        <v>-104288.6</v>
       </c>
     </row>
     <row r="154" spans="1:2" s="7" customFormat="1">
@@ -17546,7 +17773,7 @@
       </c>
       <c r="B164" s="7">
         <f>Sheet1!$D$151*Sheet1!$I$9-Sheet1!$B$7</f>
-        <v>-97421.6</v>
+        <v>-104288.6</v>
       </c>
     </row>
     <row r="165" spans="1:2" s="7" customFormat="1">
@@ -17640,7 +17867,7 @@
       </c>
       <c r="B175" s="7">
         <f>Sheet1!$D$157*Sheet1!$I$9-Sheet1!$B$7</f>
-        <v>-97421.6</v>
+        <v>-104288.6</v>
       </c>
     </row>
     <row r="176" spans="1:2" s="7" customFormat="1">
@@ -17734,7 +17961,7 @@
       </c>
       <c r="B186" s="7">
         <f>Sheet1!$D$163*Sheet1!$I$9-Sheet1!$B$7</f>
-        <v>-97421.6</v>
+        <v>-104288.6</v>
       </c>
     </row>
     <row r="187" spans="1:2" s="7" customFormat="1">
@@ -17828,7 +18055,7 @@
       </c>
       <c r="B197" s="7">
         <f>Sheet1!$D$169*Sheet1!$I$9-Sheet1!$B$7</f>
-        <v>-97421.6</v>
+        <v>-104288.6</v>
       </c>
     </row>
     <row r="198" spans="1:2" s="7" customFormat="1">
@@ -17922,7 +18149,7 @@
       </c>
       <c r="B208" s="7">
         <f>Sheet1!$D$175*Sheet1!$I$9-Sheet1!$B$7</f>
-        <v>-97421.6</v>
+        <v>-104288.6</v>
       </c>
     </row>
     <row r="209" spans="1:2" s="7" customFormat="1">
@@ -18007,7 +18234,7 @@
       </c>
       <c r="B218" s="29">
         <f>Sheet1!$D$180*Sheet1!$I$9+Sheet1!I15*Sheet1!B32</f>
-        <v>-5.8993799762530816E-3</v>
+        <v>-3.5672144441197067E-6</v>
       </c>
     </row>
     <row r="219" spans="1:2" s="7" customFormat="1">
@@ -18016,7 +18243,7 @@
       </c>
       <c r="B219" s="7">
         <f>Sheet1!$D$181*Sheet1!$I$9-Sheet1!$B$7</f>
-        <v>-97421.6</v>
+        <v>-104288.6</v>
       </c>
     </row>
     <row r="220" spans="1:2" s="7" customFormat="1">
@@ -18049,7 +18276,7 @@
       </c>
       <c r="B223" s="29">
         <f>-(Sheet1!B29^2)*Sheet1!B32</f>
-        <v>-7.3113030030239835E-8</v>
+        <v>-4.4209706414415374E-11</v>
       </c>
     </row>
     <row r="224" spans="1:2" s="8" customFormat="1">
@@ -18058,7 +18285,7 @@
       </c>
       <c r="B224" s="8">
         <f>-B223</f>
-        <v>7.3113030030239835E-8</v>
+        <v>4.4209706414415374E-11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Began python code to create coefficient matrices.
</commit_message>
<xml_diff>
--- a/pipe/coefficients-20.xlsx
+++ b/pipe/coefficients-20.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15480" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2546,6 +2546,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2570,9 +2573,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="173">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -3078,8 +3078,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:DR181"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3099,23 +3099,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" s="8" customFormat="1">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="46" t="s">
         <v>472</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="45" t="s">
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="48" t="s">
         <v>494</v>
       </c>
-      <c r="I1" s="46"/>
-      <c r="J1" s="47"/>
-      <c r="L1" s="42"/>
-      <c r="M1" s="42"/>
-      <c r="N1" s="42"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="50"/>
+      <c r="L1" s="45"/>
+      <c r="M1" s="45"/>
+      <c r="N1" s="45"/>
     </row>
     <row r="2" spans="1:17">
       <c r="A2" t="s">
@@ -3400,7 +3400,7 @@
       </c>
       <c r="I13" s="7">
         <f>-I2*B19/(B27)^2</f>
-        <v>-408576</v>
+        <v>-259445.75999999998</v>
       </c>
       <c r="J13" s="17"/>
       <c r="N13">
@@ -3548,7 +3548,8 @@
         <v>478</v>
       </c>
       <c r="B19" s="37">
-        <v>0.04</v>
+        <f>E19*F19</f>
+        <v>2.5399999999999999E-2</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>13</v>
@@ -3557,7 +3558,7 @@
         <v>492</v>
       </c>
       <c r="E19" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F19" s="7">
         <v>1.2699999999999999E-2</v>
@@ -3676,7 +3677,7 @@
       <c r="A24" s="30" t="s">
         <v>482</v>
       </c>
-      <c r="B24" s="50">
+      <c r="B24" s="42">
         <v>2.6700000000000002E-2</v>
       </c>
       <c r="C24" s="7" t="s">
@@ -3709,7 +3710,7 @@
       <c r="A25" s="30" t="s">
         <v>483</v>
       </c>
-      <c r="B25" s="50">
+      <c r="B25" s="42">
         <v>1.07E-3</v>
       </c>
       <c r="C25" s="7" t="s">
@@ -3719,7 +3720,7 @@
       <c r="E25" s="7"/>
       <c r="F25" s="7"/>
       <c r="G25" s="17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K25" t="s">
         <v>661</v>
@@ -3742,7 +3743,7 @@
       <c r="A26" s="30" t="s">
         <v>484</v>
       </c>
-      <c r="B26" s="51">
+      <c r="B26" s="43">
         <v>1.5874999999999999E-3</v>
       </c>
       <c r="C26" s="7" t="s">
@@ -3771,7 +3772,7 @@
       <c r="A27" s="30" t="s">
         <v>485</v>
       </c>
-      <c r="B27" s="51">
+      <c r="B27" s="43">
         <v>5.0000000000000002E-5</v>
       </c>
       <c r="C27" s="7" t="s">
@@ -3786,11 +3787,11 @@
         <v>0</v>
       </c>
       <c r="H27" s="3"/>
-      <c r="I27" s="48" t="s">
+      <c r="I27" s="51" t="s">
         <v>663</v>
       </c>
-      <c r="J27" s="48"/>
-      <c r="K27" s="48"/>
+      <c r="J27" s="51"/>
+      <c r="K27" s="51"/>
       <c r="L27">
         <f>PI()*(B29/2)^2*L24</f>
         <v>1.4027839516809146E-6</v>
@@ -3800,7 +3801,7 @@
       <c r="A28" s="30" t="s">
         <v>486</v>
       </c>
-      <c r="B28" s="51">
+      <c r="B28" s="43">
         <v>1.5874999999999999E-3</v>
       </c>
       <c r="C28" s="7" t="s">
@@ -3904,7 +3905,7 @@
       </c>
       <c r="I34">
         <f ca="1">1+RAND()*F16*IF(RAND()&gt;0.5,1,-1)</f>
-        <v>0.97001962417764165</v>
+        <v>1.0428538990093279</v>
       </c>
     </row>
     <row r="35" spans="1:10">
@@ -3919,7 +3920,7 @@
       </c>
       <c r="I35">
         <f ca="1">ROUND(RAND(),0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:10">
@@ -4437,7 +4438,7 @@
       </c>
       <c r="C50" s="7">
         <f ca="1">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$25+($G$25=0))*($B$25*(C54=0)+C55*C54)</f>
-        <v>1.0132931837016947E-3</v>
+        <v>1.07E-3</v>
       </c>
       <c r="D50" s="7">
         <f ca="1">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$26+($G$26=0))*($B$26*(D54=0)+D55*D54)</f>
@@ -4461,7 +4462,7 @@
       </c>
       <c r="I50" s="7">
         <f t="shared" ref="I50" ca="1" si="1">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$25+($G$25=0))*($B$25*(I54=0)+I55*I54)</f>
-        <v>1.04547238076808E-3</v>
+        <v>1.07E-3</v>
       </c>
       <c r="J50" s="7">
         <f t="shared" ref="J50" ca="1" si="2">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$26+($G$26=0))*($B$26*(J54=0)+J55*J54)</f>
@@ -4485,7 +4486,7 @@
       </c>
       <c r="O50" s="7">
         <f t="shared" ref="O50" ca="1" si="7">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$25+($G$25=0))*($B$25*(O54=0)+O55*O54)</f>
-        <v>1.14697084130545E-3</v>
+        <v>1.07E-3</v>
       </c>
       <c r="P50" s="7">
         <f t="shared" ref="P50" ca="1" si="8">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$26+($G$26=0))*($B$26*(P54=0)+P55*P54)</f>
@@ -4509,7 +4510,7 @@
       </c>
       <c r="U50" s="7">
         <f t="shared" ref="U50" ca="1" si="13">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$25+($G$25=0))*($B$25*(U54=0)+U55*U54)</f>
-        <v>1.0053008831992312E-3</v>
+        <v>1.07E-3</v>
       </c>
       <c r="V50" s="7">
         <f t="shared" ref="V50" ca="1" si="14">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$26+($G$26=0))*($B$26*(V54=0)+V55*V54)</f>
@@ -4533,7 +4534,7 @@
       </c>
       <c r="AA50" s="7">
         <f t="shared" ref="AA50" ca="1" si="19">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$25+($G$25=0))*($B$25*(AA54=0)+AA55*AA54)</f>
-        <v>1.1390437858409337E-3</v>
+        <v>1.07E-3</v>
       </c>
       <c r="AB50" s="7">
         <f t="shared" ref="AB50" ca="1" si="20">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$26+($G$26=0))*($B$26*(AB54=0)+AB55*AB54)</f>
@@ -4557,7 +4558,7 @@
       </c>
       <c r="AG50" s="7">
         <f t="shared" ref="AG50" ca="1" si="25">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$25+($G$25=0))*($B$25*(AG54=0)+AG55*AG54)</f>
-        <v>1.1363563447508215E-3</v>
+        <v>1.07E-3</v>
       </c>
       <c r="AH50" s="7">
         <f t="shared" ref="AH50" ca="1" si="26">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$26+($G$26=0))*($B$26*(AH54=0)+AH55*AH54)</f>
@@ -4581,7 +4582,7 @@
       </c>
       <c r="AM50" s="7">
         <f t="shared" ref="AM50" ca="1" si="31">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$25+($G$25=0))*($B$25*(AM54=0)+AM55*AM54)</f>
-        <v>1.0721964361281471E-3</v>
+        <v>1.07E-3</v>
       </c>
       <c r="AN50" s="7">
         <f t="shared" ref="AN50" ca="1" si="32">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$26+($G$26=0))*($B$26*(AN54=0)+AN55*AN54)</f>
@@ -4605,7 +4606,7 @@
       </c>
       <c r="AS50" s="7">
         <f t="shared" ref="AS50" ca="1" si="37">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$25+($G$25=0))*($B$25*(AS54=0)+AS55*AS54)</f>
-        <v>1.1587075773091596E-3</v>
+        <v>1.07E-3</v>
       </c>
       <c r="AT50" s="7">
         <f t="shared" ref="AT50" ca="1" si="38">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$26+($G$26=0))*($B$26*(AT54=0)+AT55*AT54)</f>
@@ -4629,7 +4630,7 @@
       </c>
       <c r="AY50" s="7">
         <f t="shared" ref="AY50" ca="1" si="43">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$25+($G$25=0))*($B$25*(AY54=0)+AY55*AY54)</f>
-        <v>1.1230612666113054E-3</v>
+        <v>1.07E-3</v>
       </c>
       <c r="AZ50" s="7">
         <f t="shared" ref="AZ50" ca="1" si="44">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$26+($G$26=0))*($B$26*(AZ54=0)+AZ55*AZ54)</f>
@@ -4653,7 +4654,7 @@
       </c>
       <c r="BE50" s="7">
         <f t="shared" ref="BE50" ca="1" si="49">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$25+($G$25=0))*($B$25*(BE54=0)+BE55*BE54)</f>
-        <v>1.0783551780947306E-3</v>
+        <v>1.07E-3</v>
       </c>
       <c r="BF50" s="7">
         <f t="shared" ref="BF50" ca="1" si="50">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$26+($G$26=0))*($B$26*(BF54=0)+BF55*BF54)</f>
@@ -4677,7 +4678,7 @@
       </c>
       <c r="BK50" s="7">
         <f t="shared" ref="BK50" ca="1" si="55">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$25+($G$25=0))*($B$25*(BK54=0)+BK55*BK54)</f>
-        <v>1.0921251904780548E-3</v>
+        <v>1.07E-3</v>
       </c>
       <c r="BL50" s="7">
         <f t="shared" ref="BL50" ca="1" si="56">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$26+($G$26=0))*($B$26*(BL54=0)+BL55*BL54)</f>
@@ -4701,7 +4702,7 @@
       </c>
       <c r="BQ50" s="7">
         <f t="shared" ref="BQ50" ca="1" si="61">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$25+($G$25=0))*($B$25*(BQ54=0)+BQ55*BQ54)</f>
-        <v>1.0860134686701977E-3</v>
+        <v>1.07E-3</v>
       </c>
       <c r="BR50" s="7">
         <f t="shared" ref="BR50" ca="1" si="62">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$26+($G$26=0))*($B$26*(BR54=0)+BR55*BR54)</f>
@@ -4725,7 +4726,7 @@
       </c>
       <c r="BW50" s="7">
         <f t="shared" ref="BW50" ca="1" si="67">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$25+($G$25=0))*($B$25*(BW54=0)+BW55*BW54)</f>
-        <v>9.7340355605420991E-4</v>
+        <v>1.07E-3</v>
       </c>
       <c r="BX50" s="7">
         <f t="shared" ref="BX50" ca="1" si="68">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$26+($G$26=0))*($B$26*(BX54=0)+BX55*BX54)</f>
@@ -4749,7 +4750,7 @@
       </c>
       <c r="CC50" s="7">
         <f t="shared" ref="CC50" ca="1" si="73">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$25+($G$25=0))*($B$25*(CC54=0)+CC55*CC54)</f>
-        <v>1.0531067984056413E-3</v>
+        <v>1.07E-3</v>
       </c>
       <c r="CD50" s="7">
         <f t="shared" ref="CD50" ca="1" si="74">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$26+($G$26=0))*($B$26*(CD54=0)+CD55*CD54)</f>
@@ -4773,7 +4774,7 @@
       </c>
       <c r="CI50" s="7">
         <f t="shared" ref="CI50" ca="1" si="79">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$25+($G$25=0))*($B$25*(CI54=0)+CI55*CI54)</f>
-        <v>1.1325881693374721E-3</v>
+        <v>1.07E-3</v>
       </c>
       <c r="CJ50" s="7">
         <f t="shared" ref="CJ50" ca="1" si="80">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$26+($G$26=0))*($B$26*(CJ54=0)+CJ55*CJ54)</f>
@@ -4797,7 +4798,7 @@
       </c>
       <c r="CO50" s="7">
         <f t="shared" ref="CO50" ca="1" si="85">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$25+($G$25=0))*($B$25*(CO54=0)+CO55*CO54)</f>
-        <v>1.0897694899737397E-3</v>
+        <v>1.07E-3</v>
       </c>
       <c r="CP50" s="7">
         <f t="shared" ref="CP50" ca="1" si="86">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$26+($G$26=0))*($B$26*(CP54=0)+CP55*CP54)</f>
@@ -4821,7 +4822,7 @@
       </c>
       <c r="CU50" s="7">
         <f t="shared" ref="CU50" ca="1" si="91">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$25+($G$25=0))*($B$25*(CU54=0)+CU55*CU54)</f>
-        <v>1.1764177046115695E-3</v>
+        <v>1.07E-3</v>
       </c>
       <c r="CV50" s="7">
         <f t="shared" ref="CV50" ca="1" si="92">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$26+($G$26=0))*($B$26*(CV54=0)+CV55*CV54)</f>
@@ -4845,7 +4846,7 @@
       </c>
       <c r="DA50" s="7">
         <f t="shared" ref="DA50" ca="1" si="97">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$25+($G$25=0))*($B$25*(DA54=0)+DA55*DA54)</f>
-        <v>1.1111285960049319E-3</v>
+        <v>1.07E-3</v>
       </c>
       <c r="DB50" s="7">
         <f t="shared" ref="DB50" ca="1" si="98">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$26+($G$26=0))*($B$26*(DB54=0)+DB55*DB54)</f>
@@ -4869,7 +4870,7 @@
       </c>
       <c r="DG50" s="7">
         <f t="shared" ref="DG50" ca="1" si="103">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$25+($G$25=0))*($B$25*(DG54=0)+DG55*DG54)</f>
-        <v>9.8920378284400872E-4</v>
+        <v>1.07E-3</v>
       </c>
       <c r="DH50" s="7">
         <f t="shared" ref="DH50" ca="1" si="104">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$26+($G$26=0))*($B$26*(DH54=0)+DH55*DH54)</f>
@@ -4893,7 +4894,7 @@
       </c>
       <c r="DM50" s="7">
         <f t="shared" ref="DM50" ca="1" si="109">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$25+($G$25=0))*($B$25*(DM54=0)+DM55*DM54)</f>
-        <v>1.0277250861664569E-3</v>
+        <v>1.07E-3</v>
       </c>
       <c r="DN50" s="7">
         <f t="shared" ref="DN50" ca="1" si="110">((1+RAND()*$F$24*(RANDBETWEEN(0,1)*2-1))*$G$26+($G$26=0))*($B$26*(DN54=0)+DN55*DN54)</f>
@@ -4934,7 +4935,7 @@
       </c>
       <c r="E51" s="7">
         <f ca="1">(RAND()*$G$19+($G$19=0))*($B$19*(E57=0)+E58*E57)</f>
-        <v>0.04</v>
+        <v>2.5399999999999999E-2</v>
       </c>
       <c r="F51" s="7">
         <f ca="1">(RAND()*$G$20+($G$20=0))*($B$20*(F57=0)+F58*F57)</f>
@@ -4958,7 +4959,7 @@
       </c>
       <c r="K51" s="7">
         <f ca="1">(RAND()*$G$19+($G$19=0))*($B$19*(K57=0)+K58*K57)</f>
-        <v>0.04</v>
+        <v>2.5399999999999999E-2</v>
       </c>
       <c r="L51" s="7">
         <f ca="1">(RAND()*$G$20+($G$20=0))*($B$20*(L57=0)+L58*L57)</f>
@@ -4982,7 +4983,7 @@
       </c>
       <c r="Q51" s="7">
         <f ca="1">(RAND()*$G$19+($G$19=0))*($B$19*(Q57=0)+Q58*Q57)</f>
-        <v>0.04</v>
+        <v>2.5399999999999999E-2</v>
       </c>
       <c r="R51" s="7">
         <f ca="1">(RAND()*$G$20+($G$20=0))*($B$20*(R57=0)+R58*R57)</f>
@@ -5006,7 +5007,7 @@
       </c>
       <c r="W51" s="7">
         <f ca="1">(RAND()*$G$19+($G$19=0))*($B$19*(W57=0)+W58*W57)</f>
-        <v>0.04</v>
+        <v>2.5399999999999999E-2</v>
       </c>
       <c r="X51" s="7">
         <f ca="1">(RAND()*$G$20+($G$20=0))*($B$20*(X57=0)+X58*X57)</f>
@@ -5030,7 +5031,7 @@
       </c>
       <c r="AC51" s="7">
         <f ca="1">(RAND()*$G$19+($G$19=0))*($B$19*(AC57=0)+AC58*AC57)</f>
-        <v>0.04</v>
+        <v>2.5399999999999999E-2</v>
       </c>
       <c r="AD51" s="7">
         <f ca="1">(RAND()*$G$20+($G$20=0))*($B$20*(AD57=0)+AD58*AD57)</f>
@@ -5054,7 +5055,7 @@
       </c>
       <c r="AI51" s="7">
         <f ca="1">(RAND()*$G$19+($G$19=0))*($B$19*(AI57=0)+AI58*AI57)</f>
-        <v>0.04</v>
+        <v>2.5399999999999999E-2</v>
       </c>
       <c r="AJ51" s="7">
         <f ca="1">(RAND()*$G$20+($G$20=0))*($B$20*(AJ57=0)+AJ58*AJ57)</f>
@@ -5078,7 +5079,7 @@
       </c>
       <c r="AO51" s="7">
         <f ca="1">(RAND()*$G$19+($G$19=0))*($B$19*(AO57=0)+AO58*AO57)</f>
-        <v>0.04</v>
+        <v>2.5399999999999999E-2</v>
       </c>
       <c r="AP51" s="7">
         <f ca="1">(RAND()*$G$20+($G$20=0))*($B$20*(AP57=0)+AP58*AP57)</f>
@@ -5102,7 +5103,7 @@
       </c>
       <c r="AU51" s="7">
         <f ca="1">(RAND()*$G$19+($G$19=0))*($B$19*(AU57=0)+AU58*AU57)</f>
-        <v>0.04</v>
+        <v>2.5399999999999999E-2</v>
       </c>
       <c r="AV51" s="7">
         <f ca="1">(RAND()*$G$20+($G$20=0))*($B$20*(AV57=0)+AV58*AV57)</f>
@@ -5126,7 +5127,7 @@
       </c>
       <c r="BA51" s="7">
         <f ca="1">(RAND()*$G$19+($G$19=0))*($B$19*(BA57=0)+BA58*BA57)</f>
-        <v>0.04</v>
+        <v>2.5399999999999999E-2</v>
       </c>
       <c r="BB51" s="7">
         <f ca="1">(RAND()*$G$20+($G$20=0))*($B$20*(BB57=0)+BB58*BB57)</f>
@@ -5150,7 +5151,7 @@
       </c>
       <c r="BG51" s="7">
         <f ca="1">(RAND()*$G$19+($G$19=0))*($B$19*(BG57=0)+BG58*BG57)</f>
-        <v>0.04</v>
+        <v>2.5399999999999999E-2</v>
       </c>
       <c r="BH51" s="7">
         <f ca="1">(RAND()*$G$20+($G$20=0))*($B$20*(BH57=0)+BH58*BH57)</f>
@@ -5174,7 +5175,7 @@
       </c>
       <c r="BM51" s="7">
         <f ca="1">(RAND()*$G$19+($G$19=0))*($B$19*(BM57=0)+BM58*BM57)</f>
-        <v>0.04</v>
+        <v>2.5399999999999999E-2</v>
       </c>
       <c r="BN51" s="7">
         <f ca="1">(RAND()*$G$20+($G$20=0))*($B$20*(BN57=0)+BN58*BN57)</f>
@@ -5198,7 +5199,7 @@
       </c>
       <c r="BS51" s="7">
         <f ca="1">(RAND()*$G$19+($G$19=0))*($B$19*(BS57=0)+BS58*BS57)</f>
-        <v>0.04</v>
+        <v>2.5399999999999999E-2</v>
       </c>
       <c r="BT51" s="7">
         <f ca="1">(RAND()*$G$20+($G$20=0))*($B$20*(BT57=0)+BT58*BT57)</f>
@@ -5222,7 +5223,7 @@
       </c>
       <c r="BY51" s="7">
         <f ca="1">(RAND()*$G$19+($G$19=0))*($B$19*(BY57=0)+BY58*BY57)</f>
-        <v>0.04</v>
+        <v>2.5399999999999999E-2</v>
       </c>
       <c r="BZ51" s="7">
         <f ca="1">(RAND()*$G$20+($G$20=0))*($B$20*(BZ57=0)+BZ58*BZ57)</f>
@@ -5246,7 +5247,7 @@
       </c>
       <c r="CE51" s="7">
         <f ca="1">(RAND()*$G$19+($G$19=0))*($B$19*(CE57=0)+CE58*CE57)</f>
-        <v>0.04</v>
+        <v>2.5399999999999999E-2</v>
       </c>
       <c r="CF51" s="7">
         <f ca="1">(RAND()*$G$20+($G$20=0))*($B$20*(CF57=0)+CF58*CF57)</f>
@@ -5270,7 +5271,7 @@
       </c>
       <c r="CK51" s="7">
         <f ca="1">(RAND()*$G$19+($G$19=0))*($B$19*(CK57=0)+CK58*CK57)</f>
-        <v>0.04</v>
+        <v>2.5399999999999999E-2</v>
       </c>
       <c r="CL51" s="7">
         <f ca="1">(RAND()*$G$20+($G$20=0))*($B$20*(CL57=0)+CL58*CL57)</f>
@@ -5294,7 +5295,7 @@
       </c>
       <c r="CQ51" s="7">
         <f ca="1">(RAND()*$G$19+($G$19=0))*($B$19*(CQ57=0)+CQ58*CQ57)</f>
-        <v>0.04</v>
+        <v>2.5399999999999999E-2</v>
       </c>
       <c r="CR51" s="7">
         <f ca="1">(RAND()*$G$20+($G$20=0))*($B$20*(CR57=0)+CR58*CR57)</f>
@@ -5318,7 +5319,7 @@
       </c>
       <c r="CW51" s="7">
         <f ca="1">(RAND()*$G$19+($G$19=0))*($B$19*(CW57=0)+CW58*CW57)</f>
-        <v>0.04</v>
+        <v>2.5399999999999999E-2</v>
       </c>
       <c r="CX51" s="7">
         <f ca="1">(RAND()*$G$20+($G$20=0))*($B$20*(CX57=0)+CX58*CX57)</f>
@@ -5342,7 +5343,7 @@
       </c>
       <c r="DC51" s="7">
         <f ca="1">(RAND()*$G$19+($G$19=0))*($B$19*(DC57=0)+DC58*DC57)</f>
-        <v>0.04</v>
+        <v>2.5399999999999999E-2</v>
       </c>
       <c r="DD51" s="7">
         <f ca="1">(RAND()*$G$20+($G$20=0))*($B$20*(DD57=0)+DD58*DD57)</f>
@@ -5366,7 +5367,7 @@
       </c>
       <c r="DI51" s="7">
         <f ca="1">(RAND()*$G$19+($G$19=0))*($B$19*(DI57=0)+DI58*DI57)</f>
-        <v>0.04</v>
+        <v>2.5399999999999999E-2</v>
       </c>
       <c r="DJ51" s="7">
         <f ca="1">(RAND()*$G$20+($G$20=0))*($B$20*(DJ57=0)+DJ58*DJ57)</f>
@@ -5390,7 +5391,7 @@
       </c>
       <c r="DO51" s="7">
         <f ca="1">(RAND()*$G$19+($G$19=0))*($B$19*(DO57=0)+DO58*DO57)</f>
-        <v>0.04</v>
+        <v>2.5399999999999999E-2</v>
       </c>
       <c r="DP51" s="7">
         <f ca="1">(RAND()*$G$20+($G$20=0))*($B$20*(DP57=0)+DP58*DP57)</f>
@@ -5415,7 +5416,7 @@
       </c>
       <c r="C52" s="7">
         <f t="shared" ref="C52:H52" ca="1" si="115">-$I$2*C51/(C50^2)</f>
-        <v>-24.870391810437251</v>
+        <v>-22.304131365184734</v>
       </c>
       <c r="D52" s="7">
         <f t="shared" ca="1" si="115"/>
@@ -5423,7 +5424,7 @@
       </c>
       <c r="E52" s="7">
         <f t="shared" ca="1" si="115"/>
-        <v>-408576</v>
+        <v>-259445.75999999998</v>
       </c>
       <c r="F52" s="7">
         <f t="shared" ca="1" si="115"/>
@@ -5439,7 +5440,7 @@
       </c>
       <c r="I52" s="7">
         <f t="shared" ref="I52" ca="1" si="116">-$I$2*I51/(I50^2)</f>
-        <v>-23.362953328125098</v>
+        <v>-22.304131365184734</v>
       </c>
       <c r="J52" s="7">
         <f t="shared" ref="J52" ca="1" si="117">-$I$2*J51/(J50^2)</f>
@@ -5447,7 +5448,7 @@
       </c>
       <c r="K52" s="7">
         <f t="shared" ref="K52" ca="1" si="118">-$I$2*K51/(K50^2)</f>
-        <v>-408576</v>
+        <v>-259445.75999999998</v>
       </c>
       <c r="L52" s="7">
         <f t="shared" ref="L52" ca="1" si="119">-$I$2*L51/(L50^2)</f>
@@ -5463,7 +5464,7 @@
       </c>
       <c r="O52" s="7">
         <f t="shared" ref="O52" ca="1" si="122">-$I$2*O51/(O50^2)</f>
-        <v>-19.411009187973061</v>
+        <v>-22.304131365184734</v>
       </c>
       <c r="P52" s="7">
         <f t="shared" ref="P52" ca="1" si="123">-$I$2*P51/(P50^2)</f>
@@ -5471,7 +5472,7 @@
       </c>
       <c r="Q52" s="7">
         <f t="shared" ref="Q52" ca="1" si="124">-$I$2*Q51/(Q50^2)</f>
-        <v>-408576</v>
+        <v>-259445.75999999998</v>
       </c>
       <c r="R52" s="7">
         <f t="shared" ref="R52" ca="1" si="125">-$I$2*R51/(R50^2)</f>
@@ -5487,7 +5488,7 @@
       </c>
       <c r="U52" s="7">
         <f t="shared" ref="U52" ca="1" si="128">-$I$2*U51/(U50^2)</f>
-        <v>-25.267410814905617</v>
+        <v>-22.304131365184734</v>
       </c>
       <c r="V52" s="7">
         <f t="shared" ref="V52" ca="1" si="129">-$I$2*V51/(V50^2)</f>
@@ -5495,7 +5496,7 @@
       </c>
       <c r="W52" s="7">
         <f t="shared" ref="W52" ca="1" si="130">-$I$2*W51/(W50^2)</f>
-        <v>-408576</v>
+        <v>-259445.75999999998</v>
       </c>
       <c r="X52" s="7">
         <f t="shared" ref="X52" ca="1" si="131">-$I$2*X51/(X50^2)</f>
@@ -5511,7 +5512,7 @@
       </c>
       <c r="AA52" s="7">
         <f t="shared" ref="AA52" ca="1" si="134">-$I$2*AA51/(AA50^2)</f>
-        <v>-19.682127079817054</v>
+        <v>-22.304131365184734</v>
       </c>
       <c r="AB52" s="7">
         <f t="shared" ref="AB52" ca="1" si="135">-$I$2*AB51/(AB50^2)</f>
@@ -5519,7 +5520,7 @@
       </c>
       <c r="AC52" s="7">
         <f t="shared" ref="AC52" ca="1" si="136">-$I$2*AC51/(AC50^2)</f>
-        <v>-408576</v>
+        <v>-259445.75999999998</v>
       </c>
       <c r="AD52" s="7">
         <f t="shared" ref="AD52" ca="1" si="137">-$I$2*AD51/(AD50^2)</f>
@@ -5535,7 +5536,7 @@
       </c>
       <c r="AG52" s="7">
         <f t="shared" ref="AG52" ca="1" si="140">-$I$2*AG51/(AG50^2)</f>
-        <v>-19.775332180741152</v>
+        <v>-22.304131365184734</v>
       </c>
       <c r="AH52" s="7">
         <f t="shared" ref="AH52" ca="1" si="141">-$I$2*AH51/(AH50^2)</f>
@@ -5543,7 +5544,7 @@
       </c>
       <c r="AI52" s="7">
         <f t="shared" ref="AI52" ca="1" si="142">-$I$2*AI51/(AI50^2)</f>
-        <v>-408576</v>
+        <v>-259445.75999999998</v>
       </c>
       <c r="AJ52" s="7">
         <f t="shared" ref="AJ52" ca="1" si="143">-$I$2*AJ51/(AJ50^2)</f>
@@ -5559,7 +5560,7 @@
       </c>
       <c r="AM52" s="7">
         <f t="shared" ref="AM52" ca="1" si="146">-$I$2*AM51/(AM50^2)</f>
-        <v>-22.212843202423976</v>
+        <v>-22.304131365184734</v>
       </c>
       <c r="AN52" s="7">
         <f t="shared" ref="AN52" ca="1" si="147">-$I$2*AN51/(AN50^2)</f>
@@ -5567,7 +5568,7 @@
       </c>
       <c r="AO52" s="7">
         <f t="shared" ref="AO52" ca="1" si="148">-$I$2*AO51/(AO50^2)</f>
-        <v>-408576</v>
+        <v>-259445.75999999998</v>
       </c>
       <c r="AP52" s="7">
         <f t="shared" ref="AP52" ca="1" si="149">-$I$2*AP51/(AP50^2)</f>
@@ -5583,7 +5584,7 @@
       </c>
       <c r="AS52" s="7">
         <f t="shared" ref="AS52" ca="1" si="152">-$I$2*AS51/(AS50^2)</f>
-        <v>-19.019766267842776</v>
+        <v>-22.304131365184734</v>
       </c>
       <c r="AT52" s="7">
         <f t="shared" ref="AT52" ca="1" si="153">-$I$2*AT51/(AT50^2)</f>
@@ -5591,7 +5592,7 @@
       </c>
       <c r="AU52" s="7">
         <f t="shared" ref="AU52" ca="1" si="154">-$I$2*AU51/(AU50^2)</f>
-        <v>-408576</v>
+        <v>-259445.75999999998</v>
       </c>
       <c r="AV52" s="7">
         <f t="shared" ref="AV52" ca="1" si="155">-$I$2*AV51/(AV50^2)</f>
@@ -5607,7 +5608,7 @@
       </c>
       <c r="AY52" s="7">
         <f t="shared" ref="AY52" ca="1" si="158">-$I$2*AY51/(AY50^2)</f>
-        <v>-20.246314162794071</v>
+        <v>-22.304131365184734</v>
       </c>
       <c r="AZ52" s="7">
         <f t="shared" ref="AZ52" ca="1" si="159">-$I$2*AZ51/(AZ50^2)</f>
@@ -5615,7 +5616,7 @@
       </c>
       <c r="BA52" s="7">
         <f t="shared" ref="BA52" ca="1" si="160">-$I$2*BA51/(BA50^2)</f>
-        <v>-408576</v>
+        <v>-259445.75999999998</v>
       </c>
       <c r="BB52" s="7">
         <f t="shared" ref="BB52" ca="1" si="161">-$I$2*BB51/(BB50^2)</f>
@@ -5631,7 +5632,7 @@
       </c>
       <c r="BE52" s="7">
         <f t="shared" ref="BE52" ca="1" si="164">-$I$2*BE51/(BE50^2)</f>
-        <v>-21.959842123116314</v>
+        <v>-22.304131365184734</v>
       </c>
       <c r="BF52" s="7">
         <f t="shared" ref="BF52" ca="1" si="165">-$I$2*BF51/(BF50^2)</f>
@@ -5639,7 +5640,7 @@
       </c>
       <c r="BG52" s="7">
         <f t="shared" ref="BG52" ca="1" si="166">-$I$2*BG51/(BG50^2)</f>
-        <v>-408576</v>
+        <v>-259445.75999999998</v>
       </c>
       <c r="BH52" s="7">
         <f t="shared" ref="BH52" ca="1" si="167">-$I$2*BH51/(BH50^2)</f>
@@ -5655,7 +5656,7 @@
       </c>
       <c r="BK52" s="7">
         <f t="shared" ref="BK52" ca="1" si="170">-$I$2*BK51/(BK50^2)</f>
-        <v>-21.409573743403005</v>
+        <v>-22.304131365184734</v>
       </c>
       <c r="BL52" s="7">
         <f t="shared" ref="BL52" ca="1" si="171">-$I$2*BL51/(BL50^2)</f>
@@ -5663,7 +5664,7 @@
       </c>
       <c r="BM52" s="7">
         <f t="shared" ref="BM52" ca="1" si="172">-$I$2*BM51/(BM50^2)</f>
-        <v>-408576</v>
+        <v>-259445.75999999998</v>
       </c>
       <c r="BN52" s="7">
         <f t="shared" ref="BN52" ca="1" si="173">-$I$2*BN51/(BN50^2)</f>
@@ -5679,7 +5680,7 @@
       </c>
       <c r="BQ52" s="7">
         <f t="shared" ref="BQ52" ca="1" si="176">-$I$2*BQ51/(BQ50^2)</f>
-        <v>-21.651223687566361</v>
+        <v>-22.304131365184734</v>
       </c>
       <c r="BR52" s="7">
         <f t="shared" ref="BR52" ca="1" si="177">-$I$2*BR51/(BR50^2)</f>
@@ -5687,7 +5688,7 @@
       </c>
       <c r="BS52" s="7">
         <f t="shared" ref="BS52" ca="1" si="178">-$I$2*BS51/(BS50^2)</f>
-        <v>-408576</v>
+        <v>-259445.75999999998</v>
       </c>
       <c r="BT52" s="7">
         <f t="shared" ref="BT52" ca="1" si="179">-$I$2*BT51/(BT50^2)</f>
@@ -5703,7 +5704,7 @@
       </c>
       <c r="BW52" s="7">
         <f t="shared" ref="BW52" ca="1" si="182">-$I$2*BW51/(BW50^2)</f>
-        <v>-26.950511532861164</v>
+        <v>-22.304131365184734</v>
       </c>
       <c r="BX52" s="7">
         <f t="shared" ref="BX52" ca="1" si="183">-$I$2*BX51/(BX50^2)</f>
@@ -5711,7 +5712,7 @@
       </c>
       <c r="BY52" s="7">
         <f t="shared" ref="BY52" ca="1" si="184">-$I$2*BY51/(BY50^2)</f>
-        <v>-408576</v>
+        <v>-259445.75999999998</v>
       </c>
       <c r="BZ52" s="7">
         <f t="shared" ref="BZ52" ca="1" si="185">-$I$2*BZ51/(BZ50^2)</f>
@@ -5727,7 +5728,7 @@
       </c>
       <c r="CC52" s="7">
         <f t="shared" ref="CC52" ca="1" si="188">-$I$2*CC51/(CC50^2)</f>
-        <v>-23.025445241807134</v>
+        <v>-22.304131365184734</v>
       </c>
       <c r="CD52" s="7">
         <f t="shared" ref="CD52" ca="1" si="189">-$I$2*CD51/(CD50^2)</f>
@@ -5735,7 +5736,7 @@
       </c>
       <c r="CE52" s="7">
         <f t="shared" ref="CE52" ca="1" si="190">-$I$2*CE51/(CE50^2)</f>
-        <v>-408576</v>
+        <v>-259445.75999999998</v>
       </c>
       <c r="CF52" s="7">
         <f t="shared" ref="CF52" ca="1" si="191">-$I$2*CF51/(CF50^2)</f>
@@ -5751,7 +5752,7 @@
       </c>
       <c r="CI52" s="7">
         <f t="shared" ref="CI52" ca="1" si="194">-$I$2*CI51/(CI50^2)</f>
-        <v>-19.907138044916</v>
+        <v>-22.304131365184734</v>
       </c>
       <c r="CJ52" s="7">
         <f t="shared" ref="CJ52" ca="1" si="195">-$I$2*CJ51/(CJ50^2)</f>
@@ -5759,7 +5760,7 @@
       </c>
       <c r="CK52" s="7">
         <f t="shared" ref="CK52" ca="1" si="196">-$I$2*CK51/(CK50^2)</f>
-        <v>-408576</v>
+        <v>-259445.75999999998</v>
       </c>
       <c r="CL52" s="7">
         <f t="shared" ref="CL52" ca="1" si="197">-$I$2*CL51/(CL50^2)</f>
@@ -5775,7 +5776,7 @@
       </c>
       <c r="CO52" s="7">
         <f t="shared" ref="CO52" ca="1" si="200">-$I$2*CO51/(CO50^2)</f>
-        <v>-21.502233806014971</v>
+        <v>-22.304131365184734</v>
       </c>
       <c r="CP52" s="7">
         <f t="shared" ref="CP52" ca="1" si="201">-$I$2*CP51/(CP50^2)</f>
@@ -5783,7 +5784,7 @@
       </c>
       <c r="CQ52" s="7">
         <f t="shared" ref="CQ52" ca="1" si="202">-$I$2*CQ51/(CQ50^2)</f>
-        <v>-408576</v>
+        <v>-259445.75999999998</v>
       </c>
       <c r="CR52" s="7">
         <f t="shared" ref="CR52" ca="1" si="203">-$I$2*CR51/(CR50^2)</f>
@@ -5799,7 +5800,7 @@
       </c>
       <c r="CU52" s="7">
         <f t="shared" ref="CU52" ca="1" si="206">-$I$2*CU51/(CU50^2)</f>
-        <v>-18.451418785127039</v>
+        <v>-22.304131365184734</v>
       </c>
       <c r="CV52" s="7">
         <f t="shared" ref="CV52" ca="1" si="207">-$I$2*CV51/(CV50^2)</f>
@@ -5807,7 +5808,7 @@
       </c>
       <c r="CW52" s="7">
         <f t="shared" ref="CW52" ca="1" si="208">-$I$2*CW51/(CW50^2)</f>
-        <v>-408576</v>
+        <v>-259445.75999999998</v>
       </c>
       <c r="CX52" s="7">
         <f t="shared" ref="CX52" ca="1" si="209">-$I$2*CX51/(CX50^2)</f>
@@ -5823,7 +5824,7 @@
       </c>
       <c r="DA52" s="7">
         <f t="shared" ref="DA52" ca="1" si="212">-$I$2*DA51/(DA50^2)</f>
-        <v>-20.68350902675154</v>
+        <v>-22.304131365184734</v>
       </c>
       <c r="DB52" s="7">
         <f t="shared" ref="DB52" ca="1" si="213">-$I$2*DB51/(DB50^2)</f>
@@ -5831,7 +5832,7 @@
       </c>
       <c r="DC52" s="7">
         <f t="shared" ref="DC52" ca="1" si="214">-$I$2*DC51/(DC50^2)</f>
-        <v>-408576</v>
+        <v>-259445.75999999998</v>
       </c>
       <c r="DD52" s="7">
         <f t="shared" ref="DD52" ca="1" si="215">-$I$2*DD51/(DD50^2)</f>
@@ -5847,7 +5848,7 @@
       </c>
       <c r="DG52" s="7">
         <f t="shared" ref="DG52" ca="1" si="218">-$I$2*DG51/(DG50^2)</f>
-        <v>-26.096443995473098</v>
+        <v>-22.304131365184734</v>
       </c>
       <c r="DH52" s="7">
         <f t="shared" ref="DH52" ca="1" si="219">-$I$2*DH51/(DH50^2)</f>
@@ -5855,7 +5856,7 @@
       </c>
       <c r="DI52" s="7">
         <f t="shared" ref="DI52" ca="1" si="220">-$I$2*DI51/(DI50^2)</f>
-        <v>-408576</v>
+        <v>-259445.75999999998</v>
       </c>
       <c r="DJ52" s="7">
         <f t="shared" ref="DJ52" ca="1" si="221">-$I$2*DJ51/(DJ50^2)</f>
@@ -5871,7 +5872,7 @@
       </c>
       <c r="DM52" s="7">
         <f t="shared" ref="DM52" ca="1" si="224">-$I$2*DM51/(DM50^2)</f>
-        <v>-24.17680761317207</v>
+        <v>-22.304131365184734</v>
       </c>
       <c r="DN52" s="7">
         <f t="shared" ref="DN52" ca="1" si="225">-$I$2*DN51/(DN50^2)</f>
@@ -5879,7 +5880,7 @@
       </c>
       <c r="DO52" s="7">
         <f t="shared" ref="DO52" ca="1" si="226">-$I$2*DO51/(DO50^2)</f>
-        <v>-408576</v>
+        <v>-259445.75999999998</v>
       </c>
       <c r="DP52" s="7">
         <f t="shared" ref="DP52" ca="1" si="227">-$I$2*DP51/(DP50^2)</f>
@@ -9294,7 +9295,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:HQ370"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="CY1" workbookViewId="0">
       <selection activeCell="CZ4" sqref="CZ4"/>
     </sheetView>
   </sheetViews>
@@ -9319,10 +9320,10 @@
       </c>
       <c r="HM1" s="5"/>
       <c r="HN1" s="5"/>
-      <c r="HP1" s="49" t="s">
+      <c r="HP1" s="52" t="s">
         <v>641</v>
       </c>
-      <c r="HQ1" s="49"/>
+      <c r="HQ1" s="52"/>
     </row>
     <row r="2" spans="1:225">
       <c r="A2" s="24"/>
@@ -10016,83 +10017,83 @@
       </c>
       <c r="CZ4">
         <f ca="1">-(Sheet1!C50^2)</f>
-        <v>-1.0267630761363164E-6</v>
+        <v>-1.1449E-6</v>
       </c>
       <c r="DF4">
         <f ca="1">-(Sheet1!I50^2)</f>
-        <v>-1.0930124989488772E-6</v>
+        <v>-1.1449E-6</v>
       </c>
       <c r="DL4">
         <f ca="1">-(Sheet1!O50^2)</f>
-        <v>-1.3155421108049316E-6</v>
+        <v>-1.1449E-6</v>
       </c>
       <c r="DR4">
         <f ca="1">-(Sheet1!U50^2)</f>
-        <v>-1.0106298657611543E-6</v>
+        <v>-1.1449E-6</v>
       </c>
       <c r="DX4">
         <f ca="1">-(Sheet1!AA50^2)</f>
-        <v>-1.2974207460628468E-6</v>
+        <v>-1.1449E-6</v>
       </c>
       <c r="ED4">
         <f ca="1">-(Sheet1!AG50^2)</f>
-        <v>-1.2913057422554479E-6</v>
+        <v>-1.1449E-6</v>
       </c>
       <c r="EJ4">
         <f ca="1">-(Sheet1!AM50^2)</f>
-        <v>-1.1496051976459E-6</v>
+        <v>-1.1449E-6</v>
       </c>
       <c r="EP4">
         <f ca="1">-(Sheet1!AS50^2)</f>
-        <v>-1.342603249713662E-6</v>
+        <v>-1.1449E-6</v>
       </c>
       <c r="EV4">
         <f ca="1">-(Sheet1!AY50^2)</f>
-        <v>-1.2612666085625894E-6</v>
+        <v>-1.1449E-6</v>
       </c>
       <c r="FB4">
         <f ca="1">-(Sheet1!BE50^2)</f>
-        <v>-1.1628498901237181E-6</v>
+        <v>-1.1449E-6</v>
       </c>
       <c r="FH4">
         <f ca="1">-(Sheet1!BK50^2)</f>
-        <v>-1.1927374316767274E-6</v>
+        <v>-1.1449E-6</v>
       </c>
       <c r="FN4">
         <f ca="1">-(Sheet1!BQ50^2)</f>
-        <v>-1.1794252541330746E-6</v>
+        <v>-1.1449E-6</v>
       </c>
       <c r="FT4">
         <f ca="1">-(Sheet1!BW50^2)</f>
-        <v>-9.4751448293898139E-7</v>
+        <v>-1.1449E-6</v>
       </c>
       <c r="FZ4">
         <f ca="1">-(Sheet1!CC50^2)</f>
-        <v>-1.1090339288481802E-6</v>
+        <v>-1.1449E-6</v>
       </c>
       <c r="GF4">
         <f ca="1">-(Sheet1!CI50^2)</f>
-        <v>-1.2827559613232064E-6</v>
+        <v>-1.1449E-6</v>
       </c>
       <c r="GL4">
         <f ca="1">-(Sheet1!CO50^2)</f>
-        <v>-1.1875975412776247E-6</v>
+        <v>-1.1449E-6</v>
       </c>
       <c r="GR4">
         <f ca="1">-(Sheet1!CU50^2)</f>
-        <v>-1.3839586157235541E-6</v>
+        <v>-1.1449E-6</v>
       </c>
       <c r="GX4">
         <f ca="1">-(Sheet1!DA50^2)</f>
-        <v>-1.2346067568598911E-6</v>
+        <v>-1.1449E-6</v>
       </c>
       <c r="HD4">
         <f ca="1">-(Sheet1!DG50^2)</f>
-        <v>-9.7852412399289666E-7</v>
+        <v>-1.1449E-6</v>
       </c>
       <c r="HJ4">
         <f ca="1">-(Sheet1!DM50^2)</f>
-        <v>-1.0562188527358513E-6</v>
+        <v>-1.1449E-6</v>
       </c>
     </row>
     <row r="5" spans="1:225" s="6" customFormat="1">
@@ -10107,7 +10108,7 @@
       </c>
       <c r="CZ5" s="6">
         <f ca="1">Sheet1!C$52</f>
-        <v>-24.870391810437251</v>
+        <v>-22.304131365184734</v>
       </c>
     </row>
     <row r="6" spans="1:225">
@@ -10137,7 +10138,7 @@
       </c>
       <c r="DB7">
         <f ca="1">Sheet1!E$52</f>
-        <v>-408576</v>
+        <v>-259445.75999999998</v>
       </c>
     </row>
     <row r="8" spans="1:225">
@@ -10188,7 +10189,7 @@
       </c>
       <c r="CZ11">
         <f ca="1">(Sheet1!C$50^2)</f>
-        <v>1.0267630761363164E-6</v>
+        <v>1.1449E-6</v>
       </c>
       <c r="DA11">
         <f ca="1">-(Sheet1!D$50^2)</f>
@@ -10259,7 +10260,7 @@
       </c>
       <c r="DF16" s="6">
         <f ca="1">Sheet1!I$52</f>
-        <v>-23.362953328125098</v>
+        <v>-22.304131365184734</v>
       </c>
     </row>
     <row r="17" spans="1:121">
@@ -10289,7 +10290,7 @@
       </c>
       <c r="DH18">
         <f ca="1">Sheet1!K$52</f>
-        <v>-408576</v>
+        <v>-259445.75999999998</v>
       </c>
     </row>
     <row r="19" spans="1:121">
@@ -10340,7 +10341,7 @@
       </c>
       <c r="DF22">
         <f ca="1">(Sheet1!I$50^2)</f>
-        <v>1.0930124989488772E-6</v>
+        <v>1.1449E-6</v>
       </c>
       <c r="DG22">
         <f ca="1">-(Sheet1!J$50^2)</f>
@@ -10411,7 +10412,7 @@
       </c>
       <c r="DL27" s="6">
         <f ca="1">Sheet1!O$52</f>
-        <v>-19.411009187973061</v>
+        <v>-22.304131365184734</v>
       </c>
     </row>
     <row r="28" spans="1:121">
@@ -10441,7 +10442,7 @@
       </c>
       <c r="DN29">
         <f ca="1">Sheet1!Q$52</f>
-        <v>-408576</v>
+        <v>-259445.75999999998</v>
       </c>
     </row>
     <row r="30" spans="1:121">
@@ -10497,7 +10498,7 @@
       <c r="L33" s="4"/>
       <c r="DL33">
         <f ca="1">(Sheet1!O$50^2)</f>
-        <v>1.3155421108049316E-6</v>
+        <v>1.1449E-6</v>
       </c>
       <c r="DM33">
         <f ca="1">-(Sheet1!P$50^2)</f>
@@ -10588,7 +10589,7 @@
       </c>
       <c r="DR38" s="6">
         <f ca="1">Sheet1!U$52</f>
-        <v>-25.267410814905617</v>
+        <v>-22.304131365184734</v>
       </c>
     </row>
     <row r="39" spans="1:127">
@@ -10618,7 +10619,7 @@
       </c>
       <c r="DT40">
         <f ca="1">Sheet1!W$52</f>
-        <v>-408576</v>
+        <v>-259445.75999999998</v>
       </c>
     </row>
     <row r="41" spans="1:127">
@@ -10684,7 +10685,7 @@
       <c r="Q44" s="4"/>
       <c r="DR44">
         <f ca="1">(Sheet1!U$50^2)</f>
-        <v>1.0106298657611543E-6</v>
+        <v>1.1449E-6</v>
       </c>
       <c r="DS44">
         <f ca="1">-(Sheet1!V$50^2)</f>
@@ -10765,7 +10766,7 @@
       </c>
       <c r="DX49" s="6">
         <f ca="1">Sheet1!AA$52</f>
-        <v>-19.682127079817054</v>
+        <v>-22.304131365184734</v>
       </c>
     </row>
     <row r="50" spans="1:138">
@@ -10800,7 +10801,7 @@
       </c>
       <c r="DZ51">
         <f ca="1">Sheet1!AC$52</f>
-        <v>-408576</v>
+        <v>-259445.75999999998</v>
       </c>
     </row>
     <row r="52" spans="1:138">
@@ -10871,7 +10872,7 @@
       <c r="V55" s="4"/>
       <c r="DX55">
         <f ca="1">(Sheet1!AA$50^2)</f>
-        <v>1.2974207460628468E-6</v>
+        <v>1.1449E-6</v>
       </c>
       <c r="DY55">
         <f ca="1">-(Sheet1!AB$50^2)</f>
@@ -10947,7 +10948,7 @@
       </c>
       <c r="ED60" s="6">
         <f ca="1">Sheet1!AG$52</f>
-        <v>-19.775332180741152</v>
+        <v>-22.304131365184734</v>
       </c>
     </row>
     <row r="61" spans="1:138">
@@ -10987,7 +10988,7 @@
       </c>
       <c r="EF62">
         <f ca="1">Sheet1!AI$52</f>
-        <v>-408576</v>
+        <v>-259445.75999999998</v>
       </c>
     </row>
     <row r="63" spans="1:138">
@@ -11048,7 +11049,7 @@
       </c>
       <c r="ED66">
         <f ca="1">(Sheet1!AG$50^2)</f>
-        <v>1.2913057422554479E-6</v>
+        <v>1.1449E-6</v>
       </c>
       <c r="EE66">
         <f ca="1">-(Sheet1!AH$50^2)</f>
@@ -11137,7 +11138,7 @@
       </c>
       <c r="EJ71" s="6">
         <f ca="1">Sheet1!AM$52</f>
-        <v>-22.212843202423976</v>
+        <v>-22.304131365184734</v>
       </c>
     </row>
     <row r="72" spans="1:145">
@@ -11179,7 +11180,7 @@
       </c>
       <c r="EL73">
         <f ca="1">Sheet1!AO$52</f>
-        <v>-408576</v>
+        <v>-259445.75999999998</v>
       </c>
     </row>
     <row r="74" spans="1:145">
@@ -11230,7 +11231,7 @@
       </c>
       <c r="EJ77">
         <f ca="1">(Sheet1!AM$50^2)</f>
-        <v>1.1496051976459E-6</v>
+        <v>1.1449E-6</v>
       </c>
       <c r="EK77">
         <f ca="1">-(Sheet1!AN$50^2)</f>
@@ -11326,7 +11327,7 @@
       </c>
       <c r="EP82" s="6">
         <f ca="1">Sheet1!AS$52</f>
-        <v>-19.019766267842776</v>
+        <v>-22.304131365184734</v>
       </c>
     </row>
     <row r="83" spans="1:155">
@@ -11356,7 +11357,7 @@
       </c>
       <c r="ER84">
         <f ca="1">Sheet1!AU$52</f>
-        <v>-408576</v>
+        <v>-259445.75999999998</v>
       </c>
     </row>
     <row r="85" spans="1:155">
@@ -11413,7 +11414,7 @@
       <c r="AP88" s="4"/>
       <c r="EP88">
         <f ca="1">(Sheet1!AS$50^2)</f>
-        <v>1.342603249713662E-6</v>
+        <v>1.1449E-6</v>
       </c>
       <c r="EQ88">
         <f ca="1">-(Sheet1!AT$50^2)</f>
@@ -11499,7 +11500,7 @@
       </c>
       <c r="EV93" s="6">
         <f ca="1">Sheet1!AY$52</f>
-        <v>-20.246314162794071</v>
+        <v>-22.304131365184734</v>
       </c>
     </row>
     <row r="94" spans="1:155">
@@ -11529,7 +11530,7 @@
       </c>
       <c r="EX95">
         <f ca="1">Sheet1!BA$52</f>
-        <v>-408576</v>
+        <v>-259445.75999999998</v>
       </c>
     </row>
     <row r="96" spans="1:155">
@@ -11588,7 +11589,7 @@
       <c r="AU99" s="4"/>
       <c r="EV99">
         <f ca="1">(Sheet1!AY$50^2)</f>
-        <v>1.2612666085625894E-6</v>
+        <v>1.1449E-6</v>
       </c>
       <c r="EW99">
         <f ca="1">-(Sheet1!AZ$50^2)</f>
@@ -11664,7 +11665,7 @@
       </c>
       <c r="FB104" s="6">
         <f ca="1">Sheet1!BE$52</f>
-        <v>-21.959842123116314</v>
+        <v>-22.304131365184734</v>
       </c>
     </row>
     <row r="105" spans="1:163">
@@ -11696,7 +11697,7 @@
       </c>
       <c r="FD106">
         <f ca="1">Sheet1!BG$52</f>
-        <v>-408576</v>
+        <v>-259445.75999999998</v>
       </c>
     </row>
     <row r="107" spans="1:163">
@@ -11750,7 +11751,7 @@
       </c>
       <c r="FB110">
         <f ca="1">(Sheet1!BE$50^2)</f>
-        <v>1.1628498901237181E-6</v>
+        <v>1.1449E-6</v>
       </c>
       <c r="FC110">
         <f ca="1">-(Sheet1!BF$50^2)</f>
@@ -11827,7 +11828,7 @@
       </c>
       <c r="FH115" s="6">
         <f ca="1">Sheet1!BK$52</f>
-        <v>-21.409573743403005</v>
+        <v>-22.304131365184734</v>
       </c>
     </row>
     <row r="116" spans="1:172">
@@ -11859,7 +11860,7 @@
       </c>
       <c r="FJ117">
         <f ca="1">Sheet1!BM$52</f>
-        <v>-408576</v>
+        <v>-259445.75999999998</v>
       </c>
     </row>
     <row r="118" spans="1:172">
@@ -11911,7 +11912,7 @@
       </c>
       <c r="FH121">
         <f ca="1">(Sheet1!BK$50^2)</f>
-        <v>1.1927374316767274E-6</v>
+        <v>1.1449E-6</v>
       </c>
       <c r="FI121">
         <f ca="1">-(Sheet1!BL$50^2)</f>
@@ -12002,7 +12003,7 @@
       </c>
       <c r="FN126" s="6">
         <f ca="1">Sheet1!BQ$52</f>
-        <v>-21.651223687566361</v>
+        <v>-22.304131365184734</v>
       </c>
     </row>
     <row r="127" spans="1:172">
@@ -12034,7 +12035,7 @@
       </c>
       <c r="FP128">
         <f ca="1">Sheet1!BS$52</f>
-        <v>-408576</v>
+        <v>-259445.75999999998</v>
       </c>
     </row>
     <row r="129" spans="1:181">
@@ -12090,7 +12091,7 @@
       <c r="BO132" s="4"/>
       <c r="FN132">
         <f ca="1">(Sheet1!BQ$50^2)</f>
-        <v>1.1794252541330746E-6</v>
+        <v>1.1449E-6</v>
       </c>
       <c r="FO132">
         <f ca="1">-(Sheet1!BR$50^2)</f>
@@ -12181,7 +12182,7 @@
       </c>
       <c r="FT137" s="6">
         <f ca="1">Sheet1!BW$52</f>
-        <v>-26.950511532861164</v>
+        <v>-22.304131365184734</v>
       </c>
     </row>
     <row r="138" spans="1:181">
@@ -12211,7 +12212,7 @@
       </c>
       <c r="FV139">
         <f ca="1">Sheet1!BY$52</f>
-        <v>-408576</v>
+        <v>-259445.75999999998</v>
       </c>
     </row>
     <row r="140" spans="1:181">
@@ -12275,7 +12276,7 @@
       <c r="BT143" s="4"/>
       <c r="FT143">
         <f ca="1">(Sheet1!BW$50^2)</f>
-        <v>9.4751448293898139E-7</v>
+        <v>1.1449E-6</v>
       </c>
       <c r="FU143">
         <f ca="1">-(Sheet1!BX$50^2)</f>
@@ -12356,7 +12357,7 @@
       </c>
       <c r="FZ148" s="6">
         <f ca="1">Sheet1!CC$52</f>
-        <v>-23.025445241807134</v>
+        <v>-22.304131365184734</v>
       </c>
     </row>
     <row r="149" spans="1:189">
@@ -12390,7 +12391,7 @@
       <c r="BY150" s="4"/>
       <c r="GB150">
         <f ca="1">Sheet1!CE$52</f>
-        <v>-408576</v>
+        <v>-259445.75999999998</v>
       </c>
     </row>
     <row r="151" spans="1:189">
@@ -12458,7 +12459,7 @@
       <c r="BY154" s="4"/>
       <c r="FZ154">
         <f ca="1">(Sheet1!CC$50^2)</f>
-        <v>1.1090339288481802E-6</v>
+        <v>1.1449E-6</v>
       </c>
       <c r="GA154">
         <f ca="1">-(Sheet1!CD$50^2)</f>
@@ -12533,7 +12534,7 @@
       <c r="CD159" s="22"/>
       <c r="GF159" s="6">
         <f ca="1">Sheet1!CI$52</f>
-        <v>-19.907138044916</v>
+        <v>-22.304131365184734</v>
       </c>
     </row>
     <row r="160" spans="1:189">
@@ -12571,7 +12572,7 @@
       <c r="CD161" s="4"/>
       <c r="GH161">
         <f ca="1">Sheet1!CK$52</f>
-        <v>-408576</v>
+        <v>-259445.75999999998</v>
       </c>
     </row>
     <row r="162" spans="1:199">
@@ -12630,7 +12631,7 @@
       </c>
       <c r="GF165">
         <f ca="1">(Sheet1!CI$50^2)</f>
-        <v>1.2827559613232064E-6</v>
+        <v>1.1449E-6</v>
       </c>
       <c r="GG165">
         <f ca="1">-(Sheet1!CJ$50^2)</f>
@@ -12715,7 +12716,7 @@
       <c r="CI170" s="22"/>
       <c r="GL170" s="6">
         <f ca="1">Sheet1!CO$52</f>
-        <v>-21.502233806014971</v>
+        <v>-22.304131365184734</v>
       </c>
     </row>
     <row r="171" spans="1:199">
@@ -12753,7 +12754,7 @@
       <c r="CI172" s="4"/>
       <c r="GN172">
         <f ca="1">Sheet1!CQ$52</f>
-        <v>-408576</v>
+        <v>-259445.75999999998</v>
       </c>
     </row>
     <row r="173" spans="1:199">
@@ -12804,7 +12805,7 @@
       </c>
       <c r="GL176">
         <f ca="1">(Sheet1!CO$50^2)</f>
-        <v>1.1875975412776247E-6</v>
+        <v>1.1449E-6</v>
       </c>
       <c r="GM176">
         <f ca="1">-(Sheet1!CP$50^2)</f>
@@ -12899,7 +12900,7 @@
       <c r="CN181" s="22"/>
       <c r="GR181" s="6">
         <f ca="1">Sheet1!CU$52</f>
-        <v>-18.451418785127039</v>
+        <v>-22.304131365184734</v>
       </c>
     </row>
     <row r="182" spans="1:206">
@@ -12929,7 +12930,7 @@
       </c>
       <c r="GT183">
         <f ca="1">Sheet1!CW$52</f>
-        <v>-408576</v>
+        <v>-259445.75999999998</v>
       </c>
     </row>
     <row r="184" spans="1:206">
@@ -12990,7 +12991,7 @@
       <c r="CS187" s="4"/>
       <c r="GR187">
         <f ca="1">(Sheet1!CU$50^2)</f>
-        <v>1.3839586157235541E-6</v>
+        <v>1.1449E-6</v>
       </c>
       <c r="GS187">
         <f ca="1">-(Sheet1!CV$50^2)</f>
@@ -13076,7 +13077,7 @@
       </c>
       <c r="GX192" s="6">
         <f ca="1">Sheet1!DA$52</f>
-        <v>-20.68350902675154</v>
+        <v>-22.304131365184734</v>
       </c>
     </row>
     <row r="193" spans="1:217">
@@ -13106,7 +13107,7 @@
       </c>
       <c r="GZ194">
         <f ca="1">Sheet1!DC$52</f>
-        <v>-408576</v>
+        <v>-259445.75999999998</v>
       </c>
     </row>
     <row r="195" spans="1:217">
@@ -13177,7 +13178,7 @@
       <c r="CX198" s="4"/>
       <c r="GX198">
         <f ca="1">(Sheet1!DA$50^2)</f>
-        <v>1.2346067568598911E-6</v>
+        <v>1.1449E-6</v>
       </c>
       <c r="GY198">
         <f ca="1">-(Sheet1!DB$50^2)</f>
@@ -13253,7 +13254,7 @@
       </c>
       <c r="HD203" s="6">
         <f ca="1">Sheet1!DG$52</f>
-        <v>-26.096443995473098</v>
+        <v>-22.304131365184734</v>
       </c>
     </row>
     <row r="204" spans="1:217">
@@ -13283,7 +13284,7 @@
       </c>
       <c r="HF205">
         <f ca="1">Sheet1!DI$52</f>
-        <v>-408576</v>
+        <v>-259445.75999999998</v>
       </c>
     </row>
     <row r="206" spans="1:217">
@@ -13334,7 +13335,7 @@
       </c>
       <c r="HD209">
         <f ca="1">(Sheet1!DG$50^2)</f>
-        <v>9.7852412399289666E-7</v>
+        <v>1.1449E-6</v>
       </c>
       <c r="HE209">
         <f ca="1">-(Sheet1!DH$50^2)</f>
@@ -13405,7 +13406,7 @@
       </c>
       <c r="HJ214" s="6">
         <f ca="1">Sheet1!DM$52</f>
-        <v>-24.17680761317207</v>
+        <v>-22.304131365184734</v>
       </c>
       <c r="HO214" s="22"/>
     </row>
@@ -13443,7 +13444,7 @@
       <c r="HK216" s="7"/>
       <c r="HL216" s="7">
         <f ca="1">Sheet1!DO$52</f>
-        <v>-408576</v>
+        <v>-259445.75999999998</v>
       </c>
       <c r="HM216" s="7"/>
       <c r="HN216" s="7"/>
@@ -13512,7 +13513,7 @@
       </c>
       <c r="HJ220" s="7">
         <f ca="1">(Sheet1!DM$50^2)</f>
-        <v>1.0562188527358513E-6</v>
+        <v>1.1449E-6</v>
       </c>
       <c r="HK220" s="7">
         <f ca="1">-(Sheet1!DN$50^2)</f>
@@ -14039,7 +14040,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:HO224"/>
   <sheetViews>
-    <sheetView topLeftCell="CR1" workbookViewId="0">
+    <sheetView topLeftCell="HA1" workbookViewId="0">
       <selection activeCell="HN3" sqref="HN3"/>
     </sheetView>
   </sheetViews>
@@ -18277,7 +18278,7 @@
       <c r="A218" s="15" t="s">
         <v>404</v>
       </c>
-      <c r="B218" s="52">
+      <c r="B218" s="44">
         <f>Sheet1!$D$180*Sheet1!$I$9</f>
         <v>0</v>
       </c>
@@ -18319,7 +18320,7 @@
       <c r="A223" s="16" t="s">
         <v>409</v>
       </c>
-      <c r="B223" s="52">
+      <c r="B223" s="44">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Completed velocity and most of pressure equations.
</commit_message>
<xml_diff>
--- a/pipe/coefficients-20.xlsx
+++ b/pipe/coefficients-20.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15480" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="11440" yWindow="0" windowWidth="12840" windowHeight="15480" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3078,8 +3078,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:DR181"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H51" sqref="H51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3905,7 +3905,7 @@
       </c>
       <c r="I34">
         <f ca="1">1+RAND()*F16*IF(RAND()&gt;0.5,1,-1)</f>
-        <v>1.0428538990093279</v>
+        <v>0.95394349660496325</v>
       </c>
     </row>
     <row r="35" spans="1:10">
@@ -9295,8 +9295,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:HQ370"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CY1" workbookViewId="0">
-      <selection activeCell="CZ4" sqref="CZ4"/>
+    <sheetView topLeftCell="HK205" workbookViewId="0">
+      <selection activeCell="DE10" sqref="DE10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -14040,7 +14040,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:HO224"/>
   <sheetViews>
-    <sheetView topLeftCell="HA1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="HF1" workbookViewId="0">
       <selection activeCell="HN3" sqref="HN3"/>
     </sheetView>
   </sheetViews>

</xml_diff>